<commit_message>
Atualização da Documentação Mapeamento - LN
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Mapeamento Stage LN.xlsx
+++ b/Documentação/Planilhas/Mapeamento Stage LN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="17235" windowHeight="6210" tabRatio="539" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="17235" windowHeight="6210" tabRatio="539" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DE-PARA Tabelas" sheetId="1" state="hidden" r:id="rId1"/>
@@ -8348,9 +8348,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -8358,6 +8355,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -10022,7 +10022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:L156"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="D84" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -12899,7 +12899,7 @@
       <c r="A88" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B88" s="171" t="s">
+      <c r="B88" s="174" t="s">
         <v>914</v>
       </c>
       <c r="C88" s="36" t="s">
@@ -12935,7 +12935,7 @@
       <c r="A89" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B89" s="171"/>
+      <c r="B89" s="174"/>
       <c r="C89" s="36" t="s">
         <v>2011</v>
       </c>
@@ -12985,7 +12985,7 @@
       <c r="A91" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B91" s="171" t="s">
+      <c r="B91" s="174" t="s">
         <v>2014</v>
       </c>
       <c r="C91" s="36" t="s">
@@ -13021,7 +13021,7 @@
       <c r="A92" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B92" s="171"/>
+      <c r="B92" s="174"/>
       <c r="C92" s="36" t="s">
         <v>2018</v>
       </c>
@@ -13055,7 +13055,7 @@
       <c r="A93" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B93" s="171"/>
+      <c r="B93" s="174"/>
       <c r="C93" s="36"/>
       <c r="D93" s="37" t="s">
         <v>1783</v>
@@ -13089,7 +13089,7 @@
       <c r="A94" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B94" s="171"/>
+      <c r="B94" s="174"/>
       <c r="C94" s="36"/>
       <c r="D94" s="37" t="s">
         <v>1783</v>
@@ -13123,7 +13123,7 @@
       <c r="A95" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B95" s="171"/>
+      <c r="B95" s="174"/>
       <c r="C95" s="36"/>
       <c r="D95" s="37" t="s">
         <v>1783</v>
@@ -13157,7 +13157,7 @@
       <c r="A96" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B96" s="171"/>
+      <c r="B96" s="174"/>
       <c r="C96" s="36" t="s">
         <v>2020</v>
       </c>
@@ -13191,7 +13191,7 @@
       <c r="A97" s="34" t="s">
         <v>1652</v>
       </c>
-      <c r="B97" s="171"/>
+      <c r="B97" s="174"/>
       <c r="C97" s="64" t="s">
         <v>2022</v>
       </c>
@@ -13213,7 +13213,7 @@
       <c r="A98" s="34" t="s">
         <v>1652</v>
       </c>
-      <c r="B98" s="171"/>
+      <c r="B98" s="174"/>
       <c r="C98" s="64" t="s">
         <v>2023</v>
       </c>
@@ -13235,7 +13235,7 @@
       <c r="A99" s="34" t="s">
         <v>1652</v>
       </c>
-      <c r="B99" s="171"/>
+      <c r="B99" s="174"/>
       <c r="C99" s="64" t="s">
         <v>2024</v>
       </c>
@@ -13513,7 +13513,7 @@
       <c r="A109" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B109" s="171" t="s">
+      <c r="B109" s="174" t="s">
         <v>948</v>
       </c>
       <c r="C109" s="36" t="s">
@@ -13549,7 +13549,7 @@
       <c r="A110" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B110" s="171"/>
+      <c r="B110" s="174"/>
       <c r="C110" s="36" t="s">
         <v>2048</v>
       </c>
@@ -13583,7 +13583,7 @@
       <c r="A111" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B111" s="171"/>
+      <c r="B111" s="174"/>
       <c r="C111" s="36" t="s">
         <v>2050</v>
       </c>
@@ -13633,7 +13633,7 @@
       <c r="A113" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B113" s="171" t="s">
+      <c r="B113" s="174" t="s">
         <v>954</v>
       </c>
       <c r="C113" s="36" t="s">
@@ -13669,7 +13669,7 @@
       <c r="A114" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B114" s="171"/>
+      <c r="B114" s="174"/>
       <c r="C114" s="36" t="s">
         <v>2057</v>
       </c>
@@ -13771,7 +13771,7 @@
       <c r="A118" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B118" s="171" t="s">
+      <c r="B118" s="174" t="s">
         <v>2064</v>
       </c>
       <c r="C118" s="36" t="s">
@@ -13807,7 +13807,7 @@
       <c r="A119" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B119" s="171"/>
+      <c r="B119" s="174"/>
       <c r="C119" s="36" t="s">
         <v>2069</v>
       </c>
@@ -13841,7 +13841,7 @@
       <c r="A120" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B120" s="171"/>
+      <c r="B120" s="174"/>
       <c r="C120" s="36" t="s">
         <v>2072</v>
       </c>
@@ -13875,7 +13875,7 @@
       <c r="A121" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B121" s="171"/>
+      <c r="B121" s="174"/>
       <c r="C121" s="36" t="s">
         <v>2075</v>
       </c>
@@ -13925,7 +13925,7 @@
       <c r="A123" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B123" s="171" t="s">
+      <c r="B123" s="174" t="s">
         <v>2078</v>
       </c>
       <c r="C123" s="36" t="s">
@@ -13961,7 +13961,7 @@
       <c r="A124" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B124" s="171"/>
+      <c r="B124" s="174"/>
       <c r="C124" s="36" t="s">
         <v>2083</v>
       </c>
@@ -13995,7 +13995,7 @@
       <c r="A125" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B125" s="171"/>
+      <c r="B125" s="174"/>
       <c r="C125" s="36" t="s">
         <v>2086</v>
       </c>
@@ -14097,7 +14097,7 @@
       <c r="A129" s="34" t="s">
         <v>1652</v>
       </c>
-      <c r="B129" s="174" t="s">
+      <c r="B129" s="173" t="s">
         <v>2094</v>
       </c>
       <c r="C129" s="52" t="s">
@@ -14127,7 +14127,7 @@
       <c r="A130" s="34" t="s">
         <v>1652</v>
       </c>
-      <c r="B130" s="174"/>
+      <c r="B130" s="173"/>
       <c r="C130" s="52" t="s">
         <v>2097</v>
       </c>
@@ -14171,7 +14171,7 @@
       <c r="A132" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B132" s="171" t="s">
+      <c r="B132" s="174" t="s">
         <v>2098</v>
       </c>
       <c r="C132" s="36" t="s">
@@ -14207,7 +14207,7 @@
       <c r="A133" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B133" s="171"/>
+      <c r="B133" s="174"/>
       <c r="C133" s="36" t="s">
         <v>2103</v>
       </c>
@@ -14257,7 +14257,7 @@
       <c r="A135" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B135" s="171" t="s">
+      <c r="B135" s="174" t="s">
         <v>2106</v>
       </c>
       <c r="C135" s="36" t="s">
@@ -14293,7 +14293,7 @@
       <c r="A136" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B136" s="171"/>
+      <c r="B136" s="174"/>
       <c r="C136" s="36" t="s">
         <v>2111</v>
       </c>
@@ -14327,7 +14327,7 @@
       <c r="A137" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B137" s="171"/>
+      <c r="B137" s="174"/>
       <c r="C137" s="36" t="s">
         <v>2114</v>
       </c>
@@ -14361,7 +14361,7 @@
       <c r="A138" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B138" s="171"/>
+      <c r="B138" s="174"/>
       <c r="C138" s="36" t="s">
         <v>2117</v>
       </c>
@@ -14615,7 +14615,7 @@
       <c r="A147" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B147" s="171" t="s">
+      <c r="B147" s="174" t="s">
         <v>2137</v>
       </c>
       <c r="C147" s="36" t="s">
@@ -14651,7 +14651,7 @@
       <c r="A148" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B148" s="171"/>
+      <c r="B148" s="174"/>
       <c r="C148" s="36" t="s">
         <v>2142</v>
       </c>
@@ -14701,7 +14701,7 @@
       <c r="A150" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B150" s="172" t="s">
+      <c r="B150" s="171" t="s">
         <v>2342</v>
       </c>
       <c r="C150" s="132" t="s">
@@ -14737,7 +14737,7 @@
       <c r="A151" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B151" s="173"/>
+      <c r="B151" s="172"/>
       <c r="C151" s="132" t="s">
         <v>2145</v>
       </c>
@@ -14771,7 +14771,7 @@
       <c r="A152" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B152" s="173"/>
+      <c r="B152" s="172"/>
       <c r="C152" s="58" t="s">
         <v>2147</v>
       </c>
@@ -14805,7 +14805,7 @@
       <c r="A153" s="34" t="s">
         <v>1652</v>
       </c>
-      <c r="B153" s="173"/>
+      <c r="B153" s="172"/>
       <c r="C153" s="58"/>
       <c r="D153" s="45" t="s">
         <v>1783</v>
@@ -14837,7 +14837,7 @@
       <c r="A154" s="34" t="s">
         <v>1985</v>
       </c>
-      <c r="B154" s="173"/>
+      <c r="B154" s="172"/>
       <c r="C154" s="58" t="s">
         <v>2149</v>
       </c>
@@ -14869,7 +14869,7 @@
       <c r="A155" s="34" t="s">
         <v>1985</v>
       </c>
-      <c r="B155" s="173"/>
+      <c r="B155" s="172"/>
       <c r="C155" s="58" t="s">
         <v>2150</v>
       </c>
@@ -14912,17 +14912,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B150:B155"/>
-    <mergeCell ref="B129:B130"/>
-    <mergeCell ref="B132:B133"/>
-    <mergeCell ref="B135:B138"/>
-    <mergeCell ref="B147:B148"/>
     <mergeCell ref="B123:B125"/>
     <mergeCell ref="B88:B89"/>
     <mergeCell ref="B91:B99"/>
     <mergeCell ref="B109:B111"/>
     <mergeCell ref="B113:B114"/>
     <mergeCell ref="B118:B121"/>
+    <mergeCell ref="B150:B155"/>
+    <mergeCell ref="B129:B130"/>
+    <mergeCell ref="B132:B133"/>
+    <mergeCell ref="B135:B138"/>
+    <mergeCell ref="B147:B148"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -14933,9 +14933,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M1423"/>
   <sheetViews>
-    <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A340" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D348" sqref="D348:D359"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A547" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G561" sqref="G561"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -33981,7 +33981,7 @@
         <v>917</v>
       </c>
       <c r="G555" s="7">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="H555" s="7" t="s">
         <v>1533</v>
@@ -34014,7 +34014,7 @@
         <v>917</v>
       </c>
       <c r="G556" s="7">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="H556" s="7" t="s">
         <v>1534</v>
@@ -34047,7 +34047,7 @@
         <v>917</v>
       </c>
       <c r="G557" s="7">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="H557" s="7" t="s">
         <v>1535</v>
@@ -34080,7 +34080,7 @@
         <v>917</v>
       </c>
       <c r="G558" s="7">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="H558" s="7" t="s">
         <v>1536</v>
@@ -34113,7 +34113,7 @@
         <v>917</v>
       </c>
       <c r="G559" s="7">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="H559" s="7" t="s">
         <v>1541</v>
@@ -34146,7 +34146,7 @@
         <v>917</v>
       </c>
       <c r="G560" s="7">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="H560" s="7" t="s">
         <v>1542</v>

</xml_diff>

<commit_message>
Atualização Mapeamento Stage LN
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Mapeamento Stage LN.xlsx
+++ b/Documentação/Planilhas/Mapeamento Stage LN.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14662" uniqueCount="2410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14662" uniqueCount="2411">
   <si>
     <t>dbo.Balancete</t>
   </si>
@@ -7260,6 +7260,9 @@
   </si>
   <si>
     <t>DT_BAIXA</t>
+  </si>
+  <si>
+    <t>DT_CRIACAO</t>
   </si>
 </sst>
 </file>
@@ -14994,9 +14997,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M1440"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A248" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M268" sqref="M268:M275"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A854" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D798" sqref="D798:D861"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -44361,10 +44364,10 @@
         <v>822</v>
       </c>
       <c r="D855" s="7" t="s">
-        <v>729</v>
+        <v>787</v>
       </c>
       <c r="E855" s="7">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F855" s="7" t="s">
         <v>918</v>
@@ -44373,7 +44376,7 @@
         <v>916</v>
       </c>
       <c r="H855" s="7" t="s">
-        <v>1262</v>
+        <v>1215</v>
       </c>
       <c r="I855" s="7"/>
       <c r="J855" s="7"/>
@@ -44394,10 +44397,10 @@
         <v>822</v>
       </c>
       <c r="D856" s="7" t="s">
-        <v>787</v>
+        <v>753</v>
       </c>
       <c r="E856" s="7">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F856" s="7" t="s">
         <v>918</v>
@@ -44406,7 +44409,7 @@
         <v>916</v>
       </c>
       <c r="H856" s="7" t="s">
-        <v>1215</v>
+        <v>1242</v>
       </c>
       <c r="I856" s="7"/>
       <c r="J856" s="7"/>
@@ -44427,10 +44430,10 @@
         <v>822</v>
       </c>
       <c r="D857" s="7" t="s">
-        <v>753</v>
+        <v>734</v>
       </c>
       <c r="E857" s="7">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F857" s="7" t="s">
         <v>918</v>
@@ -44439,7 +44442,7 @@
         <v>916</v>
       </c>
       <c r="H857" s="7" t="s">
-        <v>1242</v>
+        <v>795</v>
       </c>
       <c r="I857" s="7"/>
       <c r="J857" s="7"/>
@@ -44460,10 +44463,10 @@
         <v>822</v>
       </c>
       <c r="D858" s="7" t="s">
-        <v>734</v>
+        <v>700</v>
       </c>
       <c r="E858" s="7">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F858" s="7" t="s">
         <v>918</v>
@@ -44472,7 +44475,7 @@
         <v>916</v>
       </c>
       <c r="H858" s="7" t="s">
-        <v>795</v>
+        <v>1283</v>
       </c>
       <c r="I858" s="7"/>
       <c r="J858" s="7"/>
@@ -44493,10 +44496,10 @@
         <v>822</v>
       </c>
       <c r="D859" s="7" t="s">
-        <v>700</v>
+        <v>773</v>
       </c>
       <c r="E859" s="7">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F859" s="7" t="s">
         <v>918</v>
@@ -44505,7 +44508,7 @@
         <v>916</v>
       </c>
       <c r="H859" s="7" t="s">
-        <v>1283</v>
+        <v>1225</v>
       </c>
       <c r="I859" s="7"/>
       <c r="J859" s="7"/>
@@ -44526,10 +44529,10 @@
         <v>822</v>
       </c>
       <c r="D860" s="7" t="s">
-        <v>773</v>
+        <v>710</v>
       </c>
       <c r="E860" s="7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F860" s="7" t="s">
         <v>918</v>
@@ -44538,7 +44541,7 @@
         <v>916</v>
       </c>
       <c r="H860" s="7" t="s">
-        <v>1225</v>
+        <v>1275</v>
       </c>
       <c r="I860" s="7"/>
       <c r="J860" s="7"/>
@@ -44559,10 +44562,10 @@
         <v>822</v>
       </c>
       <c r="D861" s="7" t="s">
-        <v>710</v>
+        <v>704</v>
       </c>
       <c r="E861" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F861" s="7" t="s">
         <v>918</v>
@@ -44571,7 +44574,7 @@
         <v>916</v>
       </c>
       <c r="H861" s="7" t="s">
-        <v>1275</v>
+        <v>1279</v>
       </c>
       <c r="I861" s="7"/>
       <c r="J861" s="7"/>
@@ -44586,30 +44589,38 @@
         <v>1105</v>
       </c>
       <c r="B862" s="7" t="s">
-        <v>996</v>
+        <v>988</v>
       </c>
       <c r="C862" s="7" t="s">
-        <v>822</v>
+        <v>814</v>
       </c>
       <c r="D862" s="7" t="s">
-        <v>704</v>
-      </c>
-      <c r="E862" s="7">
-        <v>23</v>
+        <v>292</v>
+      </c>
+      <c r="E862" s="22" t="s">
+        <v>1706</v>
       </c>
       <c r="F862" s="7" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
       <c r="G862" s="7" t="s">
         <v>916</v>
       </c>
       <c r="H862" s="7" t="s">
-        <v>1279</v>
-      </c>
-      <c r="I862" s="7"/>
-      <c r="J862" s="7"/>
-      <c r="K862" s="23"/>
-      <c r="L862" s="7"/>
+        <v>1175</v>
+      </c>
+      <c r="I862" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J862" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="K862" s="23" t="s">
+        <v>837</v>
+      </c>
+      <c r="L862" s="7" t="s">
+        <v>1175</v>
+      </c>
       <c r="M862" s="10" t="s">
         <v>1652</v>
       </c>
@@ -44625,31 +44636,31 @@
         <v>814</v>
       </c>
       <c r="D863" s="7" t="s">
-        <v>292</v>
+        <v>212</v>
       </c>
       <c r="E863" s="22" t="s">
-        <v>1706</v>
+        <v>1707</v>
       </c>
       <c r="F863" s="7" t="s">
-        <v>915</v>
-      </c>
-      <c r="G863" s="7" t="s">
-        <v>916</v>
+        <v>917</v>
+      </c>
+      <c r="G863" s="7">
+        <v>12</v>
       </c>
       <c r="H863" s="7" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="I863" s="7" t="s">
         <v>73</v>
       </c>
       <c r="J863" s="7" t="s">
-        <v>184</v>
+        <v>212</v>
       </c>
       <c r="K863" s="23" t="s">
         <v>837</v>
       </c>
       <c r="L863" s="7" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="M863" s="10" t="s">
         <v>1652</v>
@@ -44666,32 +44677,24 @@
         <v>814</v>
       </c>
       <c r="D864" s="7" t="s">
-        <v>212</v>
+        <v>502</v>
       </c>
       <c r="E864" s="22" t="s">
-        <v>1707</v>
+        <v>1708</v>
       </c>
       <c r="F864" s="7" t="s">
-        <v>917</v>
-      </c>
-      <c r="G864" s="7">
-        <v>12</v>
+        <v>915</v>
+      </c>
+      <c r="G864" s="7" t="s">
+        <v>916</v>
       </c>
       <c r="H864" s="7" t="s">
-        <v>1174</v>
-      </c>
-      <c r="I864" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="J864" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="K864" s="23" t="s">
-        <v>837</v>
-      </c>
-      <c r="L864" s="7" t="s">
-        <v>1174</v>
-      </c>
+        <v>1528</v>
+      </c>
+      <c r="I864" s="7"/>
+      <c r="J864" s="7"/>
+      <c r="K864" s="23"/>
+      <c r="L864" s="7"/>
       <c r="M864" s="10" t="s">
         <v>1652</v>
       </c>
@@ -44707,19 +44710,19 @@
         <v>814</v>
       </c>
       <c r="D865" s="7" t="s">
-        <v>502</v>
+        <v>627</v>
       </c>
       <c r="E865" s="22" t="s">
-        <v>1708</v>
+        <v>1709</v>
       </c>
       <c r="F865" s="7" t="s">
-        <v>915</v>
-      </c>
-      <c r="G865" s="7" t="s">
-        <v>916</v>
+        <v>917</v>
+      </c>
+      <c r="G865" s="7">
+        <v>16</v>
       </c>
       <c r="H865" s="7" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="I865" s="7"/>
       <c r="J865" s="7"/>
@@ -44740,24 +44743,32 @@
         <v>814</v>
       </c>
       <c r="D866" s="7" t="s">
-        <v>627</v>
+        <v>239</v>
       </c>
       <c r="E866" s="22" t="s">
-        <v>1709</v>
+        <v>1710</v>
       </c>
       <c r="F866" s="7" t="s">
         <v>917</v>
       </c>
       <c r="G866" s="7">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="H866" s="7" t="s">
-        <v>1529</v>
-      </c>
-      <c r="I866" s="7"/>
-      <c r="J866" s="7"/>
-      <c r="K866" s="23"/>
-      <c r="L866" s="7"/>
+        <v>1369</v>
+      </c>
+      <c r="I866" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="J866" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="K866" s="23" t="s">
+        <v>875</v>
+      </c>
+      <c r="L866" s="7" t="s">
+        <v>1369</v>
+      </c>
       <c r="M866" s="10" t="s">
         <v>1652</v>
       </c>
@@ -44773,31 +44784,31 @@
         <v>814</v>
       </c>
       <c r="D867" s="7" t="s">
-        <v>239</v>
+        <v>623</v>
       </c>
       <c r="E867" s="22" t="s">
-        <v>1710</v>
+        <v>1711</v>
       </c>
       <c r="F867" s="7" t="s">
         <v>917</v>
       </c>
       <c r="G867" s="7">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H867" s="7" t="s">
-        <v>1369</v>
+        <v>1315</v>
       </c>
       <c r="I867" s="7" t="s">
         <v>93</v>
       </c>
       <c r="J867" s="7" t="s">
-        <v>237</v>
+        <v>616</v>
       </c>
       <c r="K867" s="23" t="s">
         <v>875</v>
       </c>
       <c r="L867" s="7" t="s">
-        <v>1369</v>
+        <v>1315</v>
       </c>
       <c r="M867" s="10" t="s">
         <v>1652</v>
@@ -44814,31 +44825,31 @@
         <v>814</v>
       </c>
       <c r="D868" s="7" t="s">
-        <v>623</v>
+        <v>268</v>
       </c>
       <c r="E868" s="22" t="s">
-        <v>1711</v>
+        <v>1712</v>
       </c>
       <c r="F868" s="7" t="s">
-        <v>917</v>
-      </c>
-      <c r="G868" s="7">
-        <v>12</v>
+        <v>915</v>
+      </c>
+      <c r="G868" s="7" t="s">
+        <v>916</v>
       </c>
       <c r="H868" s="7" t="s">
-        <v>1315</v>
+        <v>1298</v>
       </c>
       <c r="I868" s="7" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="J868" s="7" t="s">
-        <v>616</v>
+        <v>268</v>
       </c>
       <c r="K868" s="23" t="s">
-        <v>875</v>
+        <v>1146</v>
       </c>
       <c r="L868" s="7" t="s">
-        <v>1315</v>
+        <v>1298</v>
       </c>
       <c r="M868" s="10" t="s">
         <v>1652</v>
@@ -44855,32 +44866,24 @@
         <v>814</v>
       </c>
       <c r="D869" s="7" t="s">
-        <v>268</v>
+        <v>391</v>
       </c>
       <c r="E869" s="22" t="s">
-        <v>1712</v>
+        <v>1713</v>
       </c>
       <c r="F869" s="7" t="s">
-        <v>915</v>
+        <v>919</v>
       </c>
       <c r="G869" s="7" t="s">
         <v>916</v>
       </c>
       <c r="H869" s="7" t="s">
-        <v>1298</v>
-      </c>
-      <c r="I869" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="J869" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="K869" s="23" t="s">
-        <v>1146</v>
-      </c>
-      <c r="L869" s="7" t="s">
-        <v>1298</v>
-      </c>
+        <v>1404</v>
+      </c>
+      <c r="I869" s="7"/>
+      <c r="J869" s="7"/>
+      <c r="K869" s="23"/>
+      <c r="L869" s="7"/>
       <c r="M869" s="10" t="s">
         <v>1652</v>
       </c>
@@ -44896,10 +44899,10 @@
         <v>814</v>
       </c>
       <c r="D870" s="7" t="s">
-        <v>391</v>
+        <v>440</v>
       </c>
       <c r="E870" s="22" t="s">
-        <v>1713</v>
+        <v>1714</v>
       </c>
       <c r="F870" s="7" t="s">
         <v>919</v>
@@ -44908,7 +44911,7 @@
         <v>916</v>
       </c>
       <c r="H870" s="7" t="s">
-        <v>1404</v>
+        <v>1378</v>
       </c>
       <c r="I870" s="7"/>
       <c r="J870" s="7"/>
@@ -44929,24 +44932,32 @@
         <v>814</v>
       </c>
       <c r="D871" s="7" t="s">
-        <v>440</v>
+        <v>191</v>
       </c>
       <c r="E871" s="22" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
       <c r="F871" s="7" t="s">
-        <v>919</v>
-      </c>
-      <c r="G871" s="7" t="s">
-        <v>916</v>
+        <v>917</v>
+      </c>
+      <c r="G871" s="7">
+        <v>18</v>
       </c>
       <c r="H871" s="7" t="s">
-        <v>1378</v>
-      </c>
-      <c r="I871" s="7"/>
-      <c r="J871" s="7"/>
-      <c r="K871" s="23"/>
-      <c r="L871" s="7"/>
+        <v>1478</v>
+      </c>
+      <c r="I871" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="J871" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="K871" s="23" t="s">
+        <v>882</v>
+      </c>
+      <c r="L871" s="7" t="s">
+        <v>1205</v>
+      </c>
       <c r="M871" s="10" t="s">
         <v>1652</v>
       </c>
@@ -44962,10 +44973,10 @@
         <v>814</v>
       </c>
       <c r="D872" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E872" s="22" t="s">
-        <v>1715</v>
+        <v>1716</v>
       </c>
       <c r="F872" s="7" t="s">
         <v>917</v>
@@ -44974,7 +44985,7 @@
         <v>18</v>
       </c>
       <c r="H872" s="7" t="s">
-        <v>1478</v>
+        <v>1480</v>
       </c>
       <c r="I872" s="7" t="s">
         <v>100</v>
@@ -45003,31 +45014,31 @@
         <v>814</v>
       </c>
       <c r="D873" s="7" t="s">
-        <v>190</v>
+        <v>514</v>
       </c>
       <c r="E873" s="22" t="s">
-        <v>1716</v>
+        <v>1717</v>
       </c>
       <c r="F873" s="7" t="s">
         <v>917</v>
       </c>
       <c r="G873" s="7">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="H873" s="7" t="s">
-        <v>1480</v>
+        <v>1530</v>
       </c>
       <c r="I873" s="7" t="s">
-        <v>100</v>
+        <v>1004</v>
       </c>
       <c r="J873" s="7" t="s">
-        <v>285</v>
+        <v>518</v>
       </c>
       <c r="K873" s="23" t="s">
-        <v>882</v>
+        <v>824</v>
       </c>
       <c r="L873" s="7" t="s">
-        <v>1205</v>
+        <v>1530</v>
       </c>
       <c r="M873" s="10" t="s">
         <v>1652</v>
@@ -45044,32 +45055,28 @@
         <v>814</v>
       </c>
       <c r="D874" s="7" t="s">
-        <v>514</v>
+        <v>489</v>
       </c>
       <c r="E874" s="22" t="s">
-        <v>1717</v>
+        <v>1718</v>
       </c>
       <c r="F874" s="7" t="s">
         <v>917</v>
       </c>
       <c r="G874" s="7">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="H874" s="7" t="s">
-        <v>1530</v>
+        <v>1539</v>
       </c>
       <c r="I874" s="7" t="s">
-        <v>1004</v>
+        <v>1077</v>
       </c>
       <c r="J874" s="7" t="s">
-        <v>518</v>
-      </c>
-      <c r="K874" s="23" t="s">
-        <v>824</v>
-      </c>
-      <c r="L874" s="7" t="s">
-        <v>1530</v>
-      </c>
+        <v>1077</v>
+      </c>
+      <c r="K874" s="23"/>
+      <c r="L874" s="7"/>
       <c r="M874" s="10" t="s">
         <v>1652</v>
       </c>
@@ -45085,28 +45092,32 @@
         <v>814</v>
       </c>
       <c r="D875" s="7" t="s">
-        <v>489</v>
+        <v>549</v>
       </c>
       <c r="E875" s="22" t="s">
-        <v>1718</v>
+        <v>1719</v>
       </c>
       <c r="F875" s="7" t="s">
         <v>917</v>
       </c>
       <c r="G875" s="7">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="H875" s="7" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="I875" s="7" t="s">
-        <v>1077</v>
+        <v>1004</v>
       </c>
       <c r="J875" s="7" t="s">
-        <v>1077</v>
-      </c>
-      <c r="K875" s="23"/>
-      <c r="L875" s="7"/>
+        <v>549</v>
+      </c>
+      <c r="K875" s="23" t="s">
+        <v>824</v>
+      </c>
+      <c r="L875" s="7" t="s">
+        <v>1540</v>
+      </c>
       <c r="M875" s="10" t="s">
         <v>1652</v>
       </c>
@@ -45122,32 +45133,24 @@
         <v>814</v>
       </c>
       <c r="D876" s="7" t="s">
-        <v>549</v>
+        <v>744</v>
       </c>
       <c r="E876" s="22" t="s">
-        <v>1719</v>
+        <v>1720</v>
       </c>
       <c r="F876" s="7" t="s">
-        <v>917</v>
-      </c>
-      <c r="G876" s="7">
-        <v>18</v>
+        <v>918</v>
+      </c>
+      <c r="G876" s="7" t="s">
+        <v>916</v>
       </c>
       <c r="H876" s="7" t="s">
-        <v>1540</v>
-      </c>
-      <c r="I876" s="7" t="s">
-        <v>1004</v>
-      </c>
-      <c r="J876" s="7" t="s">
-        <v>549</v>
-      </c>
-      <c r="K876" s="23" t="s">
-        <v>824</v>
-      </c>
-      <c r="L876" s="7" t="s">
-        <v>1540</v>
-      </c>
+        <v>1245</v>
+      </c>
+      <c r="I876" s="7"/>
+      <c r="J876" s="7"/>
+      <c r="K876" s="23"/>
+      <c r="L876" s="7"/>
       <c r="M876" s="10" t="s">
         <v>1652</v>
       </c>
@@ -45163,10 +45166,10 @@
         <v>814</v>
       </c>
       <c r="D877" s="7" t="s">
-        <v>744</v>
+        <v>750</v>
       </c>
       <c r="E877" s="22" t="s">
-        <v>1720</v>
+        <v>1721</v>
       </c>
       <c r="F877" s="7" t="s">
         <v>918</v>
@@ -45175,7 +45178,7 @@
         <v>916</v>
       </c>
       <c r="H877" s="7" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="I877" s="7"/>
       <c r="J877" s="7"/>
@@ -45196,10 +45199,10 @@
         <v>814</v>
       </c>
       <c r="D878" s="7" t="s">
-        <v>750</v>
+        <v>755</v>
       </c>
       <c r="E878" s="22" t="s">
-        <v>1721</v>
+        <v>1722</v>
       </c>
       <c r="F878" s="7" t="s">
         <v>918</v>
@@ -45208,7 +45211,7 @@
         <v>916</v>
       </c>
       <c r="H878" s="7" t="s">
-        <v>1244</v>
+        <v>1240</v>
       </c>
       <c r="I878" s="7"/>
       <c r="J878" s="7"/>
@@ -45229,10 +45232,10 @@
         <v>814</v>
       </c>
       <c r="D879" s="7" t="s">
-        <v>755</v>
+        <v>777</v>
       </c>
       <c r="E879" s="22" t="s">
-        <v>1722</v>
+        <v>1723</v>
       </c>
       <c r="F879" s="7" t="s">
         <v>918</v>
@@ -45241,7 +45244,7 @@
         <v>916</v>
       </c>
       <c r="H879" s="7" t="s">
-        <v>1240</v>
+        <v>1221</v>
       </c>
       <c r="I879" s="7"/>
       <c r="J879" s="7"/>
@@ -45262,10 +45265,10 @@
         <v>814</v>
       </c>
       <c r="D880" s="7" t="s">
-        <v>777</v>
+        <v>738</v>
       </c>
       <c r="E880" s="22" t="s">
-        <v>1723</v>
+        <v>1724</v>
       </c>
       <c r="F880" s="7" t="s">
         <v>918</v>
@@ -45274,7 +45277,7 @@
         <v>916</v>
       </c>
       <c r="H880" s="7" t="s">
-        <v>1221</v>
+        <v>1256</v>
       </c>
       <c r="I880" s="7"/>
       <c r="J880" s="7"/>
@@ -45295,10 +45298,10 @@
         <v>814</v>
       </c>
       <c r="D881" s="7" t="s">
-        <v>738</v>
+        <v>781</v>
       </c>
       <c r="E881" s="22" t="s">
-        <v>1724</v>
+        <v>1725</v>
       </c>
       <c r="F881" s="7" t="s">
         <v>918</v>
@@ -45307,7 +45310,7 @@
         <v>916</v>
       </c>
       <c r="H881" s="7" t="s">
-        <v>1256</v>
+        <v>1219</v>
       </c>
       <c r="I881" s="7"/>
       <c r="J881" s="7"/>
@@ -45328,10 +45331,10 @@
         <v>814</v>
       </c>
       <c r="D882" s="7" t="s">
-        <v>781</v>
+        <v>730</v>
       </c>
       <c r="E882" s="22" t="s">
-        <v>1725</v>
+        <v>1726</v>
       </c>
       <c r="F882" s="7" t="s">
         <v>918</v>
@@ -45340,7 +45343,7 @@
         <v>916</v>
       </c>
       <c r="H882" s="7" t="s">
-        <v>1219</v>
+        <v>1258</v>
       </c>
       <c r="I882" s="7"/>
       <c r="J882" s="7"/>
@@ -45361,10 +45364,10 @@
         <v>814</v>
       </c>
       <c r="D883" s="7" t="s">
-        <v>730</v>
+        <v>753</v>
       </c>
       <c r="E883" s="22" t="s">
-        <v>1726</v>
+        <v>1727</v>
       </c>
       <c r="F883" s="7" t="s">
         <v>918</v>
@@ -45373,7 +45376,7 @@
         <v>916</v>
       </c>
       <c r="H883" s="7" t="s">
-        <v>1258</v>
+        <v>1242</v>
       </c>
       <c r="I883" s="7"/>
       <c r="J883" s="7"/>
@@ -45394,10 +45397,10 @@
         <v>814</v>
       </c>
       <c r="D884" s="7" t="s">
-        <v>753</v>
+        <v>727</v>
       </c>
       <c r="E884" s="22" t="s">
-        <v>1727</v>
+        <v>1728</v>
       </c>
       <c r="F884" s="7" t="s">
         <v>918</v>
@@ -45406,7 +45409,7 @@
         <v>916</v>
       </c>
       <c r="H884" s="7" t="s">
-        <v>1242</v>
+        <v>1216</v>
       </c>
       <c r="I884" s="7"/>
       <c r="J884" s="7"/>
@@ -45427,10 +45430,10 @@
         <v>814</v>
       </c>
       <c r="D885" s="7" t="s">
-        <v>727</v>
+        <v>791</v>
       </c>
       <c r="E885" s="22" t="s">
-        <v>1728</v>
+        <v>1729</v>
       </c>
       <c r="F885" s="7" t="s">
         <v>918</v>
@@ -45439,7 +45442,7 @@
         <v>916</v>
       </c>
       <c r="H885" s="7" t="s">
-        <v>1216</v>
+        <v>1212</v>
       </c>
       <c r="I885" s="7"/>
       <c r="J885" s="7"/>
@@ -45460,19 +45463,19 @@
         <v>814</v>
       </c>
       <c r="D886" s="7" t="s">
-        <v>791</v>
+        <v>503</v>
       </c>
       <c r="E886" s="22" t="s">
-        <v>1729</v>
+        <v>1730</v>
       </c>
       <c r="F886" s="7" t="s">
-        <v>918</v>
-      </c>
-      <c r="G886" s="7" t="s">
-        <v>916</v>
+        <v>917</v>
+      </c>
+      <c r="G886" s="7">
+        <v>20</v>
       </c>
       <c r="H886" s="7" t="s">
-        <v>1212</v>
+        <v>1533</v>
       </c>
       <c r="I886" s="7"/>
       <c r="J886" s="7"/>
@@ -45493,10 +45496,10 @@
         <v>814</v>
       </c>
       <c r="D887" s="7" t="s">
-        <v>503</v>
+        <v>628</v>
       </c>
       <c r="E887" s="22" t="s">
-        <v>1730</v>
+        <v>1731</v>
       </c>
       <c r="F887" s="7" t="s">
         <v>917</v>
@@ -45505,7 +45508,7 @@
         <v>20</v>
       </c>
       <c r="H887" s="7" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="I887" s="7"/>
       <c r="J887" s="7"/>
@@ -45526,10 +45529,10 @@
         <v>814</v>
       </c>
       <c r="D888" s="7" t="s">
-        <v>628</v>
+        <v>506</v>
       </c>
       <c r="E888" s="22" t="s">
-        <v>1731</v>
+        <v>1732</v>
       </c>
       <c r="F888" s="7" t="s">
         <v>917</v>
@@ -45538,7 +45541,7 @@
         <v>20</v>
       </c>
       <c r="H888" s="7" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="I888" s="7"/>
       <c r="J888" s="7"/>
@@ -45559,10 +45562,10 @@
         <v>814</v>
       </c>
       <c r="D889" s="7" t="s">
-        <v>506</v>
+        <v>630</v>
       </c>
       <c r="E889" s="22" t="s">
-        <v>1732</v>
+        <v>1733</v>
       </c>
       <c r="F889" s="7" t="s">
         <v>917</v>
@@ -45571,7 +45574,7 @@
         <v>20</v>
       </c>
       <c r="H889" s="7" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="I889" s="7"/>
       <c r="J889" s="7"/>
@@ -45592,19 +45595,19 @@
         <v>814</v>
       </c>
       <c r="D890" s="7" t="s">
-        <v>630</v>
+        <v>408</v>
       </c>
       <c r="E890" s="22" t="s">
-        <v>1733</v>
+        <v>1734</v>
       </c>
       <c r="F890" s="7" t="s">
-        <v>917</v>
-      </c>
-      <c r="G890" s="7">
-        <v>20</v>
+        <v>919</v>
+      </c>
+      <c r="G890" s="7" t="s">
+        <v>916</v>
       </c>
       <c r="H890" s="7" t="s">
-        <v>1536</v>
+        <v>1401</v>
       </c>
       <c r="I890" s="7"/>
       <c r="J890" s="7"/>
@@ -45625,24 +45628,32 @@
         <v>814</v>
       </c>
       <c r="D891" s="7" t="s">
-        <v>408</v>
+        <v>645</v>
       </c>
       <c r="E891" s="22" t="s">
-        <v>1734</v>
+        <v>1735</v>
       </c>
       <c r="F891" s="7" t="s">
-        <v>919</v>
+        <v>915</v>
       </c>
       <c r="G891" s="7" t="s">
         <v>916</v>
       </c>
       <c r="H891" s="7" t="s">
-        <v>1401</v>
-      </c>
-      <c r="I891" s="7"/>
-      <c r="J891" s="7"/>
-      <c r="K891" s="23"/>
-      <c r="L891" s="7"/>
+        <v>1311</v>
+      </c>
+      <c r="I891" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="J891" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="K891" s="23" t="s">
+        <v>896</v>
+      </c>
+      <c r="L891" s="7" t="s">
+        <v>1311</v>
+      </c>
       <c r="M891" s="10" t="s">
         <v>1652</v>
       </c>
@@ -45658,32 +45669,24 @@
         <v>814</v>
       </c>
       <c r="D892" s="7" t="s">
-        <v>645</v>
+        <v>735</v>
       </c>
       <c r="E892" s="22" t="s">
-        <v>1735</v>
+        <v>1736</v>
       </c>
       <c r="F892" s="7" t="s">
-        <v>915</v>
+        <v>918</v>
       </c>
       <c r="G892" s="7" t="s">
         <v>916</v>
       </c>
       <c r="H892" s="7" t="s">
-        <v>1311</v>
-      </c>
-      <c r="I892" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="J892" s="7" t="s">
-        <v>254</v>
-      </c>
-      <c r="K892" s="23" t="s">
-        <v>896</v>
-      </c>
-      <c r="L892" s="7" t="s">
-        <v>1311</v>
-      </c>
+        <v>1259</v>
+      </c>
+      <c r="I892" s="7"/>
+      <c r="J892" s="7"/>
+      <c r="K892" s="23"/>
+      <c r="L892" s="7"/>
       <c r="M892" s="10" t="s">
         <v>1652</v>
       </c>
@@ -45699,10 +45702,10 @@
         <v>814</v>
       </c>
       <c r="D893" s="7" t="s">
-        <v>735</v>
+        <v>771</v>
       </c>
       <c r="E893" s="22" t="s">
-        <v>1736</v>
+        <v>1737</v>
       </c>
       <c r="F893" s="7" t="s">
         <v>918</v>
@@ -45711,7 +45714,7 @@
         <v>916</v>
       </c>
       <c r="H893" s="7" t="s">
-        <v>1259</v>
+        <v>1227</v>
       </c>
       <c r="I893" s="7"/>
       <c r="J893" s="7"/>
@@ -45732,10 +45735,10 @@
         <v>814</v>
       </c>
       <c r="D894" s="7" t="s">
-        <v>771</v>
+        <v>707</v>
       </c>
       <c r="E894" s="22" t="s">
-        <v>1737</v>
+        <v>1738</v>
       </c>
       <c r="F894" s="7" t="s">
         <v>918</v>
@@ -45744,7 +45747,7 @@
         <v>916</v>
       </c>
       <c r="H894" s="7" t="s">
-        <v>1227</v>
+        <v>1277</v>
       </c>
       <c r="I894" s="7"/>
       <c r="J894" s="7"/>
@@ -45765,10 +45768,10 @@
         <v>814</v>
       </c>
       <c r="D895" s="7" t="s">
-        <v>707</v>
+        <v>717</v>
       </c>
       <c r="E895" s="22" t="s">
-        <v>1738</v>
+        <v>1739</v>
       </c>
       <c r="F895" s="7" t="s">
         <v>918</v>
@@ -45777,7 +45780,7 @@
         <v>916</v>
       </c>
       <c r="H895" s="7" t="s">
-        <v>1277</v>
+        <v>1270</v>
       </c>
       <c r="I895" s="7"/>
       <c r="J895" s="7"/>
@@ -45798,10 +45801,10 @@
         <v>814</v>
       </c>
       <c r="D896" s="7" t="s">
-        <v>717</v>
+        <v>729</v>
       </c>
       <c r="E896" s="22" t="s">
-        <v>1739</v>
+        <v>1740</v>
       </c>
       <c r="F896" s="7" t="s">
         <v>918</v>
@@ -45810,7 +45813,7 @@
         <v>916</v>
       </c>
       <c r="H896" s="7" t="s">
-        <v>1270</v>
+        <v>1262</v>
       </c>
       <c r="I896" s="7"/>
       <c r="J896" s="7"/>
@@ -45831,10 +45834,10 @@
         <v>814</v>
       </c>
       <c r="D897" s="7" t="s">
-        <v>729</v>
+        <v>734</v>
       </c>
       <c r="E897" s="22" t="s">
-        <v>1740</v>
+        <v>1741</v>
       </c>
       <c r="F897" s="7" t="s">
         <v>918</v>
@@ -45843,7 +45846,7 @@
         <v>916</v>
       </c>
       <c r="H897" s="7" t="s">
-        <v>1262</v>
+        <v>795</v>
       </c>
       <c r="I897" s="7"/>
       <c r="J897" s="7"/>
@@ -45864,10 +45867,10 @@
         <v>814</v>
       </c>
       <c r="D898" s="7" t="s">
-        <v>734</v>
+        <v>700</v>
       </c>
       <c r="E898" s="22" t="s">
-        <v>1741</v>
+        <v>1742</v>
       </c>
       <c r="F898" s="7" t="s">
         <v>918</v>
@@ -45876,7 +45879,7 @@
         <v>916</v>
       </c>
       <c r="H898" s="7" t="s">
-        <v>795</v>
+        <v>1283</v>
       </c>
       <c r="I898" s="7"/>
       <c r="J898" s="7"/>
@@ -45897,10 +45900,10 @@
         <v>814</v>
       </c>
       <c r="D899" s="7" t="s">
-        <v>700</v>
+        <v>773</v>
       </c>
       <c r="E899" s="22" t="s">
-        <v>1742</v>
+        <v>1743</v>
       </c>
       <c r="F899" s="7" t="s">
         <v>918</v>
@@ -45909,7 +45912,7 @@
         <v>916</v>
       </c>
       <c r="H899" s="7" t="s">
-        <v>1283</v>
+        <v>1225</v>
       </c>
       <c r="I899" s="7"/>
       <c r="J899" s="7"/>
@@ -45930,10 +45933,10 @@
         <v>814</v>
       </c>
       <c r="D900" s="7" t="s">
-        <v>773</v>
+        <v>710</v>
       </c>
       <c r="E900" s="22" t="s">
-        <v>1743</v>
+        <v>1744</v>
       </c>
       <c r="F900" s="7" t="s">
         <v>918</v>
@@ -45942,7 +45945,7 @@
         <v>916</v>
       </c>
       <c r="H900" s="7" t="s">
-        <v>1225</v>
+        <v>1275</v>
       </c>
       <c r="I900" s="7"/>
       <c r="J900" s="7"/>
@@ -45963,10 +45966,10 @@
         <v>814</v>
       </c>
       <c r="D901" s="7" t="s">
-        <v>710</v>
+        <v>704</v>
       </c>
       <c r="E901" s="22" t="s">
-        <v>1744</v>
+        <v>1745</v>
       </c>
       <c r="F901" s="7" t="s">
         <v>918</v>
@@ -45975,7 +45978,7 @@
         <v>916</v>
       </c>
       <c r="H901" s="7" t="s">
-        <v>1275</v>
+        <v>1279</v>
       </c>
       <c r="I901" s="7"/>
       <c r="J901" s="7"/>
@@ -45996,19 +45999,19 @@
         <v>814</v>
       </c>
       <c r="D902" s="7" t="s">
-        <v>704</v>
+        <v>384</v>
       </c>
       <c r="E902" s="22" t="s">
-        <v>1745</v>
+        <v>1746</v>
       </c>
       <c r="F902" s="7" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="G902" s="7" t="s">
         <v>916</v>
       </c>
       <c r="H902" s="7" t="s">
-        <v>1279</v>
+        <v>1406</v>
       </c>
       <c r="I902" s="7"/>
       <c r="J902" s="7"/>
@@ -46029,24 +46032,32 @@
         <v>814</v>
       </c>
       <c r="D903" s="7" t="s">
-        <v>384</v>
+        <v>686</v>
       </c>
       <c r="E903" s="22" t="s">
-        <v>1746</v>
+        <v>1747</v>
       </c>
       <c r="F903" s="7" t="s">
-        <v>919</v>
-      </c>
-      <c r="G903" s="7" t="s">
-        <v>916</v>
+        <v>917</v>
+      </c>
+      <c r="G903" s="7">
+        <v>20</v>
       </c>
       <c r="H903" s="7" t="s">
-        <v>1406</v>
-      </c>
-      <c r="I903" s="7"/>
-      <c r="J903" s="7"/>
-      <c r="K903" s="23"/>
-      <c r="L903" s="7"/>
+        <v>1586</v>
+      </c>
+      <c r="I903" s="7" t="s">
+        <v>1098</v>
+      </c>
+      <c r="J903" s="7" t="s">
+        <v>686</v>
+      </c>
+      <c r="K903" s="23" t="s">
+        <v>837</v>
+      </c>
+      <c r="L903" s="7" t="s">
+        <v>1586</v>
+      </c>
       <c r="M903" s="10" t="s">
         <v>1652</v>
       </c>
@@ -46062,31 +46073,31 @@
         <v>814</v>
       </c>
       <c r="D904" s="7" t="s">
-        <v>686</v>
+        <v>1293</v>
       </c>
       <c r="E904" s="22" t="s">
-        <v>1747</v>
+        <v>1748</v>
       </c>
       <c r="F904" s="7" t="s">
-        <v>917</v>
-      </c>
-      <c r="G904" s="7">
-        <v>20</v>
+        <v>915</v>
+      </c>
+      <c r="G904" s="7" t="s">
+        <v>916</v>
       </c>
       <c r="H904" s="7" t="s">
-        <v>1586</v>
+        <v>1293</v>
       </c>
       <c r="I904" s="7" t="s">
-        <v>1098</v>
+        <v>125</v>
       </c>
       <c r="J904" s="7" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="K904" s="23" t="s">
-        <v>837</v>
+        <v>910</v>
       </c>
       <c r="L904" s="7" t="s">
-        <v>1586</v>
+        <v>1293</v>
       </c>
       <c r="M904" s="10" t="s">
         <v>1652</v>
@@ -46103,32 +46114,24 @@
         <v>814</v>
       </c>
       <c r="D905" s="7" t="s">
-        <v>1293</v>
-      </c>
-      <c r="E905" s="22" t="s">
-        <v>1748</v>
+        <v>1524</v>
+      </c>
+      <c r="E905" s="22">
+        <v>44</v>
       </c>
       <c r="F905" s="7" t="s">
-        <v>915</v>
-      </c>
-      <c r="G905" s="7" t="s">
-        <v>916</v>
+        <v>917</v>
+      </c>
+      <c r="G905" s="7">
+        <v>30</v>
       </c>
       <c r="H905" s="7" t="s">
-        <v>1293</v>
-      </c>
-      <c r="I905" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="J905" s="7" t="s">
-        <v>689</v>
-      </c>
-      <c r="K905" s="23" t="s">
-        <v>910</v>
-      </c>
-      <c r="L905" s="7" t="s">
-        <v>1293</v>
-      </c>
+        <v>1524</v>
+      </c>
+      <c r="I905" s="7"/>
+      <c r="J905" s="7"/>
+      <c r="K905" s="23"/>
+      <c r="L905" s="7"/>
       <c r="M905" s="10" t="s">
         <v>1652</v>
       </c>
@@ -46138,30 +46141,38 @@
         <v>1105</v>
       </c>
       <c r="B906" s="7" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="C906" s="7" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="D906" s="7" t="s">
-        <v>1524</v>
-      </c>
-      <c r="E906" s="22">
-        <v>44</v>
+        <v>292</v>
+      </c>
+      <c r="E906" s="7">
+        <v>1</v>
       </c>
       <c r="F906" s="7" t="s">
-        <v>917</v>
-      </c>
-      <c r="G906" s="7">
-        <v>30</v>
+        <v>915</v>
+      </c>
+      <c r="G906" s="7" t="s">
+        <v>916</v>
       </c>
       <c r="H906" s="7" t="s">
-        <v>1524</v>
-      </c>
-      <c r="I906" s="7"/>
-      <c r="J906" s="7"/>
-      <c r="K906" s="23"/>
-      <c r="L906" s="7"/>
+        <v>1175</v>
+      </c>
+      <c r="I906" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J906" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="K906" s="23" t="s">
+        <v>837</v>
+      </c>
+      <c r="L906" s="7" t="s">
+        <v>1175</v>
+      </c>
       <c r="M906" s="10" t="s">
         <v>1652</v>
       </c>
@@ -46177,31 +46188,31 @@
         <v>815</v>
       </c>
       <c r="D907" s="7" t="s">
-        <v>292</v>
+        <v>212</v>
       </c>
       <c r="E907" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F907" s="7" t="s">
-        <v>915</v>
-      </c>
-      <c r="G907" s="7" t="s">
-        <v>916</v>
+        <v>917</v>
+      </c>
+      <c r="G907" s="7">
+        <v>12</v>
       </c>
       <c r="H907" s="7" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="I907" s="7" t="s">
         <v>73</v>
       </c>
       <c r="J907" s="7" t="s">
-        <v>184</v>
+        <v>212</v>
       </c>
       <c r="K907" s="23" t="s">
         <v>837</v>
       </c>
       <c r="L907" s="7" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="M907" s="10" t="s">
         <v>1652</v>
@@ -46218,31 +46229,31 @@
         <v>815</v>
       </c>
       <c r="D908" s="7" t="s">
-        <v>212</v>
+        <v>502</v>
       </c>
       <c r="E908" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F908" s="7" t="s">
-        <v>917</v>
-      </c>
-      <c r="G908" s="7">
-        <v>12</v>
+        <v>915</v>
+      </c>
+      <c r="G908" s="7" t="s">
+        <v>916</v>
       </c>
       <c r="H908" s="7" t="s">
-        <v>1174</v>
+        <v>1528</v>
       </c>
       <c r="I908" s="7" t="s">
-        <v>73</v>
+        <v>1099</v>
       </c>
       <c r="J908" s="7" t="s">
-        <v>212</v>
+        <v>502</v>
       </c>
       <c r="K908" s="23" t="s">
-        <v>837</v>
+        <v>814</v>
       </c>
       <c r="L908" s="7" t="s">
-        <v>1174</v>
+        <v>1528</v>
       </c>
       <c r="M908" s="10" t="s">
         <v>1652</v>
@@ -46259,31 +46270,31 @@
         <v>815</v>
       </c>
       <c r="D909" s="7" t="s">
-        <v>502</v>
+        <v>627</v>
       </c>
       <c r="E909" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F909" s="7" t="s">
-        <v>915</v>
-      </c>
-      <c r="G909" s="7" t="s">
-        <v>916</v>
+        <v>917</v>
+      </c>
+      <c r="G909" s="7">
+        <v>16</v>
       </c>
       <c r="H909" s="7" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="I909" s="7" t="s">
         <v>1099</v>
       </c>
       <c r="J909" s="7" t="s">
-        <v>502</v>
+        <v>627</v>
       </c>
       <c r="K909" s="23" t="s">
         <v>814</v>
       </c>
       <c r="L909" s="7" t="s">
-        <v>1528</v>
+        <v>1529</v>
       </c>
       <c r="M909" s="10" t="s">
         <v>1652</v>
@@ -46300,32 +46311,28 @@
         <v>815</v>
       </c>
       <c r="D910" s="7" t="s">
-        <v>627</v>
+        <v>217</v>
       </c>
       <c r="E910" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F910" s="7" t="s">
         <v>917</v>
       </c>
       <c r="G910" s="7">
-        <v>16</v>
+        <v>94</v>
       </c>
       <c r="H910" s="7" t="s">
-        <v>1529</v>
+        <v>1376</v>
       </c>
       <c r="I910" s="7" t="s">
-        <v>1099</v>
+        <v>961</v>
       </c>
       <c r="J910" s="7" t="s">
-        <v>627</v>
-      </c>
-      <c r="K910" s="23" t="s">
-        <v>814</v>
-      </c>
-      <c r="L910" s="7" t="s">
-        <v>1529</v>
-      </c>
+        <v>217</v>
+      </c>
+      <c r="K910" s="23"/>
+      <c r="L910" s="7"/>
       <c r="M910" s="10" t="s">
         <v>1652</v>
       </c>
@@ -46341,26 +46348,22 @@
         <v>815</v>
       </c>
       <c r="D911" s="7" t="s">
-        <v>217</v>
+        <v>587</v>
       </c>
       <c r="E911" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F911" s="7" t="s">
-        <v>917</v>
-      </c>
-      <c r="G911" s="7">
-        <v>94</v>
+        <v>918</v>
+      </c>
+      <c r="G911" s="7" t="s">
+        <v>916</v>
       </c>
       <c r="H911" s="7" t="s">
-        <v>1376</v>
-      </c>
-      <c r="I911" s="7" t="s">
-        <v>961</v>
-      </c>
-      <c r="J911" s="7" t="s">
-        <v>217</v>
-      </c>
+        <v>1329</v>
+      </c>
+      <c r="I911" s="7"/>
+      <c r="J911" s="7"/>
       <c r="K911" s="23"/>
       <c r="L911" s="7"/>
       <c r="M911" s="10" t="s">
@@ -46378,10 +46381,10 @@
         <v>815</v>
       </c>
       <c r="D912" s="7" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="E912" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F912" s="7" t="s">
         <v>918</v>
@@ -46390,7 +46393,7 @@
         <v>916</v>
       </c>
       <c r="H912" s="7" t="s">
-        <v>1329</v>
+        <v>1332</v>
       </c>
       <c r="I912" s="7"/>
       <c r="J912" s="7"/>
@@ -46411,10 +46414,10 @@
         <v>815</v>
       </c>
       <c r="D913" s="7" t="s">
-        <v>584</v>
+        <v>794</v>
       </c>
       <c r="E913" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F913" s="7" t="s">
         <v>918</v>
@@ -46423,7 +46426,7 @@
         <v>916</v>
       </c>
       <c r="H913" s="7" t="s">
-        <v>1332</v>
+        <v>1210</v>
       </c>
       <c r="I913" s="7"/>
       <c r="J913" s="7"/>
@@ -46444,10 +46447,10 @@
         <v>815</v>
       </c>
       <c r="D914" s="7" t="s">
-        <v>794</v>
+        <v>744</v>
       </c>
       <c r="E914" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F914" s="7" t="s">
         <v>918</v>
@@ -46456,7 +46459,7 @@
         <v>916</v>
       </c>
       <c r="H914" s="7" t="s">
-        <v>1210</v>
+        <v>1245</v>
       </c>
       <c r="I914" s="7"/>
       <c r="J914" s="7"/>
@@ -46477,10 +46480,10 @@
         <v>815</v>
       </c>
       <c r="D915" s="7" t="s">
-        <v>744</v>
+        <v>750</v>
       </c>
       <c r="E915" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F915" s="7" t="s">
         <v>918</v>
@@ -46489,7 +46492,7 @@
         <v>916</v>
       </c>
       <c r="H915" s="7" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="I915" s="7"/>
       <c r="J915" s="7"/>
@@ -46510,10 +46513,10 @@
         <v>815</v>
       </c>
       <c r="D916" s="7" t="s">
-        <v>750</v>
+        <v>755</v>
       </c>
       <c r="E916" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F916" s="7" t="s">
         <v>918</v>
@@ -46522,7 +46525,7 @@
         <v>916</v>
       </c>
       <c r="H916" s="7" t="s">
-        <v>1244</v>
+        <v>1240</v>
       </c>
       <c r="I916" s="7"/>
       <c r="J916" s="7"/>
@@ -46543,10 +46546,10 @@
         <v>815</v>
       </c>
       <c r="D917" s="7" t="s">
-        <v>755</v>
+        <v>777</v>
       </c>
       <c r="E917" s="7">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F917" s="7" t="s">
         <v>918</v>
@@ -46555,7 +46558,7 @@
         <v>916</v>
       </c>
       <c r="H917" s="7" t="s">
-        <v>1240</v>
+        <v>1221</v>
       </c>
       <c r="I917" s="7"/>
       <c r="J917" s="7"/>
@@ -46576,10 +46579,10 @@
         <v>815</v>
       </c>
       <c r="D918" s="7" t="s">
-        <v>777</v>
+        <v>738</v>
       </c>
       <c r="E918" s="7">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F918" s="7" t="s">
         <v>918</v>
@@ -46588,7 +46591,7 @@
         <v>916</v>
       </c>
       <c r="H918" s="7" t="s">
-        <v>1221</v>
+        <v>1256</v>
       </c>
       <c r="I918" s="7"/>
       <c r="J918" s="7"/>
@@ -46609,10 +46612,10 @@
         <v>815</v>
       </c>
       <c r="D919" s="7" t="s">
-        <v>738</v>
+        <v>781</v>
       </c>
       <c r="E919" s="7">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F919" s="7" t="s">
         <v>918</v>
@@ -46621,7 +46624,7 @@
         <v>916</v>
       </c>
       <c r="H919" s="7" t="s">
-        <v>1256</v>
+        <v>1219</v>
       </c>
       <c r="I919" s="7"/>
       <c r="J919" s="7"/>
@@ -46642,10 +46645,10 @@
         <v>815</v>
       </c>
       <c r="D920" s="7" t="s">
-        <v>781</v>
+        <v>730</v>
       </c>
       <c r="E920" s="7">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F920" s="7" t="s">
         <v>918</v>
@@ -46654,7 +46657,7 @@
         <v>916</v>
       </c>
       <c r="H920" s="7" t="s">
-        <v>1219</v>
+        <v>1258</v>
       </c>
       <c r="I920" s="7"/>
       <c r="J920" s="7"/>
@@ -46675,10 +46678,10 @@
         <v>815</v>
       </c>
       <c r="D921" s="7" t="s">
-        <v>730</v>
+        <v>753</v>
       </c>
       <c r="E921" s="7">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F921" s="7" t="s">
         <v>918</v>
@@ -46687,7 +46690,7 @@
         <v>916</v>
       </c>
       <c r="H921" s="7" t="s">
-        <v>1258</v>
+        <v>1242</v>
       </c>
       <c r="I921" s="7"/>
       <c r="J921" s="7"/>
@@ -46708,10 +46711,10 @@
         <v>815</v>
       </c>
       <c r="D922" s="7" t="s">
-        <v>753</v>
+        <v>727</v>
       </c>
       <c r="E922" s="7">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F922" s="7" t="s">
         <v>918</v>
@@ -46720,7 +46723,7 @@
         <v>916</v>
       </c>
       <c r="H922" s="7" t="s">
-        <v>1242</v>
+        <v>1216</v>
       </c>
       <c r="I922" s="7"/>
       <c r="J922" s="7"/>
@@ -46741,10 +46744,10 @@
         <v>815</v>
       </c>
       <c r="D923" s="7" t="s">
-        <v>727</v>
+        <v>787</v>
       </c>
       <c r="E923" s="7">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F923" s="7" t="s">
         <v>918</v>
@@ -46753,7 +46756,7 @@
         <v>916</v>
       </c>
       <c r="H923" s="7" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="I923" s="7"/>
       <c r="J923" s="7"/>
@@ -46774,24 +46777,32 @@
         <v>815</v>
       </c>
       <c r="D924" s="7" t="s">
-        <v>787</v>
+        <v>512</v>
       </c>
       <c r="E924" s="7">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F924" s="7" t="s">
-        <v>918</v>
-      </c>
-      <c r="G924" s="7" t="s">
-        <v>916</v>
+        <v>917</v>
+      </c>
+      <c r="G924" s="7">
+        <v>8</v>
       </c>
       <c r="H924" s="7" t="s">
-        <v>1215</v>
-      </c>
-      <c r="I924" s="7"/>
-      <c r="J924" s="7"/>
-      <c r="K924" s="23"/>
-      <c r="L924" s="7"/>
+        <v>1531</v>
+      </c>
+      <c r="I924" s="7" t="s">
+        <v>992</v>
+      </c>
+      <c r="J924" s="7" t="s">
+        <v>511</v>
+      </c>
+      <c r="K924" s="23" t="s">
+        <v>819</v>
+      </c>
+      <c r="L924" s="7" t="s">
+        <v>1522</v>
+      </c>
       <c r="M924" s="10" t="s">
         <v>1652</v>
       </c>
@@ -46807,32 +46818,24 @@
         <v>815</v>
       </c>
       <c r="D925" s="7" t="s">
-        <v>512</v>
+        <v>735</v>
       </c>
       <c r="E925" s="7">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F925" s="7" t="s">
-        <v>917</v>
-      </c>
-      <c r="G925" s="7">
-        <v>8</v>
+        <v>918</v>
+      </c>
+      <c r="G925" s="7" t="s">
+        <v>916</v>
       </c>
       <c r="H925" s="7" t="s">
-        <v>1531</v>
-      </c>
-      <c r="I925" s="7" t="s">
-        <v>992</v>
-      </c>
-      <c r="J925" s="7" t="s">
-        <v>511</v>
-      </c>
-      <c r="K925" s="23" t="s">
-        <v>819</v>
-      </c>
-      <c r="L925" s="7" t="s">
-        <v>1522</v>
-      </c>
+        <v>1259</v>
+      </c>
+      <c r="I925" s="7"/>
+      <c r="J925" s="7"/>
+      <c r="K925" s="23"/>
+      <c r="L925" s="7"/>
       <c r="M925" s="10" t="s">
         <v>1652</v>
       </c>
@@ -46848,10 +46851,10 @@
         <v>815</v>
       </c>
       <c r="D926" s="7" t="s">
-        <v>735</v>
+        <v>771</v>
       </c>
       <c r="E926" s="7">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F926" s="7" t="s">
         <v>918</v>
@@ -46860,7 +46863,7 @@
         <v>916</v>
       </c>
       <c r="H926" s="7" t="s">
-        <v>1259</v>
+        <v>1227</v>
       </c>
       <c r="I926" s="7"/>
       <c r="J926" s="7"/>
@@ -46881,10 +46884,10 @@
         <v>815</v>
       </c>
       <c r="D927" s="7" t="s">
-        <v>771</v>
+        <v>749</v>
       </c>
       <c r="E927" s="7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F927" s="7" t="s">
         <v>918</v>
@@ -46893,7 +46896,7 @@
         <v>916</v>
       </c>
       <c r="H927" s="7" t="s">
-        <v>1227</v>
+        <v>1246</v>
       </c>
       <c r="I927" s="7"/>
       <c r="J927" s="7"/>
@@ -46914,10 +46917,10 @@
         <v>815</v>
       </c>
       <c r="D928" s="7" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
       <c r="E928" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F928" s="7" t="s">
         <v>918</v>
@@ -46926,7 +46929,7 @@
         <v>916</v>
       </c>
       <c r="H928" s="7" t="s">
-        <v>1246</v>
+        <v>1249</v>
       </c>
       <c r="I928" s="7"/>
       <c r="J928" s="7"/>
@@ -46947,10 +46950,10 @@
         <v>815</v>
       </c>
       <c r="D929" s="7" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="E929" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F929" s="7" t="s">
         <v>918</v>
@@ -46959,7 +46962,7 @@
         <v>916</v>
       </c>
       <c r="H929" s="7" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="I929" s="7"/>
       <c r="J929" s="7"/>
@@ -46980,10 +46983,10 @@
         <v>815</v>
       </c>
       <c r="D930" s="7" t="s">
-        <v>748</v>
+        <v>707</v>
       </c>
       <c r="E930" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F930" s="7" t="s">
         <v>918</v>
@@ -46992,7 +46995,7 @@
         <v>916</v>
       </c>
       <c r="H930" s="7" t="s">
-        <v>1247</v>
+        <v>1277</v>
       </c>
       <c r="I930" s="7"/>
       <c r="J930" s="7"/>
@@ -47013,10 +47016,10 @@
         <v>815</v>
       </c>
       <c r="D931" s="7" t="s">
-        <v>707</v>
+        <v>714</v>
       </c>
       <c r="E931" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F931" s="7" t="s">
         <v>918</v>
@@ -47025,7 +47028,7 @@
         <v>916</v>
       </c>
       <c r="H931" s="7" t="s">
-        <v>1277</v>
+        <v>1272</v>
       </c>
       <c r="I931" s="7"/>
       <c r="J931" s="7"/>
@@ -47046,10 +47049,10 @@
         <v>815</v>
       </c>
       <c r="D932" s="7" t="s">
-        <v>714</v>
+        <v>708</v>
       </c>
       <c r="E932" s="7">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F932" s="7" t="s">
         <v>918</v>
@@ -47058,7 +47061,7 @@
         <v>916</v>
       </c>
       <c r="H932" s="7" t="s">
-        <v>1272</v>
+        <v>1276</v>
       </c>
       <c r="I932" s="7"/>
       <c r="J932" s="7"/>
@@ -47079,10 +47082,10 @@
         <v>815</v>
       </c>
       <c r="D933" s="7" t="s">
-        <v>708</v>
+        <v>713</v>
       </c>
       <c r="E933" s="7">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F933" s="7" t="s">
         <v>918</v>
@@ -47091,7 +47094,7 @@
         <v>916</v>
       </c>
       <c r="H933" s="7" t="s">
-        <v>1276</v>
+        <v>1273</v>
       </c>
       <c r="I933" s="7"/>
       <c r="J933" s="7"/>
@@ -47112,10 +47115,10 @@
         <v>815</v>
       </c>
       <c r="D934" s="7" t="s">
-        <v>713</v>
+        <v>776</v>
       </c>
       <c r="E934" s="7">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F934" s="7" t="s">
         <v>918</v>
@@ -47124,7 +47127,7 @@
         <v>916</v>
       </c>
       <c r="H934" s="7" t="s">
-        <v>1273</v>
+        <v>1222</v>
       </c>
       <c r="I934" s="7"/>
       <c r="J934" s="7"/>
@@ -47145,10 +47148,10 @@
         <v>815</v>
       </c>
       <c r="D935" s="7" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="E935" s="7">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F935" s="7" t="s">
         <v>918</v>
@@ -47157,7 +47160,7 @@
         <v>916</v>
       </c>
       <c r="H935" s="7" t="s">
-        <v>1222</v>
+        <v>1226</v>
       </c>
       <c r="I935" s="7"/>
       <c r="J935" s="7"/>
@@ -47178,10 +47181,10 @@
         <v>815</v>
       </c>
       <c r="D936" s="7" t="s">
-        <v>772</v>
+        <v>775</v>
       </c>
       <c r="E936" s="7">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F936" s="7" t="s">
         <v>918</v>
@@ -47190,7 +47193,7 @@
         <v>916</v>
       </c>
       <c r="H936" s="7" t="s">
-        <v>1226</v>
+        <v>1223</v>
       </c>
       <c r="I936" s="7"/>
       <c r="J936" s="7"/>
@@ -47211,10 +47214,10 @@
         <v>815</v>
       </c>
       <c r="D937" s="7" t="s">
-        <v>775</v>
+        <v>717</v>
       </c>
       <c r="E937" s="7">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F937" s="7" t="s">
         <v>918</v>
@@ -47223,7 +47226,7 @@
         <v>916</v>
       </c>
       <c r="H937" s="7" t="s">
-        <v>1223</v>
+        <v>1270</v>
       </c>
       <c r="I937" s="7"/>
       <c r="J937" s="7"/>
@@ -47244,10 +47247,10 @@
         <v>815</v>
       </c>
       <c r="D938" s="7" t="s">
-        <v>717</v>
+        <v>721</v>
       </c>
       <c r="E938" s="7">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F938" s="7" t="s">
         <v>918</v>
@@ -47256,7 +47259,7 @@
         <v>916</v>
       </c>
       <c r="H938" s="7" t="s">
-        <v>1270</v>
+        <v>1266</v>
       </c>
       <c r="I938" s="7"/>
       <c r="J938" s="7"/>
@@ -47277,10 +47280,10 @@
         <v>815</v>
       </c>
       <c r="D939" s="7" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="E939" s="7">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F939" s="7" t="s">
         <v>918</v>
@@ -47289,7 +47292,7 @@
         <v>916</v>
       </c>
       <c r="H939" s="7" t="s">
-        <v>1266</v>
+        <v>1269</v>
       </c>
       <c r="I939" s="7"/>
       <c r="J939" s="7"/>
@@ -47310,10 +47313,10 @@
         <v>815</v>
       </c>
       <c r="D940" s="7" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="E940" s="7">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F940" s="7" t="s">
         <v>918</v>
@@ -47322,7 +47325,7 @@
         <v>916</v>
       </c>
       <c r="H940" s="7" t="s">
-        <v>1269</v>
+        <v>1267</v>
       </c>
       <c r="I940" s="7"/>
       <c r="J940" s="7"/>
@@ -47343,10 +47346,10 @@
         <v>815</v>
       </c>
       <c r="D941" s="7" t="s">
-        <v>720</v>
+        <v>729</v>
       </c>
       <c r="E941" s="7">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F941" s="7" t="s">
         <v>918</v>
@@ -47355,7 +47358,7 @@
         <v>916</v>
       </c>
       <c r="H941" s="7" t="s">
-        <v>1267</v>
+        <v>1262</v>
       </c>
       <c r="I941" s="7"/>
       <c r="J941" s="7"/>
@@ -47376,19 +47379,19 @@
         <v>815</v>
       </c>
       <c r="D942" s="7" t="s">
-        <v>729</v>
+        <v>494</v>
       </c>
       <c r="E942" s="7">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F942" s="7" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
       <c r="G942" s="7" t="s">
         <v>916</v>
       </c>
       <c r="H942" s="7" t="s">
-        <v>1262</v>
+        <v>1547</v>
       </c>
       <c r="I942" s="7"/>
       <c r="J942" s="7"/>
@@ -47409,24 +47412,32 @@
         <v>815</v>
       </c>
       <c r="D943" s="7" t="s">
-        <v>494</v>
+        <v>237</v>
       </c>
       <c r="E943" s="7">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F943" s="7" t="s">
-        <v>915</v>
-      </c>
-      <c r="G943" s="7" t="s">
-        <v>916</v>
+        <v>917</v>
+      </c>
+      <c r="G943" s="7">
+        <v>20</v>
       </c>
       <c r="H943" s="7" t="s">
-        <v>1547</v>
-      </c>
-      <c r="I943" s="7"/>
-      <c r="J943" s="7"/>
-      <c r="K943" s="23"/>
-      <c r="L943" s="7"/>
+        <v>1369</v>
+      </c>
+      <c r="I943" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="J943" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="K943" s="23" t="s">
+        <v>875</v>
+      </c>
+      <c r="L943" s="7" t="s">
+        <v>1369</v>
+      </c>
       <c r="M943" s="10" t="s">
         <v>1652</v>
       </c>
@@ -47442,31 +47453,31 @@
         <v>815</v>
       </c>
       <c r="D944" s="7" t="s">
-        <v>237</v>
+        <v>616</v>
       </c>
       <c r="E944" s="7">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F944" s="7" t="s">
         <v>917</v>
       </c>
       <c r="G944" s="7">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H944" s="7" t="s">
-        <v>1369</v>
+        <v>1315</v>
       </c>
       <c r="I944" s="7" t="s">
         <v>93</v>
       </c>
       <c r="J944" s="7" t="s">
-        <v>237</v>
+        <v>616</v>
       </c>
       <c r="K944" s="23" t="s">
         <v>875</v>
       </c>
       <c r="L944" s="7" t="s">
-        <v>1369</v>
+        <v>1315</v>
       </c>
       <c r="M944" s="10" t="s">
         <v>1652</v>
@@ -47483,32 +47494,24 @@
         <v>815</v>
       </c>
       <c r="D945" s="7" t="s">
-        <v>616</v>
+        <v>734</v>
       </c>
       <c r="E945" s="7">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F945" s="7" t="s">
-        <v>917</v>
-      </c>
-      <c r="G945" s="7">
-        <v>12</v>
+        <v>918</v>
+      </c>
+      <c r="G945" s="7" t="s">
+        <v>916</v>
       </c>
       <c r="H945" s="7" t="s">
-        <v>1315</v>
-      </c>
-      <c r="I945" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="J945" s="7" t="s">
-        <v>616</v>
-      </c>
-      <c r="K945" s="23" t="s">
-        <v>875</v>
-      </c>
-      <c r="L945" s="7" t="s">
-        <v>1315</v>
-      </c>
+        <v>795</v>
+      </c>
+      <c r="I945" s="7"/>
+      <c r="J945" s="7"/>
+      <c r="K945" s="23"/>
+      <c r="L945" s="7"/>
       <c r="M945" s="10" t="s">
         <v>1652</v>
       </c>
@@ -47524,10 +47527,10 @@
         <v>815</v>
       </c>
       <c r="D946" s="7" t="s">
-        <v>734</v>
+        <v>700</v>
       </c>
       <c r="E946" s="7">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F946" s="7" t="s">
         <v>918</v>
@@ -47536,7 +47539,7 @@
         <v>916</v>
       </c>
       <c r="H946" s="7" t="s">
-        <v>795</v>
+        <v>1283</v>
       </c>
       <c r="I946" s="7"/>
       <c r="J946" s="7"/>
@@ -47557,10 +47560,10 @@
         <v>815</v>
       </c>
       <c r="D947" s="7" t="s">
-        <v>700</v>
+        <v>773</v>
       </c>
       <c r="E947" s="7">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F947" s="7" t="s">
         <v>918</v>
@@ -47569,7 +47572,7 @@
         <v>916</v>
       </c>
       <c r="H947" s="7" t="s">
-        <v>1283</v>
+        <v>1225</v>
       </c>
       <c r="I947" s="7"/>
       <c r="J947" s="7"/>
@@ -47590,10 +47593,10 @@
         <v>815</v>
       </c>
       <c r="D948" s="7" t="s">
-        <v>773</v>
+        <v>710</v>
       </c>
       <c r="E948" s="7">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F948" s="7" t="s">
         <v>918</v>
@@ -47602,7 +47605,7 @@
         <v>916</v>
       </c>
       <c r="H948" s="7" t="s">
-        <v>1225</v>
+        <v>1275</v>
       </c>
       <c r="I948" s="7"/>
       <c r="J948" s="7"/>
@@ -47623,10 +47626,10 @@
         <v>815</v>
       </c>
       <c r="D949" s="7" t="s">
-        <v>710</v>
+        <v>704</v>
       </c>
       <c r="E949" s="7">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F949" s="7" t="s">
         <v>918</v>
@@ -47635,7 +47638,7 @@
         <v>916</v>
       </c>
       <c r="H949" s="7" t="s">
-        <v>1275</v>
+        <v>1279</v>
       </c>
       <c r="I949" s="7"/>
       <c r="J949" s="7"/>
@@ -47656,19 +47659,19 @@
         <v>815</v>
       </c>
       <c r="D950" s="7" t="s">
-        <v>704</v>
+        <v>384</v>
       </c>
       <c r="E950" s="7">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F950" s="7" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="G950" s="7" t="s">
         <v>916</v>
       </c>
       <c r="H950" s="7" t="s">
-        <v>1279</v>
+        <v>1406</v>
       </c>
       <c r="I950" s="7"/>
       <c r="J950" s="7"/>
@@ -47689,24 +47692,32 @@
         <v>815</v>
       </c>
       <c r="D951" s="7" t="s">
-        <v>384</v>
+        <v>686</v>
       </c>
       <c r="E951" s="7">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F951" s="7" t="s">
-        <v>919</v>
-      </c>
-      <c r="G951" s="7" t="s">
-        <v>916</v>
+        <v>917</v>
+      </c>
+      <c r="G951" s="7">
+        <v>20</v>
       </c>
       <c r="H951" s="7" t="s">
-        <v>1406</v>
-      </c>
-      <c r="I951" s="7"/>
-      <c r="J951" s="7"/>
-      <c r="K951" s="23"/>
-      <c r="L951" s="7"/>
+        <v>1586</v>
+      </c>
+      <c r="I951" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J951" s="7" t="s">
+        <v>686</v>
+      </c>
+      <c r="K951" s="23" t="s">
+        <v>837</v>
+      </c>
+      <c r="L951" s="7" t="s">
+        <v>1586</v>
+      </c>
       <c r="M951" s="10" t="s">
         <v>1652</v>
       </c>
@@ -47722,32 +47733,24 @@
         <v>815</v>
       </c>
       <c r="D952" s="7" t="s">
-        <v>686</v>
-      </c>
-      <c r="E952" s="7">
-        <v>46</v>
+        <v>1524</v>
+      </c>
+      <c r="E952" s="22">
+        <v>47</v>
       </c>
       <c r="F952" s="7" t="s">
         <v>917</v>
       </c>
       <c r="G952" s="7">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H952" s="7" t="s">
-        <v>1586</v>
-      </c>
-      <c r="I952" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="J952" s="7" t="s">
-        <v>686</v>
-      </c>
-      <c r="K952" s="23" t="s">
-        <v>837</v>
-      </c>
-      <c r="L952" s="7" t="s">
-        <v>1586</v>
-      </c>
+        <v>1524</v>
+      </c>
+      <c r="I952" s="7"/>
+      <c r="J952" s="7"/>
+      <c r="K952" s="23"/>
+      <c r="L952" s="7"/>
       <c r="M952" s="10" t="s">
         <v>1652</v>
       </c>
@@ -47763,19 +47766,17 @@
         <v>815</v>
       </c>
       <c r="D953" s="7" t="s">
-        <v>1524</v>
+        <v>1282</v>
       </c>
       <c r="E953" s="22">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F953" s="7" t="s">
-        <v>917</v>
-      </c>
-      <c r="G953" s="7">
-        <v>30</v>
-      </c>
+        <v>918</v>
+      </c>
+      <c r="G953" s="7"/>
       <c r="H953" s="7" t="s">
-        <v>1524</v>
+        <v>1282</v>
       </c>
       <c r="I953" s="7"/>
       <c r="J953" s="7"/>
@@ -47796,17 +47797,17 @@
         <v>815</v>
       </c>
       <c r="D954" s="7" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="E954" s="22">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F954" s="7" t="s">
         <v>918</v>
       </c>
       <c r="G954" s="7"/>
       <c r="H954" s="7" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="I954" s="7"/>
       <c r="J954" s="7"/>
@@ -47821,28 +47822,38 @@
         <v>1105</v>
       </c>
       <c r="B955" s="7" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="C955" s="7" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="D955" s="7" t="s">
-        <v>1281</v>
-      </c>
-      <c r="E955" s="22">
-        <v>49</v>
+        <v>292</v>
+      </c>
+      <c r="E955" s="7">
+        <v>1</v>
       </c>
       <c r="F955" s="7" t="s">
-        <v>918</v>
-      </c>
-      <c r="G955" s="7"/>
+        <v>915</v>
+      </c>
+      <c r="G955" s="7" t="s">
+        <v>916</v>
+      </c>
       <c r="H955" s="7" t="s">
-        <v>1281</v>
-      </c>
-      <c r="I955" s="7"/>
-      <c r="J955" s="7"/>
-      <c r="K955" s="23"/>
-      <c r="L955" s="7"/>
+        <v>1175</v>
+      </c>
+      <c r="I955" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J955" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="K955" s="23" t="s">
+        <v>837</v>
+      </c>
+      <c r="L955" s="7" t="s">
+        <v>1175</v>
+      </c>
       <c r="M955" s="10" t="s">
         <v>1652</v>
       </c>
@@ -47858,31 +47869,31 @@
         <v>816</v>
       </c>
       <c r="D956" s="7" t="s">
-        <v>292</v>
+        <v>212</v>
       </c>
       <c r="E956" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F956" s="7" t="s">
-        <v>915</v>
-      </c>
-      <c r="G956" s="7" t="s">
-        <v>916</v>
+        <v>917</v>
+      </c>
+      <c r="G956" s="7">
+        <v>12</v>
       </c>
       <c r="H956" s="7" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="I956" s="7" t="s">
         <v>73</v>
       </c>
       <c r="J956" s="7" t="s">
-        <v>184</v>
+        <v>212</v>
       </c>
       <c r="K956" s="23" t="s">
         <v>837</v>
       </c>
       <c r="L956" s="7" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="M956" s="10" t="s">
         <v>1652</v>
@@ -47899,32 +47910,24 @@
         <v>816</v>
       </c>
       <c r="D957" s="7" t="s">
-        <v>212</v>
+        <v>502</v>
       </c>
       <c r="E957" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F957" s="7" t="s">
-        <v>917</v>
-      </c>
-      <c r="G957" s="7">
-        <v>12</v>
+        <v>915</v>
+      </c>
+      <c r="G957" s="7" t="s">
+        <v>916</v>
       </c>
       <c r="H957" s="7" t="s">
-        <v>1174</v>
-      </c>
-      <c r="I957" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="J957" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="K957" s="23" t="s">
-        <v>837</v>
-      </c>
-      <c r="L957" s="7" t="s">
-        <v>1174</v>
-      </c>
+        <v>1673</v>
+      </c>
+      <c r="I957" s="7"/>
+      <c r="J957" s="7"/>
+      <c r="K957" s="23"/>
+      <c r="L957" s="7"/>
       <c r="M957" s="10" t="s">
         <v>1652</v>
       </c>
@@ -47940,19 +47943,19 @@
         <v>816</v>
       </c>
       <c r="D958" s="7" t="s">
-        <v>502</v>
+        <v>627</v>
       </c>
       <c r="E958" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F958" s="7" t="s">
-        <v>915</v>
-      </c>
-      <c r="G958" s="7" t="s">
-        <v>916</v>
+        <v>917</v>
+      </c>
+      <c r="G958" s="7">
+        <v>16</v>
       </c>
       <c r="H958" s="7" t="s">
-        <v>1673</v>
+        <v>1674</v>
       </c>
       <c r="I958" s="7"/>
       <c r="J958" s="7"/>
@@ -47973,24 +47976,32 @@
         <v>816</v>
       </c>
       <c r="D959" s="7" t="s">
-        <v>627</v>
+        <v>258</v>
       </c>
       <c r="E959" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F959" s="7" t="s">
-        <v>917</v>
-      </c>
-      <c r="G959" s="7">
-        <v>16</v>
+        <v>915</v>
+      </c>
+      <c r="G959" s="7" t="s">
+        <v>916</v>
       </c>
       <c r="H959" s="7" t="s">
-        <v>1674</v>
-      </c>
-      <c r="I959" s="7"/>
-      <c r="J959" s="7"/>
-      <c r="K959" s="23"/>
-      <c r="L959" s="7"/>
+        <v>1453</v>
+      </c>
+      <c r="I959" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="J959" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="K959" s="23" t="s">
+        <v>904</v>
+      </c>
+      <c r="L959" s="7" t="s">
+        <v>1453</v>
+      </c>
       <c r="M959" s="10" t="s">
         <v>1652</v>
       </c>
@@ -48006,32 +48017,24 @@
         <v>816</v>
       </c>
       <c r="D960" s="7" t="s">
-        <v>258</v>
+        <v>2164</v>
       </c>
       <c r="E960" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F960" s="7" t="s">
-        <v>915</v>
-      </c>
-      <c r="G960" s="7" t="s">
-        <v>916</v>
+        <v>917</v>
+      </c>
+      <c r="G960" s="7">
+        <v>60</v>
       </c>
       <c r="H960" s="7" t="s">
-        <v>1453</v>
-      </c>
-      <c r="I960" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="J960" s="7" t="s">
-        <v>258</v>
-      </c>
-      <c r="K960" s="23" t="s">
-        <v>904</v>
-      </c>
-      <c r="L960" s="7" t="s">
-        <v>1453</v>
-      </c>
+        <v>2165</v>
+      </c>
+      <c r="I960" s="7"/>
+      <c r="J960" s="7"/>
+      <c r="K960" s="23"/>
+      <c r="L960" s="7"/>
       <c r="M960" s="10" t="s">
         <v>1652</v>
       </c>
@@ -48047,19 +48050,19 @@
         <v>816</v>
       </c>
       <c r="D961" s="7" t="s">
-        <v>2164</v>
+        <v>156</v>
       </c>
       <c r="E961" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F961" s="7" t="s">
         <v>917</v>
       </c>
       <c r="G961" s="7">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="H961" s="7" t="s">
-        <v>2165</v>
+        <v>1496</v>
       </c>
       <c r="I961" s="7"/>
       <c r="J961" s="7"/>
@@ -48080,19 +48083,19 @@
         <v>816</v>
       </c>
       <c r="D962" s="7" t="s">
-        <v>156</v>
+        <v>409</v>
       </c>
       <c r="E962" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F962" s="7" t="s">
-        <v>917</v>
-      </c>
-      <c r="G962" s="7">
-        <v>100</v>
+        <v>919</v>
+      </c>
+      <c r="G962" s="7" t="s">
+        <v>916</v>
       </c>
       <c r="H962" s="7" t="s">
-        <v>1496</v>
+        <v>409</v>
       </c>
       <c r="I962" s="7"/>
       <c r="J962" s="7"/>
@@ -48113,10 +48116,10 @@
         <v>816</v>
       </c>
       <c r="D963" s="7" t="s">
-        <v>409</v>
+        <v>387</v>
       </c>
       <c r="E963" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F963" s="7" t="s">
         <v>919</v>
@@ -48125,7 +48128,7 @@
         <v>916</v>
       </c>
       <c r="H963" s="7" t="s">
-        <v>409</v>
+        <v>387</v>
       </c>
       <c r="I963" s="7"/>
       <c r="J963" s="7"/>
@@ -48146,24 +48149,32 @@
         <v>816</v>
       </c>
       <c r="D964" s="7" t="s">
-        <v>387</v>
+        <v>230</v>
       </c>
       <c r="E964" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F964" s="7" t="s">
-        <v>919</v>
-      </c>
-      <c r="G964" s="7" t="s">
-        <v>916</v>
+        <v>917</v>
+      </c>
+      <c r="G964" s="7">
+        <v>20</v>
       </c>
       <c r="H964" s="7" t="s">
-        <v>387</v>
-      </c>
-      <c r="I964" s="7"/>
-      <c r="J964" s="7"/>
-      <c r="K964" s="23"/>
-      <c r="L964" s="7"/>
+        <v>1460</v>
+      </c>
+      <c r="I964" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="J964" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="K964" s="23" t="s">
+        <v>876</v>
+      </c>
+      <c r="L964" s="7" t="s">
+        <v>1613</v>
+      </c>
       <c r="M964" s="10" t="s">
         <v>1652</v>
       </c>
@@ -48179,10 +48190,10 @@
         <v>816</v>
       </c>
       <c r="D965" s="7" t="s">
-        <v>230</v>
+        <v>686</v>
       </c>
       <c r="E965" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F965" s="7" t="s">
         <v>917</v>
@@ -48191,19 +48202,19 @@
         <v>20</v>
       </c>
       <c r="H965" s="7" t="s">
-        <v>1460</v>
+        <v>1586</v>
       </c>
       <c r="I965" s="7" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="J965" s="7" t="s">
-        <v>231</v>
+        <v>686</v>
       </c>
       <c r="K965" s="23" t="s">
-        <v>876</v>
+        <v>837</v>
       </c>
       <c r="L965" s="7" t="s">
-        <v>1613</v>
+        <v>1586</v>
       </c>
       <c r="M965" s="10" t="s">
         <v>1652</v>
@@ -48220,32 +48231,24 @@
         <v>816</v>
       </c>
       <c r="D966" s="7" t="s">
-        <v>686</v>
-      </c>
-      <c r="E966" s="7">
-        <v>11</v>
+        <v>1524</v>
+      </c>
+      <c r="E966" s="22">
+        <v>12</v>
       </c>
       <c r="F966" s="7" t="s">
         <v>917</v>
       </c>
       <c r="G966" s="7">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H966" s="7" t="s">
-        <v>1586</v>
-      </c>
-      <c r="I966" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="J966" s="7" t="s">
-        <v>686</v>
-      </c>
-      <c r="K966" s="23" t="s">
-        <v>837</v>
-      </c>
-      <c r="L966" s="7" t="s">
-        <v>1586</v>
-      </c>
+        <v>1524</v>
+      </c>
+      <c r="I966" s="7"/>
+      <c r="J966" s="7"/>
+      <c r="K966" s="23"/>
+      <c r="L966" s="7"/>
       <c r="M966" s="10" t="s">
         <v>1652</v>
       </c>
@@ -48255,30 +48258,38 @@
         <v>1105</v>
       </c>
       <c r="B967" s="7" t="s">
-        <v>991</v>
+        <v>998</v>
       </c>
       <c r="C967" s="7" t="s">
-        <v>816</v>
+        <v>823</v>
       </c>
       <c r="D967" s="7" t="s">
-        <v>1524</v>
-      </c>
-      <c r="E967" s="22">
-        <v>12</v>
+        <v>292</v>
+      </c>
+      <c r="E967" s="7">
+        <v>1</v>
       </c>
       <c r="F967" s="7" t="s">
-        <v>917</v>
-      </c>
-      <c r="G967" s="7">
-        <v>30</v>
+        <v>915</v>
+      </c>
+      <c r="G967" s="7" t="s">
+        <v>916</v>
       </c>
       <c r="H967" s="7" t="s">
-        <v>1524</v>
-      </c>
-      <c r="I967" s="7"/>
-      <c r="J967" s="7"/>
-      <c r="K967" s="23"/>
-      <c r="L967" s="7"/>
+        <v>1175</v>
+      </c>
+      <c r="I967" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J967" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="K967" s="23" t="s">
+        <v>837</v>
+      </c>
+      <c r="L967" s="7" t="s">
+        <v>1175</v>
+      </c>
       <c r="M967" s="10" t="s">
         <v>1652</v>
       </c>
@@ -48294,31 +48305,31 @@
         <v>823</v>
       </c>
       <c r="D968" s="7" t="s">
-        <v>292</v>
+        <v>181</v>
       </c>
       <c r="E968" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F968" s="7" t="s">
-        <v>915</v>
-      </c>
-      <c r="G968" s="7" t="s">
-        <v>916</v>
+        <v>917</v>
+      </c>
+      <c r="G968" s="7">
+        <v>6</v>
       </c>
       <c r="H968" s="7" t="s">
-        <v>1175</v>
+        <v>1485</v>
       </c>
       <c r="I968" s="7" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="J968" s="7" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="K968" s="23" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="L968" s="7" t="s">
-        <v>1175</v>
+        <v>1503</v>
       </c>
       <c r="M968" s="10" t="s">
         <v>1652</v>
@@ -48335,32 +48346,28 @@
         <v>823</v>
       </c>
       <c r="D969" s="7" t="s">
-        <v>181</v>
+        <v>202</v>
       </c>
       <c r="E969" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F969" s="7" t="s">
         <v>917</v>
       </c>
       <c r="G969" s="7">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="H969" s="7" t="s">
-        <v>1485</v>
+        <v>1475</v>
       </c>
       <c r="I969" s="7" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="J969" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="K969" s="23" t="s">
-        <v>835</v>
-      </c>
-      <c r="L969" s="7" t="s">
-        <v>1503</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="K969" s="23"/>
+      <c r="L969" s="7"/>
       <c r="M969" s="10" t="s">
         <v>1652</v>
       </c>
@@ -48376,26 +48383,22 @@
         <v>823</v>
       </c>
       <c r="D970" s="7" t="s">
-        <v>202</v>
+        <v>322</v>
       </c>
       <c r="E970" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F970" s="7" t="s">
-        <v>917</v>
-      </c>
-      <c r="G970" s="7">
-        <v>12</v>
+        <v>919</v>
+      </c>
+      <c r="G970" s="7" t="s">
+        <v>916</v>
       </c>
       <c r="H970" s="7" t="s">
-        <v>1475</v>
-      </c>
-      <c r="I970" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="J970" s="7" t="s">
-        <v>202</v>
-      </c>
+        <v>1420</v>
+      </c>
+      <c r="I970" s="7"/>
+      <c r="J970" s="7"/>
       <c r="K970" s="23"/>
       <c r="L970" s="7"/>
       <c r="M970" s="10" t="s">
@@ -48413,19 +48416,19 @@
         <v>823</v>
       </c>
       <c r="D971" s="7" t="s">
-        <v>322</v>
+        <v>765</v>
       </c>
       <c r="E971" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F971" s="7" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="G971" s="7" t="s">
         <v>916</v>
       </c>
       <c r="H971" s="7" t="s">
-        <v>1420</v>
+        <v>1231</v>
       </c>
       <c r="I971" s="7"/>
       <c r="J971" s="7"/>
@@ -48446,24 +48449,32 @@
         <v>823</v>
       </c>
       <c r="D972" s="7" t="s">
-        <v>765</v>
+        <v>671</v>
       </c>
       <c r="E972" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F972" s="7" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
       <c r="G972" s="7" t="s">
         <v>916</v>
       </c>
       <c r="H972" s="7" t="s">
-        <v>1231</v>
-      </c>
-      <c r="I972" s="7"/>
-      <c r="J972" s="7"/>
-      <c r="K972" s="23"/>
-      <c r="L972" s="7"/>
+        <v>2324</v>
+      </c>
+      <c r="I972" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="J972" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="K972" s="23" t="s">
+        <v>881</v>
+      </c>
+      <c r="L972" s="7" t="s">
+        <v>1297</v>
+      </c>
       <c r="M972" s="10" t="s">
         <v>1652</v>
       </c>
@@ -48479,65 +48490,65 @@
         <v>823</v>
       </c>
       <c r="D973" s="7" t="s">
-        <v>671</v>
+        <v>300</v>
       </c>
       <c r="E973" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F973" s="7" t="s">
+        <v>919</v>
+      </c>
+      <c r="G973" s="7" t="s">
+        <v>916</v>
+      </c>
+      <c r="H973" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="I973" s="7"/>
+      <c r="J973" s="7"/>
+      <c r="K973" s="23"/>
+      <c r="L973" s="7"/>
+      <c r="M973" s="10" t="s">
+        <v>1652</v>
+      </c>
+    </row>
+    <row r="974" spans="1:13">
+      <c r="A974" s="6" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B974" s="7" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C974" s="7" t="s">
+        <v>826</v>
+      </c>
+      <c r="D974" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="E974" s="7">
+        <v>1</v>
+      </c>
+      <c r="F974" s="7" t="s">
         <v>915</v>
       </c>
-      <c r="G973" s="7" t="s">
-        <v>916</v>
-      </c>
-      <c r="H973" s="7" t="s">
-        <v>2324</v>
-      </c>
-      <c r="I973" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="J973" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="K973" s="23" t="s">
-        <v>881</v>
-      </c>
-      <c r="L973" s="7" t="s">
-        <v>1297</v>
-      </c>
-      <c r="M973" s="10" t="s">
-        <v>1652</v>
-      </c>
-    </row>
-    <row r="974" spans="1:13">
-      <c r="A974" s="7" t="s">
-        <v>1105</v>
-      </c>
-      <c r="B974" s="7" t="s">
-        <v>998</v>
-      </c>
-      <c r="C974" s="7" t="s">
-        <v>823</v>
-      </c>
-      <c r="D974" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="E974" s="7">
-        <v>7</v>
-      </c>
-      <c r="F974" s="7" t="s">
-        <v>919</v>
-      </c>
       <c r="G974" s="7" t="s">
         <v>916</v>
       </c>
       <c r="H974" s="7" t="s">
-        <v>383</v>
-      </c>
-      <c r="I974" s="7"/>
-      <c r="J974" s="7"/>
-      <c r="K974" s="23"/>
-      <c r="L974" s="7"/>
+        <v>1175</v>
+      </c>
+      <c r="I974" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J974" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="K974" s="23" t="s">
+        <v>837</v>
+      </c>
+      <c r="L974" s="7" t="s">
+        <v>1175</v>
+      </c>
       <c r="M974" s="10" t="s">
         <v>1652</v>
       </c>
@@ -48553,31 +48564,31 @@
         <v>826</v>
       </c>
       <c r="D975" s="7" t="s">
-        <v>292</v>
+        <v>212</v>
       </c>
       <c r="E975" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F975" s="7" t="s">
-        <v>915</v>
-      </c>
-      <c r="G975" s="7" t="s">
-        <v>916</v>
+        <v>917</v>
+      </c>
+      <c r="G975" s="7">
+        <v>12</v>
       </c>
       <c r="H975" s="7" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="I975" s="7" t="s">
         <v>73</v>
       </c>
       <c r="J975" s="7" t="s">
-        <v>184</v>
+        <v>212</v>
       </c>
       <c r="K975" s="23" t="s">
         <v>837</v>
       </c>
       <c r="L975" s="7" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="M975" s="10" t="s">
         <v>1652</v>
@@ -48594,32 +48605,24 @@
         <v>826</v>
       </c>
       <c r="D976" s="7" t="s">
-        <v>212</v>
+        <v>515</v>
       </c>
       <c r="E976" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F976" s="7" t="s">
         <v>917</v>
       </c>
       <c r="G976" s="7">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H976" s="7" t="s">
-        <v>1174</v>
-      </c>
-      <c r="I976" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="J976" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="K976" s="23" t="s">
-        <v>837</v>
-      </c>
-      <c r="L976" s="7" t="s">
-        <v>1174</v>
-      </c>
+        <v>1553</v>
+      </c>
+      <c r="I976" s="7"/>
+      <c r="J976" s="7"/>
+      <c r="K976" s="23"/>
+      <c r="L976" s="7"/>
       <c r="M976" s="10" t="s">
         <v>1652</v>
       </c>
@@ -48635,10 +48638,10 @@
         <v>826</v>
       </c>
       <c r="D977" s="7" t="s">
-        <v>515</v>
+        <v>213</v>
       </c>
       <c r="E977" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F977" s="7" t="s">
         <v>917</v>
@@ -48647,12 +48650,20 @@
         <v>18</v>
       </c>
       <c r="H977" s="7" t="s">
-        <v>1553</v>
-      </c>
-      <c r="I977" s="7"/>
-      <c r="J977" s="7"/>
-      <c r="K977" s="23"/>
-      <c r="L977" s="7"/>
+        <v>1470</v>
+      </c>
+      <c r="I977" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="J977" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="K977" s="23" t="s">
+        <v>882</v>
+      </c>
+      <c r="L977" s="7" t="s">
+        <v>1205</v>
+      </c>
       <c r="M977" s="10" t="s">
         <v>1652</v>
       </c>
@@ -48668,31 +48679,31 @@
         <v>826</v>
       </c>
       <c r="D978" s="7" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="E978" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F978" s="7" t="s">
         <v>917</v>
       </c>
       <c r="G978" s="7">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H978" s="7" t="s">
-        <v>1470</v>
+        <v>1369</v>
       </c>
       <c r="I978" s="7" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="J978" s="7" t="s">
-        <v>285</v>
+        <v>237</v>
       </c>
       <c r="K978" s="23" t="s">
-        <v>882</v>
+        <v>875</v>
       </c>
       <c r="L978" s="7" t="s">
-        <v>1205</v>
+        <v>1369</v>
       </c>
       <c r="M978" s="10" t="s">
         <v>1652</v>
@@ -48709,31 +48720,31 @@
         <v>826</v>
       </c>
       <c r="D979" s="7" t="s">
-        <v>237</v>
+        <v>623</v>
       </c>
       <c r="E979" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F979" s="7" t="s">
         <v>917</v>
       </c>
       <c r="G979" s="7">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="H979" s="7" t="s">
-        <v>1369</v>
+        <v>1315</v>
       </c>
       <c r="I979" s="7" t="s">
         <v>93</v>
       </c>
       <c r="J979" s="7" t="s">
-        <v>237</v>
+        <v>1109</v>
       </c>
       <c r="K979" s="23" t="s">
         <v>875</v>
       </c>
       <c r="L979" s="7" t="s">
-        <v>1369</v>
+        <v>1315</v>
       </c>
       <c r="M979" s="10" t="s">
         <v>1652</v>
@@ -48750,31 +48761,31 @@
         <v>826</v>
       </c>
       <c r="D980" s="7" t="s">
-        <v>623</v>
+        <v>196</v>
       </c>
       <c r="E980" s="7">
+        <v>7</v>
+      </c>
+      <c r="F980" s="7" t="s">
+        <v>917</v>
+      </c>
+      <c r="G980" s="7">
         <v>6</v>
       </c>
-      <c r="F980" s="7" t="s">
-        <v>917</v>
-      </c>
-      <c r="G980" s="7">
-        <v>2</v>
-      </c>
       <c r="H980" s="7" t="s">
-        <v>1315</v>
+        <v>1477</v>
       </c>
       <c r="I980" s="7" t="s">
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="J980" s="7" t="s">
-        <v>1109</v>
+        <v>196</v>
       </c>
       <c r="K980" s="23" t="s">
-        <v>875</v>
+        <v>839</v>
       </c>
       <c r="L980" s="7" t="s">
-        <v>1315</v>
+        <v>1477</v>
       </c>
       <c r="M980" s="10" t="s">
         <v>1652</v>
@@ -48791,32 +48802,24 @@
         <v>826</v>
       </c>
       <c r="D981" s="7" t="s">
-        <v>196</v>
+        <v>779</v>
       </c>
       <c r="E981" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F981" s="7" t="s">
-        <v>917</v>
-      </c>
-      <c r="G981" s="7">
-        <v>6</v>
+        <v>918</v>
+      </c>
+      <c r="G981" s="7" t="s">
+        <v>916</v>
       </c>
       <c r="H981" s="7" t="s">
-        <v>1477</v>
-      </c>
-      <c r="I981" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="J981" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="K981" s="23" t="s">
-        <v>839</v>
-      </c>
-      <c r="L981" s="7" t="s">
-        <v>1477</v>
-      </c>
+        <v>1698</v>
+      </c>
+      <c r="I981" s="7"/>
+      <c r="J981" s="7"/>
+      <c r="K981" s="23"/>
+      <c r="L981" s="7"/>
       <c r="M981" s="10" t="s">
         <v>1652</v>
       </c>
@@ -48832,24 +48835,32 @@
         <v>826</v>
       </c>
       <c r="D982" s="7" t="s">
-        <v>779</v>
+        <v>667</v>
       </c>
       <c r="E982" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F982" s="7" t="s">
-        <v>918</v>
-      </c>
-      <c r="G982" s="7" t="s">
-        <v>916</v>
+        <v>917</v>
+      </c>
+      <c r="G982" s="7">
+        <v>6</v>
       </c>
       <c r="H982" s="7" t="s">
-        <v>1698</v>
-      </c>
-      <c r="I982" s="7"/>
-      <c r="J982" s="7"/>
-      <c r="K982" s="23"/>
-      <c r="L982" s="7"/>
+        <v>1299</v>
+      </c>
+      <c r="I982" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J982" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="K982" s="23" t="s">
+        <v>1141</v>
+      </c>
+      <c r="L982" s="7" t="s">
+        <v>1299</v>
+      </c>
       <c r="M982" s="10" t="s">
         <v>1652</v>
       </c>
@@ -48865,32 +48876,24 @@
         <v>826</v>
       </c>
       <c r="D983" s="7" t="s">
-        <v>667</v>
+        <v>261</v>
       </c>
       <c r="E983" s="7">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F983" s="7" t="s">
         <v>917</v>
       </c>
       <c r="G983" s="7">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="H983" s="7" t="s">
-        <v>1299</v>
-      </c>
-      <c r="I983" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="J983" s="7" t="s">
-        <v>266</v>
-      </c>
-      <c r="K983" s="23" t="s">
-        <v>1141</v>
-      </c>
-      <c r="L983" s="7" t="s">
-        <v>1299</v>
-      </c>
+        <v>1454</v>
+      </c>
+      <c r="I983" s="7"/>
+      <c r="J983" s="7"/>
+      <c r="K983" s="23"/>
+      <c r="L983" s="7"/>
       <c r="M983" s="10" t="s">
         <v>1652</v>
       </c>
@@ -48906,21 +48909,23 @@
         <v>826</v>
       </c>
       <c r="D984" s="7" t="s">
-        <v>261</v>
+        <v>438</v>
       </c>
       <c r="E984" s="7">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F984" s="7" t="s">
         <v>917</v>
       </c>
       <c r="G984" s="7">
-        <v>26</v>
+        <v>80</v>
       </c>
       <c r="H984" s="7" t="s">
-        <v>1454</v>
-      </c>
-      <c r="I984" s="7"/>
+        <v>1380</v>
+      </c>
+      <c r="I984" s="7" t="s">
+        <v>1128</v>
+      </c>
       <c r="J984" s="7"/>
       <c r="K984" s="23"/>
       <c r="L984" s="7"/>
@@ -48939,23 +48944,21 @@
         <v>826</v>
       </c>
       <c r="D985" s="7" t="s">
-        <v>438</v>
+        <v>394</v>
       </c>
       <c r="E985" s="7">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F985" s="7" t="s">
-        <v>917</v>
-      </c>
-      <c r="G985" s="7">
-        <v>80</v>
+        <v>919</v>
+      </c>
+      <c r="G985" s="7" t="s">
+        <v>916</v>
       </c>
       <c r="H985" s="7" t="s">
-        <v>1380</v>
-      </c>
-      <c r="I985" s="7" t="s">
-        <v>1128</v>
-      </c>
+        <v>394</v>
+      </c>
+      <c r="I985" s="7"/>
       <c r="J985" s="7"/>
       <c r="K985" s="23"/>
       <c r="L985" s="7"/>
@@ -48974,19 +48977,19 @@
         <v>826</v>
       </c>
       <c r="D986" s="7" t="s">
-        <v>394</v>
+        <v>693</v>
       </c>
       <c r="E986" s="7">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F986" s="7" t="s">
-        <v>919</v>
-      </c>
-      <c r="G986" s="7" t="s">
-        <v>916</v>
+        <v>917</v>
+      </c>
+      <c r="G986" s="7">
+        <v>32</v>
       </c>
       <c r="H986" s="7" t="s">
-        <v>394</v>
+        <v>1290</v>
       </c>
       <c r="I986" s="7"/>
       <c r="J986" s="7"/>
@@ -49007,19 +49010,19 @@
         <v>826</v>
       </c>
       <c r="D987" s="7" t="s">
-        <v>693</v>
+        <v>433</v>
       </c>
       <c r="E987" s="7">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F987" s="7" t="s">
         <v>917</v>
       </c>
       <c r="G987" s="7">
-        <v>32</v>
+        <v>80</v>
       </c>
       <c r="H987" s="7" t="s">
-        <v>1290</v>
+        <v>1391</v>
       </c>
       <c r="I987" s="7"/>
       <c r="J987" s="7"/>
@@ -49040,19 +49043,19 @@
         <v>826</v>
       </c>
       <c r="D988" s="7" t="s">
-        <v>433</v>
+        <v>382</v>
       </c>
       <c r="E988" s="7">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F988" s="7" t="s">
-        <v>917</v>
-      </c>
-      <c r="G988" s="7">
-        <v>80</v>
+        <v>919</v>
+      </c>
+      <c r="G988" s="7" t="s">
+        <v>916</v>
       </c>
       <c r="H988" s="7" t="s">
-        <v>1391</v>
+        <v>382</v>
       </c>
       <c r="I988" s="7"/>
       <c r="J988" s="7"/>
@@ -49073,24 +49076,32 @@
         <v>826</v>
       </c>
       <c r="D989" s="7" t="s">
-        <v>382</v>
+        <v>256</v>
       </c>
       <c r="E989" s="7">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F989" s="7" t="s">
-        <v>919</v>
+        <v>915</v>
       </c>
       <c r="G989" s="7" t="s">
         <v>916</v>
       </c>
       <c r="H989" s="7" t="s">
-        <v>382</v>
-      </c>
-      <c r="I989" s="7"/>
-      <c r="J989" s="7"/>
-      <c r="K989" s="23"/>
-      <c r="L989" s="7"/>
+        <v>1445</v>
+      </c>
+      <c r="I989" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="J989" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="K989" s="23" t="s">
+        <v>1142</v>
+      </c>
+      <c r="L989" s="7" t="s">
+        <v>1445</v>
+      </c>
       <c r="M989" s="10" t="s">
         <v>1652</v>
       </c>
@@ -49106,32 +49117,24 @@
         <v>826</v>
       </c>
       <c r="D990" s="7" t="s">
-        <v>256</v>
+        <v>329</v>
       </c>
       <c r="E990" s="7">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F990" s="7" t="s">
-        <v>915</v>
+        <v>919</v>
       </c>
       <c r="G990" s="7" t="s">
         <v>916</v>
       </c>
       <c r="H990" s="7" t="s">
-        <v>1445</v>
-      </c>
-      <c r="I990" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="J990" s="7" t="s">
-        <v>256</v>
-      </c>
-      <c r="K990" s="23" t="s">
-        <v>1142</v>
-      </c>
-      <c r="L990" s="7" t="s">
-        <v>1445</v>
-      </c>
+        <v>1414</v>
+      </c>
+      <c r="I990" s="7"/>
+      <c r="J990" s="7"/>
+      <c r="K990" s="23"/>
+      <c r="L990" s="7"/>
       <c r="M990" s="10" t="s">
         <v>1652</v>
       </c>
@@ -49147,19 +49150,19 @@
         <v>826</v>
       </c>
       <c r="D991" s="7" t="s">
-        <v>329</v>
+        <v>694</v>
       </c>
       <c r="E991" s="7">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F991" s="7" t="s">
-        <v>919</v>
-      </c>
-      <c r="G991" s="7" t="s">
-        <v>916</v>
+        <v>917</v>
+      </c>
+      <c r="G991" s="7">
+        <v>32</v>
       </c>
       <c r="H991" s="7" t="s">
-        <v>1414</v>
+        <v>1289</v>
       </c>
       <c r="I991" s="7"/>
       <c r="J991" s="7"/>
@@ -49180,19 +49183,19 @@
         <v>826</v>
       </c>
       <c r="D992" s="7" t="s">
-        <v>694</v>
+        <v>398</v>
       </c>
       <c r="E992" s="7">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F992" s="7" t="s">
-        <v>917</v>
-      </c>
-      <c r="G992" s="7">
-        <v>32</v>
+        <v>919</v>
+      </c>
+      <c r="G992" s="7" t="s">
+        <v>916</v>
       </c>
       <c r="H992" s="7" t="s">
-        <v>1289</v>
+        <v>383</v>
       </c>
       <c r="I992" s="7"/>
       <c r="J992" s="7"/>
@@ -49202,7 +49205,7 @@
         <v>1652</v>
       </c>
     </row>
-    <row r="993" spans="1:13">
+    <row r="993" spans="1:13" s="7" customFormat="1">
       <c r="A993" s="6" t="s">
         <v>1105</v>
       </c>
@@ -49213,29 +49216,26 @@
         <v>826</v>
       </c>
       <c r="D993" s="7" t="s">
-        <v>398</v>
+        <v>542</v>
       </c>
       <c r="E993" s="7">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F993" s="7" t="s">
-        <v>919</v>
-      </c>
-      <c r="G993" s="7" t="s">
-        <v>916</v>
+        <v>917</v>
+      </c>
+      <c r="G993" s="7">
+        <v>300</v>
       </c>
       <c r="H993" s="7" t="s">
-        <v>383</v>
-      </c>
-      <c r="I993" s="7"/>
-      <c r="J993" s="7"/>
+        <v>1367</v>
+      </c>
       <c r="K993" s="23"/>
-      <c r="L993" s="7"/>
       <c r="M993" s="10" t="s">
         <v>1652</v>
       </c>
     </row>
-    <row r="994" spans="1:13" s="7" customFormat="1">
+    <row r="994" spans="1:13">
       <c r="A994" s="6" t="s">
         <v>1105</v>
       </c>
@@ -49246,21 +49246,32 @@
         <v>826</v>
       </c>
       <c r="D994" s="7" t="s">
-        <v>542</v>
+        <v>202</v>
       </c>
       <c r="E994" s="7">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F994" s="7" t="s">
         <v>917</v>
       </c>
       <c r="G994" s="7">
-        <v>300</v>
+        <v>12</v>
       </c>
       <c r="H994" s="7" t="s">
-        <v>1367</v>
-      </c>
-      <c r="K994" s="23"/>
+        <v>1475</v>
+      </c>
+      <c r="I994" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="J994" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="K994" s="23" t="s">
+        <v>860</v>
+      </c>
+      <c r="L994" s="7" t="s">
+        <v>1475</v>
+      </c>
       <c r="M994" s="10" t="s">
         <v>1652</v>
       </c>
@@ -49276,31 +49287,31 @@
         <v>826</v>
       </c>
       <c r="D995" s="7" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
       <c r="E995" s="7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F995" s="7" t="s">
-        <v>917</v>
-      </c>
-      <c r="G995" s="7">
-        <v>12</v>
+        <v>915</v>
+      </c>
+      <c r="G995" s="7" t="s">
+        <v>916</v>
       </c>
       <c r="H995" s="7" t="s">
-        <v>1475</v>
+        <v>1447</v>
       </c>
       <c r="I995" s="7" t="s">
-        <v>78</v>
+        <v>106</v>
       </c>
       <c r="J995" s="7" t="s">
-        <v>202</v>
+        <v>262</v>
       </c>
       <c r="K995" s="23" t="s">
-        <v>860</v>
+        <v>1140</v>
       </c>
       <c r="L995" s="7" t="s">
-        <v>1475</v>
+        <v>1447</v>
       </c>
       <c r="M995" s="10" t="s">
         <v>1652</v>
@@ -49317,32 +49328,24 @@
         <v>826</v>
       </c>
       <c r="D996" s="7" t="s">
-        <v>262</v>
+        <v>738</v>
       </c>
       <c r="E996" s="7">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F996" s="7" t="s">
-        <v>915</v>
+        <v>918</v>
       </c>
       <c r="G996" s="7" t="s">
         <v>916</v>
       </c>
       <c r="H996" s="7" t="s">
-        <v>1447</v>
-      </c>
-      <c r="I996" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="J996" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="K996" s="23" t="s">
-        <v>1140</v>
-      </c>
-      <c r="L996" s="7" t="s">
-        <v>1447</v>
-      </c>
+        <v>1256</v>
+      </c>
+      <c r="I996" s="7"/>
+      <c r="J996" s="7"/>
+      <c r="K996" s="23"/>
+      <c r="L996" s="7"/>
       <c r="M996" s="10" t="s">
         <v>1652</v>
       </c>
@@ -49358,10 +49361,10 @@
         <v>826</v>
       </c>
       <c r="D997" s="7" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E997" s="7">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F997" s="7" t="s">
         <v>918</v>
@@ -49370,7 +49373,7 @@
         <v>916</v>
       </c>
       <c r="H997" s="7" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="I997" s="7"/>
       <c r="J997" s="7"/>
@@ -49391,10 +49394,10 @@
         <v>826</v>
       </c>
       <c r="D998" s="7" t="s">
-        <v>737</v>
+        <v>781</v>
       </c>
       <c r="E998" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F998" s="7" t="s">
         <v>918</v>
@@ -49403,7 +49406,7 @@
         <v>916</v>
       </c>
       <c r="H998" s="7" t="s">
-        <v>1257</v>
+        <v>1219</v>
       </c>
       <c r="I998" s="7"/>
       <c r="J998" s="7"/>
@@ -49424,19 +49427,19 @@
         <v>826</v>
       </c>
       <c r="D999" s="7" t="s">
-        <v>781</v>
+        <v>429</v>
       </c>
       <c r="E999" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F999" s="7" t="s">
-        <v>918</v>
+        <v>937</v>
       </c>
       <c r="G999" s="7" t="s">
         <v>916</v>
       </c>
       <c r="H999" s="7" t="s">
-        <v>1219</v>
+        <v>1392</v>
       </c>
       <c r="I999" s="7"/>
       <c r="J999" s="7"/>
@@ -49457,24 +49460,32 @@
         <v>826</v>
       </c>
       <c r="D1000" s="7" t="s">
-        <v>429</v>
+        <v>686</v>
       </c>
       <c r="E1000" s="7">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F1000" s="7" t="s">
-        <v>937</v>
-      </c>
-      <c r="G1000" s="7" t="s">
-        <v>916</v>
+        <v>917</v>
+      </c>
+      <c r="G1000" s="7">
+        <v>20</v>
       </c>
       <c r="H1000" s="7" t="s">
-        <v>1392</v>
-      </c>
-      <c r="I1000" s="7"/>
-      <c r="J1000" s="7"/>
-      <c r="K1000" s="23"/>
-      <c r="L1000" s="7"/>
+        <v>1699</v>
+      </c>
+      <c r="I1000" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1000" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="K1000" s="23" t="s">
+        <v>837</v>
+      </c>
+      <c r="L1000" s="7" t="s">
+        <v>1174</v>
+      </c>
       <c r="M1000" s="10" t="s">
         <v>1652</v>
       </c>
@@ -49490,10 +49501,10 @@
         <v>826</v>
       </c>
       <c r="D1001" s="7" t="s">
-        <v>686</v>
+        <v>1129</v>
       </c>
       <c r="E1001" s="7">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F1001" s="7" t="s">
         <v>917</v>
@@ -49502,19 +49513,19 @@
         <v>20</v>
       </c>
       <c r="H1001" s="7" t="s">
-        <v>1699</v>
+        <v>1440</v>
       </c>
       <c r="I1001" s="7" t="s">
-        <v>73</v>
+        <v>122</v>
       </c>
       <c r="J1001" s="7" t="s">
-        <v>212</v>
+        <v>1129</v>
       </c>
       <c r="K1001" s="23" t="s">
-        <v>837</v>
+        <v>907</v>
       </c>
       <c r="L1001" s="7" t="s">
-        <v>1174</v>
+        <v>1646</v>
       </c>
       <c r="M1001" s="10" t="s">
         <v>1652</v>
@@ -49531,32 +49542,24 @@
         <v>826</v>
       </c>
       <c r="D1002" s="7" t="s">
-        <v>1129</v>
+        <v>796</v>
       </c>
       <c r="E1002" s="7">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F1002" s="7" t="s">
-        <v>917</v>
-      </c>
-      <c r="G1002" s="7">
-        <v>20</v>
+        <v>918</v>
+      </c>
+      <c r="G1002" s="7" t="s">
+        <v>916</v>
       </c>
       <c r="H1002" s="7" t="s">
-        <v>1440</v>
-      </c>
-      <c r="I1002" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="J1002" s="7" t="s">
-        <v>1129</v>
-      </c>
-      <c r="K1002" s="23" t="s">
-        <v>907</v>
-      </c>
-      <c r="L1002" s="7" t="s">
-        <v>1646</v>
-      </c>
+        <v>1209</v>
+      </c>
+      <c r="I1002" s="7"/>
+      <c r="J1002" s="7"/>
+      <c r="K1002" s="23"/>
+      <c r="L1002" s="7"/>
       <c r="M1002" s="10" t="s">
         <v>1652</v>
       </c>
@@ -49572,24 +49575,32 @@
         <v>826</v>
       </c>
       <c r="D1003" s="7" t="s">
-        <v>796</v>
+        <v>268</v>
       </c>
       <c r="E1003" s="7">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F1003" s="7" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
       <c r="G1003" s="7" t="s">
         <v>916</v>
       </c>
       <c r="H1003" s="7" t="s">
-        <v>1209</v>
-      </c>
-      <c r="I1003" s="7"/>
-      <c r="J1003" s="7"/>
-      <c r="K1003" s="23"/>
-      <c r="L1003" s="7"/>
+        <v>1298</v>
+      </c>
+      <c r="I1003" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="J1003" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="K1003" s="23" t="s">
+        <v>1146</v>
+      </c>
+      <c r="L1003" s="7" t="s">
+        <v>1298</v>
+      </c>
       <c r="M1003" s="10" t="s">
         <v>1652</v>
       </c>
@@ -49605,31 +49616,31 @@
         <v>826</v>
       </c>
       <c r="D1004" s="7" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="E1004" s="7">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F1004" s="7" t="s">
-        <v>915</v>
-      </c>
-      <c r="G1004" s="7" t="s">
-        <v>916</v>
+        <v>917</v>
+      </c>
+      <c r="G1004" s="7">
+        <v>20</v>
       </c>
       <c r="H1004" s="7" t="s">
-        <v>1298</v>
+        <v>1442</v>
       </c>
       <c r="I1004" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J1004" s="7" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="K1004" s="23" t="s">
-        <v>1146</v>
+        <v>905</v>
       </c>
       <c r="L1004" s="7" t="s">
-        <v>1298</v>
+        <v>1442</v>
       </c>
       <c r="M1004" s="10" t="s">
         <v>1652</v>
@@ -49646,32 +49657,24 @@
         <v>826</v>
       </c>
       <c r="D1005" s="7" t="s">
-        <v>264</v>
+        <v>790</v>
       </c>
       <c r="E1005" s="7">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F1005" s="7" t="s">
-        <v>917</v>
-      </c>
-      <c r="G1005" s="7">
-        <v>20</v>
+        <v>918</v>
+      </c>
+      <c r="G1005" s="7" t="s">
+        <v>916</v>
       </c>
       <c r="H1005" s="7" t="s">
-        <v>1442</v>
-      </c>
-      <c r="I1005" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="J1005" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="K1005" s="23" t="s">
-        <v>905</v>
-      </c>
-      <c r="L1005" s="7" t="s">
-        <v>1442</v>
-      </c>
+        <v>1213</v>
+      </c>
+      <c r="I1005" s="7"/>
+      <c r="J1005" s="7"/>
+      <c r="K1005" s="23"/>
+      <c r="L1005" s="7"/>
       <c r="M1005" s="10" t="s">
         <v>1652</v>
       </c>
@@ -49687,19 +49690,19 @@
         <v>826</v>
       </c>
       <c r="D1006" s="7" t="s">
-        <v>790</v>
+        <v>2410</v>
       </c>
       <c r="E1006" s="7">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F1006" s="7" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="G1006" s="7" t="s">
         <v>916</v>
       </c>
       <c r="H1006" s="7" t="s">
-        <v>1213</v>
+        <v>2410</v>
       </c>
       <c r="I1006" s="7"/>
       <c r="J1006" s="7"/>

</xml_diff>

<commit_message>
Atualização Documentação Mapeamento Stage LN
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Mapeamento Stage LN.xlsx
+++ b/Documentação/Planilhas/Mapeamento Stage LN.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14664" uniqueCount="2411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14664" uniqueCount="2412">
   <si>
     <t>dbo.Balancete</t>
   </si>
@@ -7263,6 +7263,9 @@
   </si>
   <si>
     <t>DT_CRIACAO</t>
+  </si>
+  <si>
+    <t>DT_ULTIMA_ATUALIZ_NF</t>
   </si>
 </sst>
 </file>
@@ -8418,6 +8421,15 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -8427,20 +8439,11 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -12975,7 +12978,7 @@
       <c r="A88" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B88" s="176" t="s">
+      <c r="B88" s="175" t="s">
         <v>914</v>
       </c>
       <c r="C88" s="36" t="s">
@@ -13011,7 +13014,7 @@
       <c r="A89" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B89" s="176"/>
+      <c r="B89" s="175"/>
       <c r="C89" s="36" t="s">
         <v>2011</v>
       </c>
@@ -13061,7 +13064,7 @@
       <c r="A91" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B91" s="176" t="s">
+      <c r="B91" s="175" t="s">
         <v>2014</v>
       </c>
       <c r="C91" s="36" t="s">
@@ -13097,7 +13100,7 @@
       <c r="A92" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B92" s="176"/>
+      <c r="B92" s="175"/>
       <c r="C92" s="36" t="s">
         <v>2018</v>
       </c>
@@ -13131,7 +13134,7 @@
       <c r="A93" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B93" s="176"/>
+      <c r="B93" s="175"/>
       <c r="C93" s="36"/>
       <c r="D93" s="37" t="s">
         <v>1783</v>
@@ -13165,7 +13168,7 @@
       <c r="A94" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B94" s="176"/>
+      <c r="B94" s="175"/>
       <c r="C94" s="36"/>
       <c r="D94" s="37" t="s">
         <v>1783</v>
@@ -13199,7 +13202,7 @@
       <c r="A95" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B95" s="176"/>
+      <c r="B95" s="175"/>
       <c r="C95" s="36"/>
       <c r="D95" s="37" t="s">
         <v>1783</v>
@@ -13233,7 +13236,7 @@
       <c r="A96" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B96" s="176"/>
+      <c r="B96" s="175"/>
       <c r="C96" s="36" t="s">
         <v>2020</v>
       </c>
@@ -13267,7 +13270,7 @@
       <c r="A97" s="34" t="s">
         <v>1652</v>
       </c>
-      <c r="B97" s="176"/>
+      <c r="B97" s="175"/>
       <c r="C97" s="64" t="s">
         <v>2022</v>
       </c>
@@ -13289,7 +13292,7 @@
       <c r="A98" s="34" t="s">
         <v>1652</v>
       </c>
-      <c r="B98" s="176"/>
+      <c r="B98" s="175"/>
       <c r="C98" s="64" t="s">
         <v>2023</v>
       </c>
@@ -13311,7 +13314,7 @@
       <c r="A99" s="34" t="s">
         <v>1652</v>
       </c>
-      <c r="B99" s="176"/>
+      <c r="B99" s="175"/>
       <c r="C99" s="64" t="s">
         <v>2024</v>
       </c>
@@ -13589,7 +13592,7 @@
       <c r="A109" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B109" s="176" t="s">
+      <c r="B109" s="175" t="s">
         <v>948</v>
       </c>
       <c r="C109" s="36" t="s">
@@ -13625,7 +13628,7 @@
       <c r="A110" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B110" s="176"/>
+      <c r="B110" s="175"/>
       <c r="C110" s="36" t="s">
         <v>2048</v>
       </c>
@@ -13659,7 +13662,7 @@
       <c r="A111" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B111" s="176"/>
+      <c r="B111" s="175"/>
       <c r="C111" s="36" t="s">
         <v>2050</v>
       </c>
@@ -13709,7 +13712,7 @@
       <c r="A113" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B113" s="176" t="s">
+      <c r="B113" s="175" t="s">
         <v>954</v>
       </c>
       <c r="C113" s="36" t="s">
@@ -13745,7 +13748,7 @@
       <c r="A114" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B114" s="176"/>
+      <c r="B114" s="175"/>
       <c r="C114" s="36" t="s">
         <v>2057</v>
       </c>
@@ -13847,7 +13850,7 @@
       <c r="A118" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B118" s="176" t="s">
+      <c r="B118" s="175" t="s">
         <v>2064</v>
       </c>
       <c r="C118" s="36" t="s">
@@ -13883,7 +13886,7 @@
       <c r="A119" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B119" s="176"/>
+      <c r="B119" s="175"/>
       <c r="C119" s="36" t="s">
         <v>2069</v>
       </c>
@@ -13917,7 +13920,7 @@
       <c r="A120" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B120" s="176"/>
+      <c r="B120" s="175"/>
       <c r="C120" s="36" t="s">
         <v>2072</v>
       </c>
@@ -13951,7 +13954,7 @@
       <c r="A121" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B121" s="176"/>
+      <c r="B121" s="175"/>
       <c r="C121" s="36" t="s">
         <v>2075</v>
       </c>
@@ -14001,7 +14004,7 @@
       <c r="A123" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B123" s="176" t="s">
+      <c r="B123" s="175" t="s">
         <v>2078</v>
       </c>
       <c r="C123" s="36" t="s">
@@ -14037,7 +14040,7 @@
       <c r="A124" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B124" s="176"/>
+      <c r="B124" s="175"/>
       <c r="C124" s="36" t="s">
         <v>2083</v>
       </c>
@@ -14071,7 +14074,7 @@
       <c r="A125" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B125" s="176"/>
+      <c r="B125" s="175"/>
       <c r="C125" s="36" t="s">
         <v>2086</v>
       </c>
@@ -14173,7 +14176,7 @@
       <c r="A129" s="34" t="s">
         <v>1652</v>
       </c>
-      <c r="B129" s="175" t="s">
+      <c r="B129" s="178" t="s">
         <v>2094</v>
       </c>
       <c r="C129" s="52" t="s">
@@ -14203,7 +14206,7 @@
       <c r="A130" s="34" t="s">
         <v>1652</v>
       </c>
-      <c r="B130" s="175"/>
+      <c r="B130" s="178"/>
       <c r="C130" s="52" t="s">
         <v>2097</v>
       </c>
@@ -14247,7 +14250,7 @@
       <c r="A132" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B132" s="176" t="s">
+      <c r="B132" s="175" t="s">
         <v>2098</v>
       </c>
       <c r="C132" s="36" t="s">
@@ -14283,7 +14286,7 @@
       <c r="A133" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B133" s="176"/>
+      <c r="B133" s="175"/>
       <c r="C133" s="36" t="s">
         <v>2103</v>
       </c>
@@ -14333,7 +14336,7 @@
       <c r="A135" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B135" s="176" t="s">
+      <c r="B135" s="175" t="s">
         <v>2106</v>
       </c>
       <c r="C135" s="36" t="s">
@@ -14369,7 +14372,7 @@
       <c r="A136" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B136" s="176"/>
+      <c r="B136" s="175"/>
       <c r="C136" s="36" t="s">
         <v>2111</v>
       </c>
@@ -14403,7 +14406,7 @@
       <c r="A137" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B137" s="176"/>
+      <c r="B137" s="175"/>
       <c r="C137" s="36" t="s">
         <v>2114</v>
       </c>
@@ -14437,7 +14440,7 @@
       <c r="A138" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B138" s="176"/>
+      <c r="B138" s="175"/>
       <c r="C138" s="36" t="s">
         <v>2117</v>
       </c>
@@ -14691,7 +14694,7 @@
       <c r="A147" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B147" s="176" t="s">
+      <c r="B147" s="175" t="s">
         <v>2137</v>
       </c>
       <c r="C147" s="36" t="s">
@@ -14727,7 +14730,7 @@
       <c r="A148" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B148" s="176"/>
+      <c r="B148" s="175"/>
       <c r="C148" s="36" t="s">
         <v>2142</v>
       </c>
@@ -14777,7 +14780,7 @@
       <c r="A150" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B150" s="173" t="s">
+      <c r="B150" s="176" t="s">
         <v>2342</v>
       </c>
       <c r="C150" s="132" t="s">
@@ -14813,7 +14816,7 @@
       <c r="A151" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B151" s="174"/>
+      <c r="B151" s="177"/>
       <c r="C151" s="132" t="s">
         <v>2145</v>
       </c>
@@ -14847,7 +14850,7 @@
       <c r="A152" s="34" t="s">
         <v>1653</v>
       </c>
-      <c r="B152" s="174"/>
+      <c r="B152" s="177"/>
       <c r="C152" s="58" t="s">
         <v>2147</v>
       </c>
@@ -14881,7 +14884,7 @@
       <c r="A153" s="34" t="s">
         <v>1652</v>
       </c>
-      <c r="B153" s="174"/>
+      <c r="B153" s="177"/>
       <c r="C153" s="58"/>
       <c r="D153" s="45" t="s">
         <v>1783</v>
@@ -14913,7 +14916,7 @@
       <c r="A154" s="34" t="s">
         <v>1985</v>
       </c>
-      <c r="B154" s="174"/>
+      <c r="B154" s="177"/>
       <c r="C154" s="58" t="s">
         <v>2149</v>
       </c>
@@ -14945,7 +14948,7 @@
       <c r="A155" s="34" t="s">
         <v>1985</v>
       </c>
-      <c r="B155" s="174"/>
+      <c r="B155" s="177"/>
       <c r="C155" s="58" t="s">
         <v>2150</v>
       </c>
@@ -14988,17 +14991,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B150:B155"/>
+    <mergeCell ref="B129:B130"/>
+    <mergeCell ref="B132:B133"/>
+    <mergeCell ref="B135:B138"/>
+    <mergeCell ref="B147:B148"/>
     <mergeCell ref="B123:B125"/>
     <mergeCell ref="B88:B89"/>
     <mergeCell ref="B91:B99"/>
     <mergeCell ref="B109:B111"/>
     <mergeCell ref="B113:B114"/>
     <mergeCell ref="B118:B121"/>
-    <mergeCell ref="B150:B155"/>
-    <mergeCell ref="B129:B130"/>
-    <mergeCell ref="B132:B133"/>
-    <mergeCell ref="B135:B138"/>
-    <mergeCell ref="B147:B148"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -15010,8 +15013,8 @@
   <dimension ref="A1:M1440"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A256" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G273" sqref="G273"/>
+      <pane ySplit="1" topLeftCell="A460" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H485" sqref="H485"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -23860,16 +23863,16 @@
       <c r="C272" s="171" t="s">
         <v>2398</v>
       </c>
-      <c r="D272" s="179" t="s">
+      <c r="D272" s="173" t="s">
         <v>1205</v>
       </c>
-      <c r="E272" s="179">
+      <c r="E272" s="173">
         <v>11</v>
       </c>
-      <c r="F272" s="179" t="s">
-        <v>917</v>
-      </c>
-      <c r="G272" s="179">
+      <c r="F272" s="173" t="s">
+        <v>917</v>
+      </c>
+      <c r="G272" s="173">
         <v>18</v>
       </c>
       <c r="H272" s="7" t="s">
@@ -23887,7 +23890,7 @@
       <c r="L272" s="7" t="s">
         <v>1205</v>
       </c>
-      <c r="M272" s="180"/>
+      <c r="M272" s="174"/>
     </row>
     <row r="273" spans="1:13" ht="15.75" customHeight="1">
       <c r="A273" s="6" t="s">
@@ -31029,7 +31032,7 @@
         <v>916</v>
       </c>
       <c r="H472" s="7" t="s">
-        <v>683</v>
+        <v>2411</v>
       </c>
       <c r="I472" s="7"/>
       <c r="J472" s="7"/>
@@ -64737,19 +64740,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="178" t="s">
+      <c r="A1" s="180" t="s">
         <v>1064</v>
       </c>
-      <c r="B1" s="178"/>
-      <c r="C1" s="178"/>
-      <c r="D1" s="178"/>
-      <c r="E1" s="178"/>
-      <c r="F1" s="178"/>
-      <c r="H1" s="178" t="s">
+      <c r="B1" s="180"/>
+      <c r="C1" s="180"/>
+      <c r="D1" s="180"/>
+      <c r="E1" s="180"/>
+      <c r="F1" s="180"/>
+      <c r="H1" s="180" t="s">
         <v>1103</v>
       </c>
-      <c r="I1" s="178"/>
-      <c r="J1" s="178"/>
+      <c r="I1" s="180"/>
+      <c r="J1" s="180"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
@@ -64934,11 +64937,11 @@
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="177"/>
-      <c r="B12" s="177"/>
-      <c r="C12" s="177"/>
-      <c r="D12" s="177"/>
-      <c r="E12" s="177"/>
+      <c r="A12" s="179"/>
+      <c r="B12" s="179"/>
+      <c r="C12" s="179"/>
+      <c r="D12" s="179"/>
+      <c r="E12" s="179"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Atualização de Views e Documentações
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Mapeamento Stage LN.xlsx
+++ b/Documentação/Planilhas/Mapeamento Stage LN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="17235" windowHeight="6210" tabRatio="539" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="17235" windowHeight="6210" tabRatio="539" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DE-PARA Tabelas" sheetId="1" state="hidden" r:id="rId1"/>
@@ -13,7 +13,8 @@
     <sheet name="Dicionario" sheetId="3" r:id="rId4"/>
     <sheet name="Processo de Carga" sheetId="6" r:id="rId5"/>
     <sheet name="Cubos" sheetId="7" r:id="rId6"/>
-    <sheet name="Plan1" sheetId="8" r:id="rId7"/>
+    <sheet name="Controle criação Views e CIA 1" sheetId="9" r:id="rId7"/>
+    <sheet name="Plan1" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'DE - PARA Atributos'!$A$1:$M$1554</definedName>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18417" uniqueCount="3081">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18597" uniqueCount="3125">
   <si>
     <t>dbo.Balancete</t>
   </si>
@@ -9276,6 +9277,138 @@
   </si>
   <si>
     <t>dim.dim_produto</t>
+  </si>
+  <si>
+    <t>JUVENTUS</t>
+  </si>
+  <si>
+    <t>CRICIUMA</t>
+  </si>
+  <si>
+    <t>VW_NFR_Cab</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>GitHub</t>
+  </si>
+  <si>
+    <t>VW_NFR_Det</t>
+  </si>
+  <si>
+    <t>VW_NFR_Rascunho_Cab</t>
+  </si>
+  <si>
+    <t>VW_NFR_Rascunho_Det</t>
+  </si>
+  <si>
+    <t>não tem CIA</t>
+  </si>
+  <si>
+    <t>VW_NFR_Ultimo_Recebimento</t>
+  </si>
+  <si>
+    <t>VW_CAP_Conciliacao_CAP_CAR</t>
+  </si>
+  <si>
+    <t>VW_CAP_Titulo</t>
+  </si>
+  <si>
+    <t>VW_CAP_Titulo_Lancamento</t>
+  </si>
+  <si>
+    <t>VW_CAP_Titulo_Mvmt</t>
+  </si>
+  <si>
+    <t>VW_CAP_Titulo_Pgto</t>
+  </si>
+  <si>
+    <t>VW_CAP_Titulo_Referencia</t>
+  </si>
+  <si>
+    <t>VW_CAP_Titulo_Reversao</t>
+  </si>
+  <si>
+    <t>VW_CAR_Pedido_Venda</t>
+  </si>
+  <si>
+    <t>VW_CAR_Remessa</t>
+  </si>
+  <si>
+    <t>VW_CAR_Remessa_Cobr_Eletr</t>
+  </si>
+  <si>
+    <t>VW_CAR_Remessa_Cobranca_Eletronica</t>
+  </si>
+  <si>
+    <t>ARQUIVO SQL</t>
+  </si>
+  <si>
+    <t>VW_CAR_Retorno_Cobr_Eletr</t>
+  </si>
+  <si>
+    <t>VW_CAR_Retorno_Cobranca_Eletronica</t>
+  </si>
+  <si>
+    <t>VW_CAR_Titulo</t>
+  </si>
+  <si>
+    <t>VW_CAR_Titulo_Mvmt</t>
+  </si>
+  <si>
+    <t>VW_CAR_Titulo_Parcelamento</t>
+  </si>
+  <si>
+    <t>VW_CAR_Titulo_Remessa</t>
+  </si>
+  <si>
+    <t>VW_CAR_VPC</t>
+  </si>
+  <si>
+    <t>VW_EST_Estoque</t>
+  </si>
+  <si>
+    <t>VW_DOM_Condicao_Pagamento</t>
+  </si>
+  <si>
+    <t>VW_DOM_Filial</t>
+  </si>
+  <si>
+    <t>não tem view</t>
+  </si>
+  <si>
+    <t>VW_EST_Crossdocking</t>
+  </si>
+  <si>
+    <t>VW_EST_Referencia</t>
+  </si>
+  <si>
+    <t>VW_EST_Fechamento_Estoque</t>
+  </si>
+  <si>
+    <t>VW_NFV_Cab</t>
+  </si>
+  <si>
+    <t>VW_NFV_Det</t>
+  </si>
+  <si>
+    <t>VW_NFV_Eletronica</t>
+  </si>
+  <si>
+    <t>VW_PEC_Cab</t>
+  </si>
+  <si>
+    <t>VW_PEC_Det</t>
+  </si>
+  <si>
+    <t>VW_SKU_CMV</t>
+  </si>
+  <si>
+    <t>VW_SKU_Condicao_Pagamento</t>
+  </si>
+  <si>
+    <t>VW_SKU</t>
   </si>
 </sst>
 </file>
@@ -9882,7 +10015,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="156">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -10283,6 +10416,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -10328,12 +10465,26 @@
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="32">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
@@ -10830,28 +10981,28 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A1:M1554" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A1:M1554" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A1:M1554">
     <filterColumn colId="2">
       <filters>
-        <filter val="stg_nfv_cab"/>
+        <filter val="stg_nfr_rascunho_cab"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <tableColumns count="13">
-    <tableColumn id="1" name="Tipo" dataDxfId="24"/>
-    <tableColumn id="2" name="DE - TABLE_NAME" dataDxfId="23"/>
-    <tableColumn id="3" name="PARA - TABLE_NAME" dataDxfId="22"/>
-    <tableColumn id="4" name="DE - COLUMN_NAME " dataDxfId="21"/>
-    <tableColumn id="5" name="ORDINAL_POSITION" dataDxfId="20"/>
-    <tableColumn id="6" name="DATA_TYPE" dataDxfId="19"/>
-    <tableColumn id="7" name="CHARACTER_OCTET_LENGTH" dataDxfId="18"/>
-    <tableColumn id="8" name="PARA - COLUMN_NAME" dataDxfId="17"/>
-    <tableColumn id="9" name="DE:Tabela Dominio" dataDxfId="16"/>
-    <tableColumn id="10" name="DE:Campo Dominio" dataDxfId="15"/>
-    <tableColumn id="14" name="PARA:Tabela Dominio2" dataDxfId="14"/>
-    <tableColumn id="15" name="PARA:Campo Dominio3" dataDxfId="13"/>
-    <tableColumn id="11" name="IN_ATIVA" dataDxfId="12"/>
+    <tableColumn id="1" name="Tipo" dataDxfId="29"/>
+    <tableColumn id="2" name="DE - TABLE_NAME" dataDxfId="28"/>
+    <tableColumn id="3" name="PARA - TABLE_NAME" dataDxfId="27"/>
+    <tableColumn id="4" name="DE - COLUMN_NAME " dataDxfId="26"/>
+    <tableColumn id="5" name="ORDINAL_POSITION" dataDxfId="25"/>
+    <tableColumn id="6" name="DATA_TYPE" dataDxfId="24"/>
+    <tableColumn id="7" name="CHARACTER_OCTET_LENGTH" dataDxfId="23"/>
+    <tableColumn id="8" name="PARA - COLUMN_NAME" dataDxfId="22"/>
+    <tableColumn id="9" name="DE:Tabela Dominio" dataDxfId="21"/>
+    <tableColumn id="10" name="DE:Campo Dominio" dataDxfId="20"/>
+    <tableColumn id="14" name="PARA:Tabela Dominio2" dataDxfId="19"/>
+    <tableColumn id="15" name="PARA:Campo Dominio3" dataDxfId="18"/>
+    <tableColumn id="11" name="IN_ATIVA" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -10885,7 +11036,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="A2:I493" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="A2:I493" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A2:I493">
     <filterColumn colId="6"/>
     <filterColumn colId="7">
@@ -10895,28 +11046,42 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="9">
-    <tableColumn id="1" name="Sequence Container" dataDxfId="9"/>
-    <tableColumn id="2" name="EPT" dataDxfId="8"/>
-    <tableColumn id="3" name="Package" dataDxfId="7"/>
-    <tableColumn id="4" name="DTSX Controlador" dataDxfId="6"/>
-    <tableColumn id="5" name="Sequence Container Controlador" dataDxfId="5"/>
-    <tableColumn id="6" name="EPT Controlador" dataDxfId="4"/>
-    <tableColumn id="7" name="Tabelas Geradas" dataDxfId="3"/>
-    <tableColumn id="8" name="Database Destino" dataDxfId="2"/>
-    <tableColumn id="9" name="Observação" dataDxfId="1"/>
+    <tableColumn id="1" name="Sequence Container" dataDxfId="14"/>
+    <tableColumn id="2" name="EPT" dataDxfId="13"/>
+    <tableColumn id="3" name="Package" dataDxfId="12"/>
+    <tableColumn id="4" name="DTSX Controlador" dataDxfId="11"/>
+    <tableColumn id="5" name="Sequence Container Controlador" dataDxfId="10"/>
+    <tableColumn id="6" name="EPT Controlador" dataDxfId="9"/>
+    <tableColumn id="7" name="Tabelas Geradas" dataDxfId="8"/>
+    <tableColumn id="8" name="Database Destino" dataDxfId="7"/>
+    <tableColumn id="9" name="Observação" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela6" displayName="Tabela6" ref="A1:B46" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela6" displayName="Tabela6" ref="A1:B46" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A1:B46"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Databases"/>
     <tableColumn id="2" name="Cubes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela5" displayName="Tabela5" ref="A1:E36" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:E36"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="ARQUIVO SQL"/>
+    <tableColumn id="2" name="JUVENTUS" dataDxfId="4"/>
+    <tableColumn id="3" name="CRICIUMA" dataDxfId="3"/>
+    <tableColumn id="4" name="GitHub" dataDxfId="2"/>
+    <tableColumn id="5" name="VIEW"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -12273,7 +12438,7 @@
       <c r="A3" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B3" s="140" t="s">
+      <c r="B3" s="142" t="s">
         <v>1757</v>
       </c>
       <c r="C3" s="31" t="s">
@@ -12293,7 +12458,7 @@
       <c r="A4" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B4" s="141"/>
+      <c r="B4" s="143"/>
       <c r="C4" s="31" t="s">
         <v>1763</v>
       </c>
@@ -12312,7 +12477,7 @@
       <c r="A5" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B5" s="141"/>
+      <c r="B5" s="143"/>
       <c r="C5" s="31" t="s">
         <v>1765</v>
       </c>
@@ -12331,7 +12496,7 @@
       <c r="A6" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B6" s="141"/>
+      <c r="B6" s="143"/>
       <c r="C6" s="31" t="s">
         <v>1767</v>
       </c>
@@ -12350,7 +12515,7 @@
       <c r="A7" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B7" s="141"/>
+      <c r="B7" s="143"/>
       <c r="C7" s="31" t="s">
         <v>1769</v>
       </c>
@@ -12369,7 +12534,7 @@
       <c r="A8" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B8" s="141"/>
+      <c r="B8" s="143"/>
       <c r="C8" s="31" t="s">
         <v>2294</v>
       </c>
@@ -12388,7 +12553,7 @@
       <c r="A9" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B9" s="141"/>
+      <c r="B9" s="143"/>
       <c r="C9" s="31" t="s">
         <v>1771</v>
       </c>
@@ -12407,7 +12572,7 @@
       <c r="A10" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B10" s="141"/>
+      <c r="B10" s="143"/>
       <c r="C10" s="31" t="s">
         <v>1773</v>
       </c>
@@ -12426,7 +12591,7 @@
       <c r="A11" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B11" s="141"/>
+      <c r="B11" s="143"/>
       <c r="C11" s="31" t="s">
         <v>1775</v>
       </c>
@@ -12445,7 +12610,7 @@
       <c r="A12" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B12" s="141"/>
+      <c r="B12" s="143"/>
       <c r="C12" s="31" t="s">
         <v>1777</v>
       </c>
@@ -12464,7 +12629,7 @@
       <c r="A13" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B13" s="141"/>
+      <c r="B13" s="143"/>
       <c r="C13" s="31" t="s">
         <v>1779</v>
       </c>
@@ -12483,7 +12648,7 @@
       <c r="A14" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B14" s="141"/>
+      <c r="B14" s="143"/>
       <c r="C14" s="31" t="s">
         <v>1781</v>
       </c>
@@ -12502,7 +12667,7 @@
       <c r="A15" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B15" s="141"/>
+      <c r="B15" s="143"/>
       <c r="C15" s="31" t="s">
         <v>1783</v>
       </c>
@@ -12521,7 +12686,7 @@
       <c r="A16" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B16" s="141"/>
+      <c r="B16" s="143"/>
       <c r="C16" s="31" t="s">
         <v>1785</v>
       </c>
@@ -12540,7 +12705,7 @@
       <c r="A17" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B17" s="141"/>
+      <c r="B17" s="143"/>
       <c r="C17" s="31" t="s">
         <v>1787</v>
       </c>
@@ -12559,7 +12724,7 @@
       <c r="A18" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B18" s="141"/>
+      <c r="B18" s="143"/>
       <c r="C18" s="31" t="s">
         <v>1796</v>
       </c>
@@ -12577,7 +12742,7 @@
       <c r="A19" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B19" s="141"/>
+      <c r="B19" s="143"/>
       <c r="C19" s="31" t="s">
         <v>1800</v>
       </c>
@@ -12596,7 +12761,7 @@
       <c r="A20" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B20" s="141"/>
+      <c r="B20" s="143"/>
       <c r="C20" s="31" t="s">
         <v>1802</v>
       </c>
@@ -12615,7 +12780,7 @@
       <c r="A21" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B21" s="141"/>
+      <c r="B21" s="143"/>
       <c r="C21" s="31" t="s">
         <v>1804</v>
       </c>
@@ -12634,7 +12799,7 @@
       <c r="A22" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B22" s="141"/>
+      <c r="B22" s="143"/>
       <c r="C22" s="31" t="s">
         <v>2271</v>
       </c>
@@ -12653,7 +12818,7 @@
       <c r="A23" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B23" s="141"/>
+      <c r="B23" s="143"/>
       <c r="C23" s="31" t="s">
         <v>1807</v>
       </c>
@@ -12672,7 +12837,7 @@
       <c r="A24" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B24" s="141"/>
+      <c r="B24" s="143"/>
       <c r="C24" s="31" t="s">
         <v>1813</v>
       </c>
@@ -12691,7 +12856,7 @@
       <c r="A25" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B25" s="141"/>
+      <c r="B25" s="143"/>
       <c r="C25" s="31" t="s">
         <v>1823</v>
       </c>
@@ -12710,7 +12875,7 @@
       <c r="A26" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B26" s="141"/>
+      <c r="B26" s="143"/>
       <c r="C26" s="31" t="s">
         <v>1825</v>
       </c>
@@ -12729,7 +12894,7 @@
       <c r="A27" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B27" s="141"/>
+      <c r="B27" s="143"/>
       <c r="C27" s="31" t="s">
         <v>1827</v>
       </c>
@@ -12748,7 +12913,7 @@
       <c r="A28" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B28" s="141"/>
+      <c r="B28" s="143"/>
       <c r="C28" s="31" t="s">
         <v>1829</v>
       </c>
@@ -12767,7 +12932,7 @@
       <c r="A29" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B29" s="141"/>
+      <c r="B29" s="143"/>
       <c r="C29" s="31" t="s">
         <v>1831</v>
       </c>
@@ -12786,7 +12951,7 @@
       <c r="A30" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B30" s="141"/>
+      <c r="B30" s="143"/>
       <c r="C30" s="31" t="s">
         <v>1833</v>
       </c>
@@ -12805,7 +12970,7 @@
       <c r="A31" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B31" s="141"/>
+      <c r="B31" s="143"/>
       <c r="C31" s="31" t="s">
         <v>1835</v>
       </c>
@@ -12824,7 +12989,7 @@
       <c r="A32" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B32" s="141"/>
+      <c r="B32" s="143"/>
       <c r="C32" s="31" t="s">
         <v>1874</v>
       </c>
@@ -12843,7 +13008,7 @@
       <c r="A33" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B33" s="141"/>
+      <c r="B33" s="143"/>
       <c r="C33" s="31" t="s">
         <v>1875</v>
       </c>
@@ -12862,7 +13027,7 @@
       <c r="A34" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B34" s="141"/>
+      <c r="B34" s="143"/>
       <c r="C34" s="31" t="s">
         <v>2357</v>
       </c>
@@ -12881,7 +13046,7 @@
       <c r="A35" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B35" s="141"/>
+      <c r="B35" s="143"/>
       <c r="C35" s="31" t="s">
         <v>2340</v>
       </c>
@@ -12900,7 +13065,7 @@
       <c r="A36" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B36" s="141"/>
+      <c r="B36" s="143"/>
       <c r="C36" s="31" t="s">
         <v>1882</v>
       </c>
@@ -12919,7 +13084,7 @@
       <c r="A37" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B37" s="141"/>
+      <c r="B37" s="143"/>
       <c r="C37" s="31" t="s">
         <v>1884</v>
       </c>
@@ -12938,7 +13103,7 @@
       <c r="A38" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B38" s="141"/>
+      <c r="B38" s="143"/>
       <c r="C38" s="31" t="s">
         <v>1886</v>
       </c>
@@ -12957,7 +13122,7 @@
       <c r="A39" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B39" s="141"/>
+      <c r="B39" s="143"/>
       <c r="C39" s="31" t="s">
         <v>1888</v>
       </c>
@@ -12976,7 +13141,7 @@
       <c r="A40" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B40" s="141"/>
+      <c r="B40" s="143"/>
       <c r="C40" s="31" t="s">
         <v>1895</v>
       </c>
@@ -12995,7 +13160,7 @@
       <c r="A41" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B41" s="141"/>
+      <c r="B41" s="143"/>
       <c r="C41" s="31" t="s">
         <v>1897</v>
       </c>
@@ -13014,7 +13179,7 @@
       <c r="A42" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B42" s="142"/>
+      <c r="B42" s="144"/>
       <c r="C42" s="31" t="s">
         <v>2048</v>
       </c>
@@ -13041,7 +13206,7 @@
       <c r="G43" s="34"/>
     </row>
     <row r="44" spans="1:7" ht="15" customHeight="1">
-      <c r="B44" s="140" t="s">
+      <c r="B44" s="142" t="s">
         <v>2345</v>
       </c>
       <c r="C44" s="31" t="s">
@@ -13062,7 +13227,7 @@
       <c r="A45" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B45" s="141"/>
+      <c r="B45" s="143"/>
       <c r="C45" s="31" t="s">
         <v>1761</v>
       </c>
@@ -13081,7 +13246,7 @@
       <c r="A46" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B46" s="141"/>
+      <c r="B46" s="143"/>
       <c r="C46" s="31" t="s">
         <v>1789</v>
       </c>
@@ -13100,7 +13265,7 @@
       <c r="A47" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B47" s="141"/>
+      <c r="B47" s="143"/>
       <c r="C47" s="31" t="s">
         <v>1791</v>
       </c>
@@ -13119,7 +13284,7 @@
       <c r="A48" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B48" s="141"/>
+      <c r="B48" s="143"/>
       <c r="C48" s="31" t="s">
         <v>1792</v>
       </c>
@@ -13138,7 +13303,7 @@
       <c r="A49" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B49" s="141"/>
+      <c r="B49" s="143"/>
       <c r="C49" s="31" t="s">
         <v>2019</v>
       </c>
@@ -13157,7 +13322,7 @@
       <c r="A50" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B50" s="141"/>
+      <c r="B50" s="143"/>
       <c r="C50" s="31" t="s">
         <v>1794</v>
       </c>
@@ -13176,7 +13341,7 @@
       <c r="A51" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B51" s="141"/>
+      <c r="B51" s="143"/>
       <c r="C51" s="31" t="s">
         <v>1799</v>
       </c>
@@ -13195,7 +13360,7 @@
       <c r="A52" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B52" s="141"/>
+      <c r="B52" s="143"/>
       <c r="C52" s="31" t="s">
         <v>1809</v>
       </c>
@@ -13214,7 +13379,7 @@
       <c r="A53" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B53" s="141"/>
+      <c r="B53" s="143"/>
       <c r="C53" s="31" t="s">
         <v>1811</v>
       </c>
@@ -13233,7 +13398,7 @@
       <c r="A54" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B54" s="141"/>
+      <c r="B54" s="143"/>
       <c r="C54" s="31" t="s">
         <v>1815</v>
       </c>
@@ -13252,7 +13417,7 @@
       <c r="A55" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B55" s="141"/>
+      <c r="B55" s="143"/>
       <c r="C55" s="31" t="s">
         <v>1817</v>
       </c>
@@ -13271,7 +13436,7 @@
       <c r="A56" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B56" s="141"/>
+      <c r="B56" s="143"/>
       <c r="C56" s="31" t="s">
         <v>1819</v>
       </c>
@@ -13290,7 +13455,7 @@
       <c r="A57" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B57" s="141"/>
+      <c r="B57" s="143"/>
       <c r="C57" s="31" t="s">
         <v>1821</v>
       </c>
@@ -13309,7 +13474,7 @@
       <c r="A58" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B58" s="141"/>
+      <c r="B58" s="143"/>
       <c r="C58" s="31" t="s">
         <v>1837</v>
       </c>
@@ -13328,7 +13493,7 @@
       <c r="A59" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B59" s="141"/>
+      <c r="B59" s="143"/>
       <c r="C59" s="31" t="s">
         <v>1839</v>
       </c>
@@ -13347,7 +13512,7 @@
       <c r="A60" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B60" s="141"/>
+      <c r="B60" s="143"/>
       <c r="C60" s="31" t="s">
         <v>1841</v>
       </c>
@@ -13366,7 +13531,7 @@
       <c r="A61" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B61" s="141"/>
+      <c r="B61" s="143"/>
       <c r="C61" s="31" t="s">
         <v>1843</v>
       </c>
@@ -13385,7 +13550,7 @@
       <c r="A62" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B62" s="141"/>
+      <c r="B62" s="143"/>
       <c r="C62" s="31" t="s">
         <v>1845</v>
       </c>
@@ -13404,7 +13569,7 @@
       <c r="A63" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B63" s="141"/>
+      <c r="B63" s="143"/>
       <c r="C63" s="31" t="s">
         <v>1847</v>
       </c>
@@ -13423,7 +13588,7 @@
       <c r="A64" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B64" s="141"/>
+      <c r="B64" s="143"/>
       <c r="C64" s="31" t="s">
         <v>1849</v>
       </c>
@@ -13442,7 +13607,7 @@
       <c r="A65" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B65" s="141"/>
+      <c r="B65" s="143"/>
       <c r="C65" s="31" t="s">
         <v>2341</v>
       </c>
@@ -13461,7 +13626,7 @@
       <c r="A66" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B66" s="141"/>
+      <c r="B66" s="143"/>
       <c r="C66" s="31" t="s">
         <v>1852</v>
       </c>
@@ -13480,7 +13645,7 @@
       <c r="A67" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B67" s="141"/>
+      <c r="B67" s="143"/>
       <c r="C67" s="31" t="s">
         <v>1854</v>
       </c>
@@ -13499,7 +13664,7 @@
       <c r="A68" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B68" s="141"/>
+      <c r="B68" s="143"/>
       <c r="C68" s="31" t="s">
         <v>1856</v>
       </c>
@@ -13518,7 +13683,7 @@
       <c r="A69" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B69" s="141"/>
+      <c r="B69" s="143"/>
       <c r="C69" s="31" t="s">
         <v>1858</v>
       </c>
@@ -13537,7 +13702,7 @@
       <c r="A70" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B70" s="141"/>
+      <c r="B70" s="143"/>
       <c r="C70" s="31" t="s">
         <v>1860</v>
       </c>
@@ -13556,7 +13721,7 @@
       <c r="A71" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B71" s="141"/>
+      <c r="B71" s="143"/>
       <c r="C71" s="31" t="s">
         <v>1862</v>
       </c>
@@ -13575,7 +13740,7 @@
       <c r="A72" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B72" s="141"/>
+      <c r="B72" s="143"/>
       <c r="C72" s="31" t="s">
         <v>1864</v>
       </c>
@@ -13594,7 +13759,7 @@
       <c r="A73" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B73" s="141"/>
+      <c r="B73" s="143"/>
       <c r="C73" s="31" t="s">
         <v>1866</v>
       </c>
@@ -13613,7 +13778,7 @@
       <c r="A74" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B74" s="141"/>
+      <c r="B74" s="143"/>
       <c r="C74" s="31" t="s">
         <v>1868</v>
       </c>
@@ -13632,7 +13797,7 @@
       <c r="A75" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B75" s="141"/>
+      <c r="B75" s="143"/>
       <c r="C75" s="31" t="s">
         <v>1870</v>
       </c>
@@ -13651,7 +13816,7 @@
       <c r="A76" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B76" s="141"/>
+      <c r="B76" s="143"/>
       <c r="C76" s="31" t="s">
         <v>1877</v>
       </c>
@@ -13672,7 +13837,7 @@
       <c r="A77" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B77" s="141"/>
+      <c r="B77" s="143"/>
       <c r="C77" s="31" t="s">
         <v>1880</v>
       </c>
@@ -13691,7 +13856,7 @@
       <c r="A78" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B78" s="141"/>
+      <c r="B78" s="143"/>
       <c r="C78" s="31" t="s">
         <v>2314</v>
       </c>
@@ -13712,7 +13877,7 @@
       <c r="A79" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B79" s="142"/>
+      <c r="B79" s="144"/>
       <c r="C79" s="31" t="s">
         <v>1890</v>
       </c>
@@ -13742,7 +13907,7 @@
       <c r="A81" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B81" s="149" t="s">
+      <c r="B81" s="151" t="s">
         <v>911</v>
       </c>
       <c r="C81" s="31" t="s">
@@ -13763,7 +13928,7 @@
       <c r="A82" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B82" s="150"/>
+      <c r="B82" s="152"/>
       <c r="C82" s="31" t="s">
         <v>1908</v>
       </c>
@@ -13793,7 +13958,7 @@
       <c r="A84" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B84" s="145" t="s">
+      <c r="B84" s="147" t="s">
         <v>1910</v>
       </c>
       <c r="C84" s="31" t="s">
@@ -13814,7 +13979,7 @@
       <c r="A85" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B85" s="146"/>
+      <c r="B85" s="148"/>
       <c r="C85" s="31" t="s">
         <v>1914</v>
       </c>
@@ -13833,7 +13998,7 @@
       <c r="A86" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B86" s="146"/>
+      <c r="B86" s="148"/>
       <c r="C86" s="31" t="s">
         <v>2346</v>
       </c>
@@ -13852,7 +14017,7 @@
       <c r="A87" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B87" s="146"/>
+      <c r="B87" s="148"/>
       <c r="C87" s="31" t="s">
         <v>1911</v>
       </c>
@@ -13871,7 +14036,7 @@
       <c r="A88" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B88" s="146"/>
+      <c r="B88" s="148"/>
       <c r="C88" s="31" t="s">
         <v>1913</v>
       </c>
@@ -13890,7 +14055,7 @@
       <c r="A89" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B89" s="146"/>
+      <c r="B89" s="148"/>
       <c r="C89" s="31" t="s">
         <v>2213</v>
       </c>
@@ -13909,7 +14074,7 @@
       <c r="A90" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B90" s="146"/>
+      <c r="B90" s="148"/>
       <c r="C90" s="31" t="s">
         <v>2147</v>
       </c>
@@ -13928,7 +14093,7 @@
       <c r="A91" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B91" s="147"/>
+      <c r="B91" s="149"/>
       <c r="C91" s="31" t="s">
         <v>2215</v>
       </c>
@@ -13958,7 +14123,7 @@
       <c r="A93" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B93" s="149" t="s">
+      <c r="B93" s="151" t="s">
         <v>1919</v>
       </c>
       <c r="C93" s="31" t="s">
@@ -13979,7 +14144,7 @@
       <c r="A94" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B94" s="151"/>
+      <c r="B94" s="153"/>
       <c r="C94" s="31" t="s">
         <v>1920</v>
       </c>
@@ -13998,7 +14163,7 @@
       <c r="A95" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B95" s="151"/>
+      <c r="B95" s="153"/>
       <c r="C95" s="31" t="s">
         <v>1923</v>
       </c>
@@ -14017,7 +14182,7 @@
       <c r="A96" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B96" s="151"/>
+      <c r="B96" s="153"/>
       <c r="C96" s="31" t="s">
         <v>1925</v>
       </c>
@@ -14036,7 +14201,7 @@
       <c r="A97" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B97" s="151"/>
+      <c r="B97" s="153"/>
       <c r="C97" s="31" t="s">
         <v>1929</v>
       </c>
@@ -14055,7 +14220,7 @@
       <c r="A98" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B98" s="151"/>
+      <c r="B98" s="153"/>
       <c r="C98" s="31" t="s">
         <v>1927</v>
       </c>
@@ -14074,7 +14239,7 @@
       <c r="A99" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B99" s="151"/>
+      <c r="B99" s="153"/>
       <c r="C99" s="31" t="s">
         <v>2259</v>
       </c>
@@ -14093,7 +14258,7 @@
       <c r="A100" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B100" s="151"/>
+      <c r="B100" s="153"/>
       <c r="C100" s="31" t="s">
         <v>2260</v>
       </c>
@@ -14112,7 +14277,7 @@
       <c r="A101" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B101" s="150"/>
+      <c r="B101" s="152"/>
       <c r="C101" s="31" t="s">
         <v>2287</v>
       </c>
@@ -14142,7 +14307,7 @@
       <c r="A103" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B103" s="140" t="s">
+      <c r="B103" s="142" t="s">
         <v>964</v>
       </c>
       <c r="C103" s="31" t="s">
@@ -14163,7 +14328,7 @@
       <c r="A104" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B104" s="141"/>
+      <c r="B104" s="143"/>
       <c r="C104" s="31" t="s">
         <v>2333</v>
       </c>
@@ -14182,7 +14347,7 @@
       <c r="A105" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B105" s="142"/>
+      <c r="B105" s="144"/>
       <c r="C105" s="31" t="s">
         <v>2335</v>
       </c>
@@ -14244,7 +14409,7 @@
       <c r="A109" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B109" s="149" t="s">
+      <c r="B109" s="151" t="s">
         <v>945</v>
       </c>
       <c r="C109" s="31" t="s">
@@ -14265,7 +14430,7 @@
       <c r="A110" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B110" s="151"/>
+      <c r="B110" s="153"/>
       <c r="C110" s="31" t="s">
         <v>1937</v>
       </c>
@@ -14284,7 +14449,7 @@
       <c r="A111" s="30" t="s">
         <v>2301</v>
       </c>
-      <c r="B111" s="151"/>
+      <c r="B111" s="153"/>
       <c r="C111" s="31" t="s">
         <v>2289</v>
       </c>
@@ -14303,7 +14468,7 @@
       <c r="A112" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B112" s="150"/>
+      <c r="B112" s="152"/>
       <c r="C112" s="31" t="s">
         <v>1939</v>
       </c>
@@ -14333,7 +14498,7 @@
       <c r="A114" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B114" s="149" t="s">
+      <c r="B114" s="151" t="s">
         <v>951</v>
       </c>
       <c r="C114" s="31" t="s">
@@ -14354,7 +14519,7 @@
       <c r="A115" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B115" s="150"/>
+      <c r="B115" s="152"/>
       <c r="C115" s="31" t="s">
         <v>1944</v>
       </c>
@@ -14448,7 +14613,7 @@
       <c r="A121" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B121" s="145" t="s">
+      <c r="B121" s="147" t="s">
         <v>1950</v>
       </c>
       <c r="C121" s="31" t="s">
@@ -14469,7 +14634,7 @@
       <c r="A122" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B122" s="146"/>
+      <c r="B122" s="148"/>
       <c r="C122" s="31" t="s">
         <v>1954</v>
       </c>
@@ -14488,7 +14653,7 @@
       <c r="A123" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B123" s="146"/>
+      <c r="B123" s="148"/>
       <c r="C123" s="31" t="s">
         <v>1956</v>
       </c>
@@ -14507,7 +14672,7 @@
       <c r="A124" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B124" s="146"/>
+      <c r="B124" s="148"/>
       <c r="C124" s="31" t="s">
         <v>1958</v>
       </c>
@@ -14526,7 +14691,7 @@
       <c r="A125" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B125" s="147"/>
+      <c r="B125" s="149"/>
       <c r="C125" s="31" t="s">
         <v>2268</v>
       </c>
@@ -14556,7 +14721,7 @@
       <c r="A127" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B127" s="149" t="s">
+      <c r="B127" s="151" t="s">
         <v>1960</v>
       </c>
       <c r="C127" s="31" t="s">
@@ -14577,7 +14742,7 @@
       <c r="A128" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B128" s="151"/>
+      <c r="B128" s="153"/>
       <c r="C128" s="31" t="s">
         <v>1964</v>
       </c>
@@ -14596,7 +14761,7 @@
       <c r="A129" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B129" s="150"/>
+      <c r="B129" s="152"/>
       <c r="C129" s="31" t="s">
         <v>1966</v>
       </c>
@@ -14658,7 +14823,7 @@
       <c r="A133" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B133" s="149" t="s">
+      <c r="B133" s="151" t="s">
         <v>1976</v>
       </c>
       <c r="C133" s="31" t="s">
@@ -14679,7 +14844,7 @@
       <c r="A134" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B134" s="150"/>
+      <c r="B134" s="152"/>
       <c r="C134" s="31" t="s">
         <v>1980</v>
       </c>
@@ -14709,7 +14874,7 @@
       <c r="A136" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B136" s="149" t="s">
+      <c r="B136" s="151" t="s">
         <v>1982</v>
       </c>
       <c r="C136" s="31" t="s">
@@ -14730,7 +14895,7 @@
       <c r="A137" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B137" s="151"/>
+      <c r="B137" s="153"/>
       <c r="C137" s="31" t="s">
         <v>1986</v>
       </c>
@@ -14749,7 +14914,7 @@
       <c r="A138" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B138" s="151"/>
+      <c r="B138" s="153"/>
       <c r="C138" s="31" t="s">
         <v>1988</v>
       </c>
@@ -14768,7 +14933,7 @@
       <c r="A139" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B139" s="150"/>
+      <c r="B139" s="152"/>
       <c r="C139" s="31" t="s">
         <v>1990</v>
       </c>
@@ -14798,7 +14963,7 @@
       <c r="A141" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B141" s="145" t="s">
+      <c r="B141" s="147" t="s">
         <v>1994</v>
       </c>
       <c r="C141" s="31" t="s">
@@ -14819,7 +14984,7 @@
       <c r="A142" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B142" s="146"/>
+      <c r="B142" s="148"/>
       <c r="C142" s="31" t="s">
         <v>1998</v>
       </c>
@@ -14838,7 +15003,7 @@
       <c r="A143" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B143" s="147"/>
+      <c r="B143" s="149"/>
       <c r="C143" s="31" t="s">
         <v>2000</v>
       </c>
@@ -14900,7 +15065,7 @@
       <c r="A147" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B147" s="149" t="s">
+      <c r="B147" s="151" t="s">
         <v>2005</v>
       </c>
       <c r="C147" s="31" t="s">
@@ -14921,7 +15086,7 @@
       <c r="A148" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B148" s="151"/>
+      <c r="B148" s="153"/>
       <c r="C148" s="31" t="s">
         <v>2320</v>
       </c>
@@ -14940,7 +15105,7 @@
       <c r="A149" s="30" t="s">
         <v>1642</v>
       </c>
-      <c r="B149" s="150"/>
+      <c r="B149" s="152"/>
       <c r="C149" s="31" t="s">
         <v>2010</v>
       </c>
@@ -15101,22 +15266,22 @@
       <c r="G158" s="34"/>
     </row>
     <row r="160" spans="1:7">
-      <c r="C160" s="143"/>
-      <c r="D160" s="143"/>
-      <c r="E160" s="143"/>
-      <c r="F160" s="143"/>
+      <c r="C160" s="145"/>
+      <c r="D160" s="145"/>
+      <c r="E160" s="145"/>
+      <c r="F160" s="145"/>
     </row>
     <row r="161" spans="1:7">
-      <c r="C161" s="143"/>
-      <c r="D161" s="143"/>
-      <c r="E161" s="143"/>
-      <c r="F161" s="143"/>
+      <c r="C161" s="145"/>
+      <c r="D161" s="145"/>
+      <c r="E161" s="145"/>
+      <c r="F161" s="145"/>
     </row>
     <row r="162" spans="1:7">
-      <c r="C162" s="144"/>
-      <c r="D162" s="144"/>
-      <c r="E162" s="144"/>
-      <c r="F162" s="144"/>
+      <c r="C162" s="146"/>
+      <c r="D162" s="146"/>
+      <c r="E162" s="146"/>
+      <c r="F162" s="146"/>
     </row>
     <row r="163" spans="1:7">
       <c r="A163" s="116" t="s">
@@ -15292,7 +15457,7 @@
       <c r="A173" s="30" t="s">
         <v>1641</v>
       </c>
-      <c r="B173" s="148" t="s">
+      <c r="B173" s="150" t="s">
         <v>1972</v>
       </c>
       <c r="C173" s="113" t="s">
@@ -15311,7 +15476,7 @@
       <c r="A174" s="30" t="s">
         <v>1641</v>
       </c>
-      <c r="B174" s="148"/>
+      <c r="B174" s="150"/>
       <c r="C174" s="113" t="s">
         <v>1975</v>
       </c>
@@ -15411,9 +15576,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M1554"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A980" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1563" sqref="B1563"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A898" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I906" sqref="I906"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -45813,7 +45978,7 @@
       <c r="L882" s="7"/>
       <c r="M882" s="10"/>
     </row>
-    <row r="883" spans="1:13" hidden="1">
+    <row r="883" spans="1:13">
       <c r="A883" s="7" t="s">
         <v>1102</v>
       </c>
@@ -45846,7 +46011,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="884" spans="1:13" hidden="1">
+    <row r="884" spans="1:13">
       <c r="A884" s="7" t="s">
         <v>1102</v>
       </c>
@@ -45887,7 +46052,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="885" spans="1:13" hidden="1">
+    <row r="885" spans="1:13">
       <c r="A885" s="7" t="s">
         <v>1102</v>
       </c>
@@ -45928,7 +46093,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="886" spans="1:13" hidden="1">
+    <row r="886" spans="1:13">
       <c r="A886" s="7" t="s">
         <v>1102</v>
       </c>
@@ -45969,7 +46134,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="887" spans="1:13" hidden="1">
+    <row r="887" spans="1:13">
       <c r="A887" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46010,7 +46175,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="888" spans="1:13" hidden="1">
+    <row r="888" spans="1:13">
       <c r="A888" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46051,7 +46216,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="889" spans="1:13" hidden="1">
+    <row r="889" spans="1:13">
       <c r="A889" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46084,7 +46249,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="890" spans="1:13" hidden="1">
+    <row r="890" spans="1:13">
       <c r="A890" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46117,7 +46282,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="891" spans="1:13" hidden="1">
+    <row r="891" spans="1:13">
       <c r="A891" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46150,7 +46315,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="892" spans="1:13" hidden="1">
+    <row r="892" spans="1:13">
       <c r="A892" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46183,7 +46348,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="893" spans="1:13" hidden="1">
+    <row r="893" spans="1:13">
       <c r="A893" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46216,7 +46381,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="894" spans="1:13" hidden="1">
+    <row r="894" spans="1:13">
       <c r="A894" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46249,7 +46414,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="895" spans="1:13" hidden="1">
+    <row r="895" spans="1:13">
       <c r="A895" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46282,7 +46447,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="896" spans="1:13" hidden="1">
+    <row r="896" spans="1:13">
       <c r="A896" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46315,7 +46480,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="897" spans="1:13" hidden="1">
+    <row r="897" spans="1:13">
       <c r="A897" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46348,7 +46513,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="898" spans="1:13" hidden="1">
+    <row r="898" spans="1:13">
       <c r="A898" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46381,7 +46546,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="899" spans="1:13" hidden="1">
+    <row r="899" spans="1:13">
       <c r="A899" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46414,7 +46579,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="900" spans="1:13" hidden="1">
+    <row r="900" spans="1:13">
       <c r="A900" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46447,7 +46612,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="901" spans="1:13" hidden="1">
+    <row r="901" spans="1:13">
       <c r="A901" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46480,7 +46645,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="902" spans="1:13" hidden="1">
+    <row r="902" spans="1:13">
       <c r="A902" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46513,7 +46678,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="903" spans="1:13" hidden="1">
+    <row r="903" spans="1:13">
       <c r="A903" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46546,7 +46711,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="904" spans="1:13" hidden="1">
+    <row r="904" spans="1:13">
       <c r="A904" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46579,7 +46744,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="905" spans="1:13" hidden="1">
+    <row r="905" spans="1:13">
       <c r="A905" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46612,7 +46777,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="906" spans="1:13" hidden="1">
+    <row r="906" spans="1:13">
       <c r="A906" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46653,7 +46818,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="907" spans="1:13" hidden="1">
+    <row r="907" spans="1:13">
       <c r="A907" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46686,7 +46851,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="908" spans="1:13" hidden="1">
+    <row r="908" spans="1:13">
       <c r="A908" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46719,7 +46884,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="909" spans="1:13" hidden="1">
+    <row r="909" spans="1:13">
       <c r="A909" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46752,7 +46917,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="910" spans="1:13" hidden="1">
+    <row r="910" spans="1:13">
       <c r="A910" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46785,7 +46950,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="911" spans="1:13" hidden="1">
+    <row r="911" spans="1:13">
       <c r="A911" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46818,7 +46983,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="912" spans="1:13" hidden="1">
+    <row r="912" spans="1:13">
       <c r="A912" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46851,7 +47016,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="913" spans="1:13" hidden="1">
+    <row r="913" spans="1:13">
       <c r="A913" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46884,7 +47049,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="914" spans="1:13" hidden="1">
+    <row r="914" spans="1:13">
       <c r="A914" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46919,7 +47084,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="915" spans="1:13" hidden="1">
+    <row r="915" spans="1:13">
       <c r="A915" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46954,7 +47119,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="916" spans="1:13" hidden="1">
+    <row r="916" spans="1:13">
       <c r="A916" s="7" t="s">
         <v>1102</v>
       </c>
@@ -46995,7 +47160,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="917" spans="1:13" hidden="1">
+    <row r="917" spans="1:13">
       <c r="A917" s="7" t="s">
         <v>1102</v>
       </c>
@@ -47036,7 +47201,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="918" spans="1:13" hidden="1">
+    <row r="918" spans="1:13">
       <c r="A918" s="7" t="s">
         <v>1102</v>
       </c>
@@ -47069,7 +47234,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="919" spans="1:13" hidden="1">
+    <row r="919" spans="1:13">
       <c r="A919" s="7" t="s">
         <v>1102</v>
       </c>
@@ -47102,7 +47267,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="920" spans="1:13" hidden="1">
+    <row r="920" spans="1:13">
       <c r="A920" s="7" t="s">
         <v>1102</v>
       </c>
@@ -47135,7 +47300,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="921" spans="1:13" hidden="1">
+    <row r="921" spans="1:13">
       <c r="A921" s="7" t="s">
         <v>1102</v>
       </c>
@@ -47168,7 +47333,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="922" spans="1:13" hidden="1">
+    <row r="922" spans="1:13">
       <c r="A922" s="7" t="s">
         <v>1102</v>
       </c>
@@ -47201,7 +47366,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="923" spans="1:13" hidden="1">
+    <row r="923" spans="1:13">
       <c r="A923" s="7" t="s">
         <v>1102</v>
       </c>
@@ -47234,7 +47399,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="924" spans="1:13" hidden="1">
+    <row r="924" spans="1:13">
       <c r="A924" s="7" t="s">
         <v>1102</v>
       </c>
@@ -48247,7 +48412,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="953" spans="1:13">
+    <row r="953" spans="1:13" hidden="1">
       <c r="A953" s="7" t="s">
         <v>1102</v>
       </c>
@@ -48288,7 +48453,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="954" spans="1:13">
+    <row r="954" spans="1:13" hidden="1">
       <c r="A954" s="7" t="s">
         <v>1102</v>
       </c>
@@ -48329,7 +48494,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="955" spans="1:13">
+    <row r="955" spans="1:13" hidden="1">
       <c r="A955" s="7" t="s">
         <v>1102</v>
       </c>
@@ -48362,7 +48527,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="956" spans="1:13">
+    <row r="956" spans="1:13" hidden="1">
       <c r="A956" s="7" t="s">
         <v>1102</v>
       </c>
@@ -48395,7 +48560,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="957" spans="1:13">
+    <row r="957" spans="1:13" hidden="1">
       <c r="A957" s="7" t="s">
         <v>1102</v>
       </c>
@@ -48436,7 +48601,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="958" spans="1:13">
+    <row r="958" spans="1:13" hidden="1">
       <c r="A958" s="7" t="s">
         <v>1102</v>
       </c>
@@ -48477,7 +48642,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="959" spans="1:13">
+    <row r="959" spans="1:13" hidden="1">
       <c r="A959" s="7" t="s">
         <v>1102</v>
       </c>
@@ -48518,7 +48683,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="960" spans="1:13">
+    <row r="960" spans="1:13" hidden="1">
       <c r="A960" s="7" t="s">
         <v>1102</v>
       </c>
@@ -48551,7 +48716,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="961" spans="1:13">
+    <row r="961" spans="1:13" hidden="1">
       <c r="A961" s="7" t="s">
         <v>1102</v>
       </c>
@@ -48584,7 +48749,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="962" spans="1:13">
+    <row r="962" spans="1:13" hidden="1">
       <c r="A962" s="7" t="s">
         <v>1102</v>
       </c>
@@ -48625,7 +48790,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="963" spans="1:13">
+    <row r="963" spans="1:13" hidden="1">
       <c r="A963" s="7" t="s">
         <v>1102</v>
       </c>
@@ -48666,7 +48831,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="964" spans="1:13">
+    <row r="964" spans="1:13" hidden="1">
       <c r="A964" s="7" t="s">
         <v>1102</v>
       </c>
@@ -48707,7 +48872,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="965" spans="1:13">
+    <row r="965" spans="1:13" hidden="1">
       <c r="A965" s="7" t="s">
         <v>1102</v>
       </c>
@@ -48744,7 +48909,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="966" spans="1:13">
+    <row r="966" spans="1:13" hidden="1">
       <c r="A966" s="7" t="s">
         <v>1102</v>
       </c>
@@ -48785,7 +48950,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="967" spans="1:13">
+    <row r="967" spans="1:13" hidden="1">
       <c r="A967" s="7" t="s">
         <v>1102</v>
       </c>
@@ -48818,7 +48983,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="968" spans="1:13">
+    <row r="968" spans="1:13" hidden="1">
       <c r="A968" s="7" t="s">
         <v>1102</v>
       </c>
@@ -48851,7 +49016,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="969" spans="1:13">
+    <row r="969" spans="1:13" hidden="1">
       <c r="A969" s="7" t="s">
         <v>1102</v>
       </c>
@@ -48884,7 +49049,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="970" spans="1:13">
+    <row r="970" spans="1:13" hidden="1">
       <c r="A970" s="7" t="s">
         <v>1102</v>
       </c>
@@ -48917,7 +49082,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="971" spans="1:13">
+    <row r="971" spans="1:13" hidden="1">
       <c r="A971" s="7" t="s">
         <v>1102</v>
       </c>
@@ -48950,7 +49115,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="972" spans="1:13">
+    <row r="972" spans="1:13" hidden="1">
       <c r="A972" s="7" t="s">
         <v>1102</v>
       </c>
@@ -48983,7 +49148,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="973" spans="1:13">
+    <row r="973" spans="1:13" hidden="1">
       <c r="A973" s="7" t="s">
         <v>1102</v>
       </c>
@@ -49016,7 +49181,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="974" spans="1:13">
+    <row r="974" spans="1:13" hidden="1">
       <c r="A974" s="7" t="s">
         <v>1102</v>
       </c>
@@ -49049,7 +49214,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="975" spans="1:13">
+    <row r="975" spans="1:13" hidden="1">
       <c r="A975" s="7" t="s">
         <v>1102</v>
       </c>
@@ -49082,7 +49247,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="976" spans="1:13">
+    <row r="976" spans="1:13" hidden="1">
       <c r="A976" s="7" t="s">
         <v>1102</v>
       </c>
@@ -49115,7 +49280,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="977" spans="1:13">
+    <row r="977" spans="1:13" hidden="1">
       <c r="A977" s="7" t="s">
         <v>1102</v>
       </c>
@@ -49148,7 +49313,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="978" spans="1:13">
+    <row r="978" spans="1:13" hidden="1">
       <c r="A978" s="7" t="s">
         <v>1102</v>
       </c>
@@ -49181,7 +49346,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="979" spans="1:13">
+    <row r="979" spans="1:13" hidden="1">
       <c r="A979" s="7" t="s">
         <v>1102</v>
       </c>
@@ -49214,7 +49379,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="980" spans="1:13">
+    <row r="980" spans="1:13" hidden="1">
       <c r="A980" s="7" t="s">
         <v>1102</v>
       </c>
@@ -49247,7 +49412,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="981" spans="1:13">
+    <row r="981" spans="1:13" hidden="1">
       <c r="A981" s="7" t="s">
         <v>1102</v>
       </c>
@@ -49280,7 +49445,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="982" spans="1:13">
+    <row r="982" spans="1:13" hidden="1">
       <c r="A982" s="7" t="s">
         <v>1102</v>
       </c>
@@ -49321,7 +49486,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="983" spans="1:13">
+    <row r="983" spans="1:13" hidden="1">
       <c r="A983" s="7" t="s">
         <v>1102</v>
       </c>
@@ -49354,7 +49519,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="984" spans="1:13">
+    <row r="984" spans="1:13" hidden="1">
       <c r="A984" s="7" t="s">
         <v>1102</v>
       </c>
@@ -49387,7 +49552,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="985" spans="1:13">
+    <row r="985" spans="1:13" hidden="1">
       <c r="A985" s="7" t="s">
         <v>1102</v>
       </c>
@@ -49420,7 +49585,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="986" spans="1:13">
+    <row r="986" spans="1:13" hidden="1">
       <c r="A986" s="7" t="s">
         <v>1102</v>
       </c>
@@ -49453,7 +49618,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="987" spans="1:13">
+    <row r="987" spans="1:13" hidden="1">
       <c r="A987" s="7" t="s">
         <v>1102</v>
       </c>
@@ -49486,7 +49651,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="988" spans="1:13">
+    <row r="988" spans="1:13" hidden="1">
       <c r="A988" s="7" t="s">
         <v>1102</v>
       </c>
@@ -49519,7 +49684,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="989" spans="1:13">
+    <row r="989" spans="1:13" hidden="1">
       <c r="A989" s="7" t="s">
         <v>1102</v>
       </c>
@@ -49552,7 +49717,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="990" spans="1:13">
+    <row r="990" spans="1:13" hidden="1">
       <c r="A990" s="7" t="s">
         <v>1102</v>
       </c>
@@ -49585,7 +49750,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="991" spans="1:13">
+    <row r="991" spans="1:13" hidden="1">
       <c r="A991" s="7" t="s">
         <v>1102</v>
       </c>
@@ -49618,7 +49783,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="992" spans="1:13">
+    <row r="992" spans="1:13" hidden="1">
       <c r="A992" s="7" t="s">
         <v>1102</v>
       </c>
@@ -49651,7 +49816,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="993" spans="1:13">
+    <row r="993" spans="1:13" hidden="1">
       <c r="A993" s="7" t="s">
         <v>1102</v>
       </c>
@@ -49684,7 +49849,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="994" spans="1:13">
+    <row r="994" spans="1:13" hidden="1">
       <c r="A994" s="7" t="s">
         <v>1102</v>
       </c>
@@ -49725,7 +49890,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="995" spans="1:13">
+    <row r="995" spans="1:13" hidden="1">
       <c r="A995" s="7" t="s">
         <v>1102</v>
       </c>
@@ -49766,7 +49931,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="996" spans="1:13">
+    <row r="996" spans="1:13" hidden="1">
       <c r="A996" s="7" t="s">
         <v>1102</v>
       </c>
@@ -49799,7 +49964,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="997" spans="1:13">
+    <row r="997" spans="1:13" hidden="1">
       <c r="A997" s="7" t="s">
         <v>1102</v>
       </c>
@@ -49840,7 +50005,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="998" spans="1:13">
+    <row r="998" spans="1:13" hidden="1">
       <c r="A998" s="7" t="s">
         <v>1102</v>
       </c>
@@ -49881,7 +50046,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="999" spans="1:13">
+    <row r="999" spans="1:13" hidden="1">
       <c r="A999" s="7" t="s">
         <v>1102</v>
       </c>
@@ -69129,19 +69294,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="153" t="s">
+      <c r="A1" s="155" t="s">
         <v>1061</v>
       </c>
-      <c r="B1" s="153"/>
-      <c r="C1" s="153"/>
-      <c r="D1" s="153"/>
-      <c r="E1" s="153"/>
-      <c r="F1" s="153"/>
-      <c r="H1" s="153" t="s">
+      <c r="B1" s="155"/>
+      <c r="C1" s="155"/>
+      <c r="D1" s="155"/>
+      <c r="E1" s="155"/>
+      <c r="F1" s="155"/>
+      <c r="H1" s="155" t="s">
         <v>1100</v>
       </c>
-      <c r="I1" s="153"/>
-      <c r="J1" s="153"/>
+      <c r="I1" s="155"/>
+      <c r="J1" s="155"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
@@ -69326,11 +69491,11 @@
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="152"/>
-      <c r="B12" s="152"/>
-      <c r="C12" s="152"/>
-      <c r="D12" s="152"/>
-      <c r="E12" s="152"/>
+      <c r="A12" s="154"/>
+      <c r="B12" s="154"/>
+      <c r="C12" s="154"/>
+      <c r="D12" s="154"/>
+      <c r="E12" s="154"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -69350,9 +69515,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I493"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F494" sqref="F494"/>
+      <selection pane="bottomLeft" activeCell="G507" sqref="G507"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -69370,11 +69535,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" customHeight="1">
-      <c r="A1" s="154" t="s">
+      <c r="A1" s="156" t="s">
         <v>2896</v>
       </c>
-      <c r="B1" s="154"/>
-      <c r="C1" s="154"/>
+      <c r="B1" s="156"/>
+      <c r="C1" s="156"/>
       <c r="I1" s="135" t="s">
         <v>3047</v>
       </c>
@@ -81868,22 +82033,22 @@
       </c>
     </row>
     <row r="459" spans="1:9" hidden="1">
-      <c r="A459" s="155"/>
-      <c r="B459" s="155"/>
-      <c r="C459" s="155"/>
-      <c r="D459" s="155" t="s">
+      <c r="A459" s="141"/>
+      <c r="B459" s="141"/>
+      <c r="C459" s="141"/>
+      <c r="D459" s="141" t="s">
         <v>3048</v>
       </c>
-      <c r="E459" s="155" t="s">
+      <c r="E459" s="141" t="s">
         <v>3049</v>
       </c>
-      <c r="F459" s="155" t="s">
+      <c r="F459" s="141" t="s">
         <v>3050</v>
       </c>
-      <c r="G459" s="155" t="s">
+      <c r="G459" s="141" t="s">
         <v>3051</v>
       </c>
-      <c r="H459" s="155" t="s">
+      <c r="H459" s="141" t="s">
         <v>2501</v>
       </c>
       <c r="I459" s="135" t="s">
@@ -81891,22 +82056,22 @@
       </c>
     </row>
     <row r="460" spans="1:9" hidden="1">
-      <c r="A460" s="155"/>
-      <c r="B460" s="155"/>
-      <c r="C460" s="155"/>
-      <c r="D460" s="155" t="s">
+      <c r="A460" s="141"/>
+      <c r="B460" s="141"/>
+      <c r="C460" s="141"/>
+      <c r="D460" s="141" t="s">
         <v>3048</v>
       </c>
-      <c r="E460" s="155" t="s">
+      <c r="E460" s="141" t="s">
         <v>3049</v>
       </c>
-      <c r="F460" s="155" t="s">
+      <c r="F460" s="141" t="s">
         <v>3052</v>
       </c>
-      <c r="G460" s="155" t="s">
+      <c r="G460" s="141" t="s">
         <v>3053</v>
       </c>
-      <c r="H460" s="155" t="s">
+      <c r="H460" s="141" t="s">
         <v>2501</v>
       </c>
       <c r="I460" s="135" t="s">
@@ -81914,22 +82079,22 @@
       </c>
     </row>
     <row r="461" spans="1:9" hidden="1">
-      <c r="A461" s="155"/>
-      <c r="B461" s="155"/>
-      <c r="C461" s="155"/>
-      <c r="D461" s="155" t="s">
+      <c r="A461" s="141"/>
+      <c r="B461" s="141"/>
+      <c r="C461" s="141"/>
+      <c r="D461" s="141" t="s">
         <v>3048</v>
       </c>
-      <c r="E461" s="155" t="s">
+      <c r="E461" s="141" t="s">
         <v>3049</v>
       </c>
-      <c r="F461" s="155" t="s">
+      <c r="F461" s="141" t="s">
         <v>3052</v>
       </c>
-      <c r="G461" s="155" t="s">
+      <c r="G461" s="141" t="s">
         <v>3056</v>
       </c>
-      <c r="H461" s="155" t="s">
+      <c r="H461" s="141" t="s">
         <v>2501</v>
       </c>
       <c r="I461" s="135" t="s">
@@ -81937,22 +82102,22 @@
       </c>
     </row>
     <row r="462" spans="1:9" hidden="1">
-      <c r="A462" s="155"/>
-      <c r="B462" s="155"/>
-      <c r="C462" s="155"/>
-      <c r="D462" s="155" t="s">
+      <c r="A462" s="141"/>
+      <c r="B462" s="141"/>
+      <c r="C462" s="141"/>
+      <c r="D462" s="141" t="s">
         <v>3048</v>
       </c>
-      <c r="E462" s="155" t="s">
+      <c r="E462" s="141" t="s">
         <v>3049</v>
       </c>
-      <c r="F462" s="155" t="s">
+      <c r="F462" s="141" t="s">
         <v>3054</v>
       </c>
-      <c r="G462" s="155" t="s">
+      <c r="G462" s="141" t="s">
         <v>3055</v>
       </c>
-      <c r="H462" s="155" t="s">
+      <c r="H462" s="141" t="s">
         <v>2501</v>
       </c>
       <c r="I462" s="135" t="s">
@@ -81960,22 +82125,22 @@
       </c>
     </row>
     <row r="463" spans="1:9" hidden="1">
-      <c r="A463" s="155"/>
-      <c r="B463" s="155"/>
-      <c r="C463" s="155"/>
-      <c r="D463" s="155" t="s">
+      <c r="A463" s="141"/>
+      <c r="B463" s="141"/>
+      <c r="C463" s="141"/>
+      <c r="D463" s="141" t="s">
         <v>3048</v>
       </c>
-      <c r="E463" s="155" t="s">
+      <c r="E463" s="141" t="s">
         <v>3049</v>
       </c>
-      <c r="F463" s="155" t="s">
+      <c r="F463" s="141" t="s">
         <v>3054</v>
       </c>
-      <c r="G463" s="155" t="s">
+      <c r="G463" s="141" t="s">
         <v>3057</v>
       </c>
-      <c r="H463" s="155" t="s">
+      <c r="H463" s="141" t="s">
         <v>2501</v>
       </c>
       <c r="I463" s="135" t="s">
@@ -81983,22 +82148,22 @@
       </c>
     </row>
     <row r="464" spans="1:9" hidden="1">
-      <c r="A464" s="155"/>
-      <c r="B464" s="155"/>
-      <c r="C464" s="155"/>
-      <c r="D464" s="155" t="s">
+      <c r="A464" s="141"/>
+      <c r="B464" s="141"/>
+      <c r="C464" s="141"/>
+      <c r="D464" s="141" t="s">
         <v>3048</v>
       </c>
-      <c r="E464" s="155" t="s">
+      <c r="E464" s="141" t="s">
         <v>3049</v>
       </c>
-      <c r="F464" s="155" t="s">
+      <c r="F464" s="141" t="s">
         <v>3054</v>
       </c>
-      <c r="G464" s="155" t="s">
+      <c r="G464" s="141" t="s">
         <v>3058</v>
       </c>
-      <c r="H464" s="155" t="s">
+      <c r="H464" s="141" t="s">
         <v>2501</v>
       </c>
       <c r="I464" s="135" t="s">
@@ -82006,22 +82171,22 @@
       </c>
     </row>
     <row r="465" spans="1:9" hidden="1">
-      <c r="A465" s="155"/>
-      <c r="B465" s="155"/>
-      <c r="C465" s="155"/>
-      <c r="D465" s="155" t="s">
+      <c r="A465" s="141"/>
+      <c r="B465" s="141"/>
+      <c r="C465" s="141"/>
+      <c r="D465" s="141" t="s">
         <v>3048</v>
       </c>
-      <c r="E465" s="155" t="s">
+      <c r="E465" s="141" t="s">
         <v>3049</v>
       </c>
-      <c r="F465" s="155" t="s">
+      <c r="F465" s="141" t="s">
         <v>3054</v>
       </c>
-      <c r="G465" s="155" t="s">
+      <c r="G465" s="141" t="s">
         <v>3059</v>
       </c>
-      <c r="H465" s="155" t="s">
+      <c r="H465" s="141" t="s">
         <v>2501</v>
       </c>
       <c r="I465" s="135" t="s">
@@ -82029,22 +82194,22 @@
       </c>
     </row>
     <row r="466" spans="1:9" hidden="1">
-      <c r="A466" s="155"/>
-      <c r="B466" s="155"/>
-      <c r="C466" s="155"/>
-      <c r="D466" s="155" t="s">
+      <c r="A466" s="141"/>
+      <c r="B466" s="141"/>
+      <c r="C466" s="141"/>
+      <c r="D466" s="141" t="s">
         <v>3048</v>
       </c>
-      <c r="E466" s="155" t="s">
+      <c r="E466" s="141" t="s">
         <v>3049</v>
       </c>
-      <c r="F466" s="155" t="s">
+      <c r="F466" s="141" t="s">
         <v>3054</v>
       </c>
-      <c r="G466" s="155" t="s">
+      <c r="G466" s="141" t="s">
         <v>3060</v>
       </c>
-      <c r="H466" s="155" t="s">
+      <c r="H466" s="141" t="s">
         <v>2501</v>
       </c>
       <c r="I466" s="135" t="s">
@@ -82052,22 +82217,22 @@
       </c>
     </row>
     <row r="467" spans="1:9" hidden="1">
-      <c r="A467" s="155"/>
-      <c r="B467" s="155"/>
-      <c r="C467" s="155"/>
-      <c r="D467" s="155" t="s">
+      <c r="A467" s="141"/>
+      <c r="B467" s="141"/>
+      <c r="C467" s="141"/>
+      <c r="D467" s="141" t="s">
         <v>3048</v>
       </c>
-      <c r="E467" s="155" t="s">
+      <c r="E467" s="141" t="s">
         <v>3049</v>
       </c>
-      <c r="F467" s="155" t="s">
+      <c r="F467" s="141" t="s">
         <v>3061</v>
       </c>
-      <c r="G467" s="155" t="s">
+      <c r="G467" s="141" t="s">
         <v>2846</v>
       </c>
-      <c r="H467" s="155" t="s">
+      <c r="H467" s="141" t="s">
         <v>2501</v>
       </c>
       <c r="I467" s="135" t="s">
@@ -82075,22 +82240,22 @@
       </c>
     </row>
     <row r="468" spans="1:9" hidden="1">
-      <c r="A468" s="155"/>
-      <c r="B468" s="155"/>
-      <c r="C468" s="155"/>
-      <c r="D468" s="155" t="s">
+      <c r="A468" s="141"/>
+      <c r="B468" s="141"/>
+      <c r="C468" s="141"/>
+      <c r="D468" s="141" t="s">
         <v>3048</v>
       </c>
-      <c r="E468" s="155" t="s">
+      <c r="E468" s="141" t="s">
         <v>3049</v>
       </c>
-      <c r="F468" s="155" t="s">
+      <c r="F468" s="141" t="s">
         <v>3063</v>
       </c>
-      <c r="G468" s="155" t="s">
+      <c r="G468" s="141" t="s">
         <v>3062</v>
       </c>
-      <c r="H468" s="155" t="s">
+      <c r="H468" s="141" t="s">
         <v>2501</v>
       </c>
       <c r="I468" s="135" t="s">
@@ -82098,70 +82263,70 @@
       </c>
     </row>
     <row r="469" spans="1:9" hidden="1">
-      <c r="A469" s="155"/>
-      <c r="B469" s="155"/>
-      <c r="C469" s="155"/>
-      <c r="D469" s="155"/>
-      <c r="E469" s="155"/>
-      <c r="F469" s="155"/>
-      <c r="G469" s="155"/>
-      <c r="H469" s="155"/>
-      <c r="I469" s="155"/>
+      <c r="A469" s="141"/>
+      <c r="B469" s="141"/>
+      <c r="C469" s="141"/>
+      <c r="D469" s="141"/>
+      <c r="E469" s="141"/>
+      <c r="F469" s="141"/>
+      <c r="G469" s="141"/>
+      <c r="H469" s="141"/>
+      <c r="I469" s="141"/>
     </row>
     <row r="470" spans="1:9" hidden="1">
-      <c r="A470" s="155"/>
-      <c r="B470" s="155"/>
-      <c r="C470" s="155"/>
-      <c r="D470" s="155"/>
-      <c r="E470" s="155"/>
-      <c r="F470" s="155"/>
-      <c r="G470" s="155"/>
-      <c r="H470" s="155"/>
-      <c r="I470" s="155"/>
+      <c r="A470" s="141"/>
+      <c r="B470" s="141"/>
+      <c r="C470" s="141"/>
+      <c r="D470" s="141"/>
+      <c r="E470" s="141"/>
+      <c r="F470" s="141"/>
+      <c r="G470" s="141"/>
+      <c r="H470" s="141"/>
+      <c r="I470" s="141"/>
     </row>
     <row r="471" spans="1:9" hidden="1">
-      <c r="A471" s="155"/>
-      <c r="B471" s="155"/>
-      <c r="C471" s="155"/>
-      <c r="D471" s="155"/>
-      <c r="E471" s="155"/>
-      <c r="F471" s="155"/>
-      <c r="G471" s="155"/>
-      <c r="H471" s="155"/>
-      <c r="I471" s="155"/>
+      <c r="A471" s="141"/>
+      <c r="B471" s="141"/>
+      <c r="C471" s="141"/>
+      <c r="D471" s="141"/>
+      <c r="E471" s="141"/>
+      <c r="F471" s="141"/>
+      <c r="G471" s="141"/>
+      <c r="H471" s="141"/>
+      <c r="I471" s="141"/>
     </row>
     <row r="472" spans="1:9" hidden="1">
-      <c r="A472" s="155"/>
-      <c r="B472" s="155"/>
-      <c r="C472" s="155"/>
-      <c r="D472" s="155"/>
-      <c r="E472" s="155"/>
-      <c r="F472" s="155"/>
-      <c r="G472" s="155"/>
-      <c r="H472" s="155"/>
-      <c r="I472" s="155"/>
+      <c r="A472" s="141"/>
+      <c r="B472" s="141"/>
+      <c r="C472" s="141"/>
+      <c r="D472" s="141"/>
+      <c r="E472" s="141"/>
+      <c r="F472" s="141"/>
+      <c r="G472" s="141"/>
+      <c r="H472" s="141"/>
+      <c r="I472" s="141"/>
     </row>
     <row r="473" spans="1:9" hidden="1">
-      <c r="A473" s="155"/>
-      <c r="B473" s="155"/>
-      <c r="C473" s="155"/>
-      <c r="D473" s="155"/>
-      <c r="E473" s="155"/>
-      <c r="F473" s="155"/>
-      <c r="G473" s="155"/>
-      <c r="H473" s="155"/>
-      <c r="I473" s="155"/>
+      <c r="A473" s="141"/>
+      <c r="B473" s="141"/>
+      <c r="C473" s="141"/>
+      <c r="D473" s="141"/>
+      <c r="E473" s="141"/>
+      <c r="F473" s="141"/>
+      <c r="G473" s="141"/>
+      <c r="H473" s="141"/>
+      <c r="I473" s="141"/>
     </row>
     <row r="474" spans="1:9" hidden="1">
-      <c r="A474" s="155"/>
-      <c r="B474" s="155"/>
-      <c r="C474" s="155"/>
-      <c r="D474" s="155"/>
-      <c r="E474" s="155"/>
-      <c r="F474" s="155"/>
-      <c r="G474" s="155"/>
-      <c r="H474" s="155"/>
-      <c r="I474" s="155"/>
+      <c r="A474" s="141"/>
+      <c r="B474" s="141"/>
+      <c r="C474" s="141"/>
+      <c r="D474" s="141"/>
+      <c r="E474" s="141"/>
+      <c r="F474" s="141"/>
+      <c r="G474" s="141"/>
+      <c r="H474" s="141"/>
+      <c r="I474" s="141"/>
     </row>
     <row r="475" spans="1:9" hidden="1">
       <c r="A475" s="139"/>
@@ -82540,8 +82705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:B11"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -82928,6 +83093,642 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="15.7109375" style="140" customWidth="1"/>
+    <col min="5" max="5" width="29.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="140" t="s">
+        <v>3102</v>
+      </c>
+      <c r="B1" s="140" t="s">
+        <v>3081</v>
+      </c>
+      <c r="C1" s="140" t="s">
+        <v>3082</v>
+      </c>
+      <c r="D1" s="140" t="s">
+        <v>3085</v>
+      </c>
+      <c r="E1" s="140" t="s">
+        <v>2328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>3083</v>
+      </c>
+      <c r="B2" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C2" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D2" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3083</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>3086</v>
+      </c>
+      <c r="B3" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C3" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D3" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3086</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>3087</v>
+      </c>
+      <c r="B4" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C4" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D4" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3087</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>3088</v>
+      </c>
+      <c r="B5" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C5" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D5" s="140" t="s">
+        <v>3089</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3088</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>3090</v>
+      </c>
+      <c r="B6" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C6" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D6" s="140" t="s">
+        <v>3089</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3090</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>3091</v>
+      </c>
+      <c r="B7" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C7" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D7" s="140" t="s">
+        <v>3089</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3091</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>3092</v>
+      </c>
+      <c r="B8" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C8" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D8" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3092</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>3093</v>
+      </c>
+      <c r="B9" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C9" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D9" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3093</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>3094</v>
+      </c>
+      <c r="B10" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C10" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D10" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3094</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>3095</v>
+      </c>
+      <c r="B11" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C11" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D11" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3095</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>3096</v>
+      </c>
+      <c r="B12" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C12" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D12" s="140" t="s">
+        <v>3089</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3096</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>3097</v>
+      </c>
+      <c r="B13" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C13" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D13" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3097</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>3098</v>
+      </c>
+      <c r="B14" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C14" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D14" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3098</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>3099</v>
+      </c>
+      <c r="B15" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C15" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D15" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3099</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>3101</v>
+      </c>
+      <c r="B16" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C16" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D16" s="140" t="s">
+        <v>3089</v>
+      </c>
+      <c r="E16" t="s">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>3104</v>
+      </c>
+      <c r="B17" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C17" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D17" s="140" t="s">
+        <v>3089</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>3105</v>
+      </c>
+      <c r="B18" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C18" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D18" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>3106</v>
+      </c>
+      <c r="B19" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C19" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D19" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>3107</v>
+      </c>
+      <c r="B20" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C20" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D20" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="E20" t="s">
+        <v>3107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>3108</v>
+      </c>
+      <c r="B21" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C21" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D21" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="E21" t="s">
+        <v>3108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>3109</v>
+      </c>
+      <c r="B22" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C22" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D22" s="140" t="s">
+        <v>3089</v>
+      </c>
+      <c r="E22" t="s">
+        <v>3109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>3111</v>
+      </c>
+      <c r="B23" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C23" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D23" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="E23" t="s">
+        <v>3113</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>3112</v>
+      </c>
+      <c r="B24" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C24" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D24" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="E24" t="s">
+        <v>3113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>3110</v>
+      </c>
+      <c r="B25" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C25" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D25" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="E25" t="s">
+        <v>3110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>3114</v>
+      </c>
+      <c r="B26" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C26" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D26" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="E26" t="s">
+        <v>3114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>3116</v>
+      </c>
+      <c r="B27" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C27" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D27" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="E27" t="s">
+        <v>3116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>3115</v>
+      </c>
+      <c r="B28" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C28" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D28" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="E28" t="s">
+        <v>3115</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>3117</v>
+      </c>
+      <c r="B29" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C29" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D29" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="E29" t="s">
+        <v>3117</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>3118</v>
+      </c>
+      <c r="B30" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C30" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D30" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="E30" t="s">
+        <v>3118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>3119</v>
+      </c>
+      <c r="B31" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C31" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D31" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="E31" t="s">
+        <v>3119</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>3120</v>
+      </c>
+      <c r="B32" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C32" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D32" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="E32" t="s">
+        <v>3120</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>3121</v>
+      </c>
+      <c r="B33" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C33" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D33" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="E33" t="s">
+        <v>3121</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>3122</v>
+      </c>
+      <c r="B34" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C34" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D34" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="E34" t="s">
+        <v>3122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>3123</v>
+      </c>
+      <c r="B35" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C35" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D35" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="E35" t="s">
+        <v>3123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>3124</v>
+      </c>
+      <c r="B36" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="C36" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="D36" s="140" t="s">
+        <v>3084</v>
+      </c>
+      <c r="E36" t="s">
+        <v>3124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:K15"/>
   <sheetViews>

</xml_diff>